<commit_message>
feat: Test case changes for new file structure
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE97A472-D0B0-1947-BA11-D62D757BD41E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8991DFDA-2383-614C-A1EB-BFD86ABD8430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19540" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="11" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="1199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="1200">
   <si>
     <t>Region</t>
   </si>
@@ -3641,13 +3641,15 @@
   </si>
   <si>
     <t>Future Operations</t>
+  </si>
+  <si>
+    <t>caseworker-iac</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4932,7 +4934,7 @@
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AB98"/>
+  <dimension ref="A1:AH98"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="X90" sqref="X90"/>
@@ -4940,7 +4942,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="29" max="34" style="32" width="9.1640625" collapsed="true"/>
+    <col min="29" max="34" width="9.1640625" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="26" x14ac:dyDescent="0.3">
@@ -7446,8 +7448,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="104.1640625" collapsed="true"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="104.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -7639,42 +7641,42 @@
   </sheetPr>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="40" width="21.83203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="40" width="24.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="40" width="30.1640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="40" width="20.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" hidden="true" width="20.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="40" width="62.5" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" hidden="true" width="33.83203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="40" width="49.83203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" hidden="true" width="32.1640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="40" width="15.5" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="40" width="25.5" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="40" width="19.5" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="40" width="24.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" hidden="true" width="24.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="40" width="21.33203125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" hidden="true" width="21.33203125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="40" width="19.1640625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" hidden="true" width="19.1640625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="40" width="19.1640625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" hidden="true" width="19.1640625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="40" width="16.0" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" hidden="true" width="16.0" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="40" width="14.5" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" hidden="true" width="14.5" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="40" width="17.33203125" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" hidden="true" width="17.33203125" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="40" width="14.5" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" hidden="true" width="14.5" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="40" width="25.5" collapsed="true"/>
-    <col min="30" max="30" style="40" width="9.1640625" collapsed="true"/>
+    <col min="1" max="1" width="21.83203125" style="40" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="40" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" style="40" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="40" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="62.5" style="40" customWidth="1"/>
+    <col min="7" max="7" width="33.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="49.83203125" style="40" customWidth="1"/>
+    <col min="9" max="9" width="32.1640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="40" customWidth="1"/>
+    <col min="11" max="11" width="25.5" style="40" customWidth="1"/>
+    <col min="12" max="12" width="19.5" style="40" customWidth="1"/>
+    <col min="13" max="13" width="24" style="40" customWidth="1"/>
+    <col min="14" max="14" width="24" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="21.33203125" style="40" customWidth="1"/>
+    <col min="16" max="16" width="21.33203125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="19.1640625" style="40" customWidth="1"/>
+    <col min="18" max="18" width="19.1640625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" style="40" customWidth="1"/>
+    <col min="20" max="20" width="19.1640625" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="16" style="40" customWidth="1"/>
+    <col min="22" max="22" width="16" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5" style="40" customWidth="1"/>
+    <col min="24" max="24" width="14.5" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" style="40" customWidth="1"/>
+    <col min="26" max="26" width="17.33203125" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5" style="40" customWidth="1"/>
+    <col min="28" max="28" width="14.5" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="25.5" style="40" customWidth="1"/>
+    <col min="30" max="30" width="9.1640625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -7772,89 +7774,89 @@
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>2240op</v>
+        <v>0851oe</v>
       </c>
       <c r="B2" s="41" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>2107nr</v>
+        <v>4676fi</v>
       </c>
       <c r="C2" s="42" t="str">
         <f ca="1">CONCATENATE(A2,".",B2,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>2240op.2107nr501320@justice.gov.uk</v>
+        <v>0851oe.4676fi511977@justice.gov.uk</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1">
-        <f>_xlfn.IFNA(VLOOKUP(D2,Region!$A$2:$B$11,2),"")</f>
-        <v>2</v>
+        <f>IF(ISNA(VLOOKUP(D2,Region!$A$2:$B$11,2)),"",VLOOKUP(D2,Region!$A$2:$B$11,2))</f>
+        <v>3</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G2" s="1">
-        <f>_xlfn.IFNA(VLOOKUP(F2,'Base Locations'!$A$1:$F$341,2),"")</f>
-        <v>219164</v>
+        <f>IF(ISNA(VLOOKUP(F2,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F2,'Base Locations'!$A$1:$F$341,2))</f>
+        <v>271588</v>
       </c>
       <c r="H2" s="41" t="s">
         <v>74</v>
       </c>
       <c r="I2" s="1">
-        <f>_xlfn.IFNA(VLOOKUP(H2,'Base Locations'!A1:F341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H2,'Base Locations'!A1:F341,2)),"",VLOOKUP(H2,'Base Locations'!A1:F341,2))</f>
         <v>817181</v>
       </c>
       <c r="J2" s="41" t="s">
         <v>52</v>
       </c>
       <c r="K2" s="41" t="s">
-        <v>408</v>
-      </c>
-      <c r="L2" s="41" t="s">
         <v>409</v>
       </c>
+      <c r="L2" s="41"/>
       <c r="M2" s="41" t="s">
-        <v>13</v>
+        <v>1169</v>
       </c>
       <c r="N2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M2,Services!$A$1:$B$45,2),"")</f>
-        <v>BAB1</v>
+        <f>IF(ISNA(VLOOKUP(M2,Services!$A$1:$B$45,2)),"",VLOOKUP(M2,Services!$A$1:$B$45,2))</f>
+        <v>BHA3</v>
       </c>
       <c r="O2" s="41"/>
       <c r="P2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O2,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O2,Services!$A$1:$B$45,2)),"",VLOOKUP(O2,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q2" s="41"/>
       <c r="R2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q2,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q2,Services!$A$1:$B$45,2)),"",VLOOKUP(Q2,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S2" s="41"/>
       <c r="T2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S2,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S2,Services!$A$1:$B$45,2)),"",VLOOKUP(S2,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U2" s="41"/>
       <c r="V2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U2,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U2,Services!$A$1:$B$45,2)),"",VLOOKUP(U2,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W2" s="41"/>
       <c r="X2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W2,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W2,Services!$A$1:$B$45,2)),"",VLOOKUP(W2,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y2" s="41"/>
       <c r="Z2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y2,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y2,Services!$A$1:$B$45,2)),"",VLOOKUP(Y2,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA2" s="41"/>
       <c r="AB2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA2,Services!$A$1:$B$45,2),"")</f>
-        <v/>
-      </c>
-      <c r="AC2" s="41"/>
+        <f>IF(ISNA(VLOOKUP(AA2,Services!$A$1:$B$45,2)),"",VLOOKUP(AA2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AC2" s="41" t="s">
+        <v>1199</v>
+      </c>
       <c r="AD2" s="41" t="s">
         <v>1121</v>
       </c>
@@ -7862,86 +7864,82 @@
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>3809cc</v>
+        <v>0803pw</v>
       </c>
       <c r="B3" s="41" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>9166tg</v>
+        <v>2686td</v>
       </c>
       <c r="C3" s="42" t="str">
         <f ca="1">CONCATENATE(A3,".",B3,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>3809cc.9166tg299028@justice.gov.uk</v>
+        <v>0803pw.2686td494233@justice.gov.uk</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1">
-        <f>_xlfn.IFNA(VLOOKUP(D3,Region!$A$2:$B$11,2),"")</f>
-        <v>3</v>
+        <f>IF(ISNA(VLOOKUP(D3,Region!$A$2:$B$11,2)),"",VLOOKUP(D3,Region!$A$2:$B$11,2))</f>
+        <v>4</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G3" s="1">
-        <f>_xlfn.IFNA(VLOOKUP(F3,'Base Locations'!$A$1:$F$341,2),"")</f>
-        <v>229786</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="1">
-        <f>_xlfn.IFNA(VLOOKUP(H3,'Base Locations'!A2:F342,2),"")</f>
-        <v>574546</v>
+        <f>IF(ISNA(VLOOKUP(F3,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F3,'Base Locations'!$A$1:$F$341,2))</f>
+        <v>206150</v>
+      </c>
+      <c r="H3" s="41"/>
+      <c r="I3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(H3,'Base Locations'!A2:F342,2)),"",VLOOKUP(H3,'Base Locations'!A2:F342,2))</f>
+        <v/>
       </c>
       <c r="J3" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="41" t="s">
-        <v>408</v>
-      </c>
+        <v>1198</v>
+      </c>
+      <c r="K3" s="41"/>
       <c r="L3" s="41" t="s">
         <v>409</v>
       </c>
-      <c r="M3" s="41" t="s">
-        <v>14</v>
-      </c>
+      <c r="M3" s="41"/>
       <c r="N3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M3,Services!$A$1:$B$45,2),"")</f>
-        <v>BAA4</v>
-      </c>
-      <c r="O3" s="41"/>
+        <f>IF(ISNA(VLOOKUP(M3,Services!$A$1:$B$45,2)),"",VLOOKUP(M3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="O3" s="41" t="s">
+        <v>1168</v>
+      </c>
       <c r="P3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O3,Services!$A$1:$B$45,2),"")</f>
-        <v/>
+        <f>IF(ISNA(VLOOKUP(O3,Services!$A$1:$B$45,2)),"",VLOOKUP(O3,Services!$A$1:$B$45,2))</f>
+        <v>BAB2</v>
       </c>
       <c r="Q3" s="41"/>
       <c r="R3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q3,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q3,Services!$A$1:$B$45,2)),"",VLOOKUP(Q3,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S3" s="41"/>
       <c r="T3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S3,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S3,Services!$A$1:$B$45,2)),"",VLOOKUP(S3,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U3" s="41"/>
       <c r="V3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U3,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U3,Services!$A$1:$B$45,2)),"",VLOOKUP(U3,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W3" s="41"/>
       <c r="X3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W3,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W3,Services!$A$1:$B$45,2)),"",VLOOKUP(W3,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y3" s="41"/>
       <c r="Z3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y3,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y3,Services!$A$1:$B$45,2)),"",VLOOKUP(Y3,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA3" s="41"/>
       <c r="AB3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA3,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA3,Services!$A$1:$B$45,2)),"",VLOOKUP(AA3,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC3" s="41"/>
@@ -7950,65 +7948,86 @@
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D4,Region!$A$2:$B$11,2),"")</f>
-        <v/>
-      </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F4,'Base Locations'!$A$1:$F$341,2),"")</f>
-        <v/>
-      </c>
-      <c r="H4" s="41"/>
-      <c r="I4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H4,'Base Locations'!A3:F343,2),"")</f>
-        <v/>
-      </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
+      <c r="A4" s="41" t="str">
+        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
+        <v>5444qe</v>
+      </c>
+      <c r="B4" s="41" t="str">
+        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
+        <v>7318rb</v>
+      </c>
+      <c r="C4" s="42" t="str">
+        <f ca="1">CONCATENATE(A4,".",B4,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
+        <v>5444qe.7318rb44305@justice.gov.uk</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <f>IF(ISNA(VLOOKUP(D4,Region!$A$2:$B$11,2)),"",VLOOKUP(D4,Region!$A$2:$B$11,2))</f>
+        <v>5</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="1">
+        <f>IF(ISNA(VLOOKUP(F4,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F4,'Base Locations'!$A$1:$F$341,2))</f>
+        <v>574546</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="1">
+        <f>IF(ISNA(VLOOKUP(H4,'Base Locations'!A3:F343,2)),"",VLOOKUP(H4,'Base Locations'!A3:F343,2))</f>
+        <v>229786</v>
+      </c>
+      <c r="J4" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="41" t="s">
+        <v>408</v>
+      </c>
       <c r="L4" s="41"/>
       <c r="M4" s="41"/>
       <c r="N4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M4,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M4,Services!$A$1:$B$45,2)),"",VLOOKUP(M4,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O4" s="41"/>
       <c r="P4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O4,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O4,Services!$A$1:$B$45,2)),"",VLOOKUP(O4,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q4" s="41"/>
       <c r="R4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q4,Services!$A$1:$B$45,2),"")</f>
-        <v/>
-      </c>
-      <c r="S4" s="41"/>
+        <f>IF(ISNA(VLOOKUP(Q4,Services!$A$1:$B$45,2)),"",VLOOKUP(Q4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="S4" s="41" t="s">
+        <v>1167</v>
+      </c>
       <c r="T4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S4,Services!$A$1:$B$45,2),"")</f>
-        <v/>
+        <f>IF(ISNA(VLOOKUP(S4,Services!$A$1:$B$45,2)),"",VLOOKUP(S4,Services!$A$1:$B$45,2))</f>
+        <v>BAB2</v>
       </c>
       <c r="U4" s="41"/>
       <c r="V4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U4,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U4,Services!$A$1:$B$45,2)),"",VLOOKUP(U4,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W4" s="41"/>
       <c r="X4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W4,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W4,Services!$A$1:$B$45,2)),"",VLOOKUP(W4,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y4" s="41"/>
       <c r="Z4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y4,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y4,Services!$A$1:$B$45,2)),"",VLOOKUP(Y4,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA4" s="41"/>
       <c r="AB4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA4,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA4,Services!$A$1:$B$45,2)),"",VLOOKUP(AA4,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC4" s="41"/>
@@ -8020,17 +8039,17 @@
       <c r="C5" s="42"/>
       <c r="D5" s="41"/>
       <c r="E5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D5,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D5,Region!$A$2:$B$11,2)),"",VLOOKUP(D5,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F5" s="41"/>
       <c r="G5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F5,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F5,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F5,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H5" s="41"/>
       <c r="I5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H5,'Base Locations'!A4:F344,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H5,'Base Locations'!A4:F344,2)),"",VLOOKUP(H5,'Base Locations'!A4:F344,2))</f>
         <v/>
       </c>
       <c r="J5" s="41"/>
@@ -8038,42 +8057,42 @@
       <c r="L5" s="41"/>
       <c r="M5" s="41"/>
       <c r="N5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M5,Services!$A$1:$B$45,2)),"",VLOOKUP(M5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O5,Services!$A$1:$B$45,2)),"",VLOOKUP(O5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q5" s="41"/>
       <c r="R5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q5,Services!$A$1:$B$45,2)),"",VLOOKUP(Q5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S5" s="41"/>
       <c r="T5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S5,Services!$A$1:$B$45,2)),"",VLOOKUP(S5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U5" s="41"/>
       <c r="V5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U5,Services!$A$1:$B$45,2)),"",VLOOKUP(U5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W5" s="41"/>
       <c r="X5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W5,Services!$A$1:$B$45,2)),"",VLOOKUP(W5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y5" s="41"/>
       <c r="Z5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y5,Services!$A$1:$B$45,2)),"",VLOOKUP(Y5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA5" s="41"/>
       <c r="AB5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA5,Services!$A$1:$B$45,2)),"",VLOOKUP(AA5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC5" s="41"/>
@@ -8085,17 +8104,17 @@
       <c r="C6" s="42"/>
       <c r="D6" s="41"/>
       <c r="E6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D6,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D6,Region!$A$2:$B$11,2)),"",VLOOKUP(D6,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F6" s="41"/>
       <c r="G6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F6,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F6,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F6,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H6" s="41"/>
       <c r="I6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H6,'Base Locations'!A5:F345,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H6,'Base Locations'!A5:F345,2)),"",VLOOKUP(H6,'Base Locations'!A5:F345,2))</f>
         <v/>
       </c>
       <c r="J6" s="41"/>
@@ -8103,42 +8122,42 @@
       <c r="L6" s="41"/>
       <c r="M6" s="41"/>
       <c r="N6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M6,Services!$A$1:$B$45,2)),"",VLOOKUP(M6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O6" s="41"/>
       <c r="P6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O6,Services!$A$1:$B$45,2)),"",VLOOKUP(O6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q6" s="41"/>
       <c r="R6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q6,Services!$A$1:$B$45,2)),"",VLOOKUP(Q6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S6" s="41"/>
       <c r="T6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S6,Services!$A$1:$B$45,2)),"",VLOOKUP(S6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U6" s="41"/>
       <c r="V6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U6,Services!$A$1:$B$45,2)),"",VLOOKUP(U6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W6" s="41"/>
       <c r="X6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W6,Services!$A$1:$B$45,2)),"",VLOOKUP(W6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y6" s="41"/>
       <c r="Z6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y6,Services!$A$1:$B$45,2)),"",VLOOKUP(Y6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA6" s="41"/>
       <c r="AB6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA6,Services!$A$1:$B$45,2)),"",VLOOKUP(AA6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC6" s="41"/>
@@ -8150,17 +8169,17 @@
       <c r="C7" s="42"/>
       <c r="D7" s="41"/>
       <c r="E7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D7,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D7,Region!$A$2:$B$11,2)),"",VLOOKUP(D7,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F7" s="41"/>
       <c r="G7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F7,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F7,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F7,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H7" s="41"/>
       <c r="I7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H7,'Base Locations'!A6:F346,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H7,'Base Locations'!A6:F346,2)),"",VLOOKUP(H7,'Base Locations'!A6:F346,2))</f>
         <v/>
       </c>
       <c r="J7" s="41"/>
@@ -8168,42 +8187,42 @@
       <c r="L7" s="41"/>
       <c r="M7" s="41"/>
       <c r="N7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M7,Services!$A$1:$B$45,2)),"",VLOOKUP(M7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O7" s="41"/>
       <c r="P7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O7,Services!$A$1:$B$45,2)),"",VLOOKUP(O7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q7" s="41"/>
       <c r="R7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q7,Services!$A$1:$B$45,2)),"",VLOOKUP(Q7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S7" s="41"/>
       <c r="T7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S7,Services!$A$1:$B$45,2)),"",VLOOKUP(S7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U7" s="41"/>
       <c r="V7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U7,Services!$A$1:$B$45,2)),"",VLOOKUP(U7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W7" s="41"/>
       <c r="X7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W7,Services!$A$1:$B$45,2)),"",VLOOKUP(W7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y7" s="41"/>
       <c r="Z7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y7,Services!$A$1:$B$45,2)),"",VLOOKUP(Y7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA7" s="41"/>
       <c r="AB7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA7,Services!$A$1:$B$45,2)),"",VLOOKUP(AA7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC7" s="41"/>
@@ -8215,17 +8234,17 @@
       <c r="C8" s="42"/>
       <c r="D8" s="41"/>
       <c r="E8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D8,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D8,Region!$A$2:$B$11,2)),"",VLOOKUP(D8,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F8" s="41"/>
       <c r="G8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F8,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F8,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F8,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H8" s="41"/>
       <c r="I8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H8,'Base Locations'!A7:F347,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H8,'Base Locations'!A7:F347,2)),"",VLOOKUP(H8,'Base Locations'!A7:F347,2))</f>
         <v/>
       </c>
       <c r="J8" s="41"/>
@@ -8233,42 +8252,42 @@
       <c r="L8" s="41"/>
       <c r="M8" s="41"/>
       <c r="N8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M8,Services!$A$1:$B$45,2)),"",VLOOKUP(M8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O8" s="41"/>
       <c r="P8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O8,Services!$A$1:$B$45,2)),"",VLOOKUP(O8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q8" s="41"/>
       <c r="R8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q8,Services!$A$1:$B$45,2)),"",VLOOKUP(Q8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S8" s="41"/>
       <c r="T8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S8,Services!$A$1:$B$45,2)),"",VLOOKUP(S8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U8" s="41"/>
       <c r="V8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U8,Services!$A$1:$B$45,2)),"",VLOOKUP(U8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W8" s="41"/>
       <c r="X8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W8,Services!$A$1:$B$45,2)),"",VLOOKUP(W8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y8" s="41"/>
       <c r="Z8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y8,Services!$A$1:$B$45,2)),"",VLOOKUP(Y8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA8" s="41"/>
       <c r="AB8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA8,Services!$A$1:$B$45,2)),"",VLOOKUP(AA8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC8" s="41"/>
@@ -8280,17 +8299,17 @@
       <c r="C9" s="42"/>
       <c r="D9" s="41"/>
       <c r="E9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D9,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D9,Region!$A$2:$B$11,2)),"",VLOOKUP(D9,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F9" s="41"/>
       <c r="G9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F9,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F9,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F9,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H9" s="41"/>
       <c r="I9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H9,'Base Locations'!A8:F348,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H9,'Base Locations'!A8:F348,2)),"",VLOOKUP(H9,'Base Locations'!A8:F348,2))</f>
         <v/>
       </c>
       <c r="J9" s="41"/>
@@ -8298,42 +8317,42 @@
       <c r="L9" s="41"/>
       <c r="M9" s="41"/>
       <c r="N9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M9,Services!$A$1:$B$45,2)),"",VLOOKUP(M9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O9" s="41"/>
       <c r="P9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O9,Services!$A$1:$B$45,2)),"",VLOOKUP(O9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q9" s="41"/>
       <c r="R9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q9,Services!$A$1:$B$45,2)),"",VLOOKUP(Q9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S9" s="41"/>
       <c r="T9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S9,Services!$A$1:$B$45,2)),"",VLOOKUP(S9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U9" s="41"/>
       <c r="V9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U9,Services!$A$1:$B$45,2)),"",VLOOKUP(U9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W9" s="41"/>
       <c r="X9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W9,Services!$A$1:$B$45,2)),"",VLOOKUP(W9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y9" s="41"/>
       <c r="Z9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y9,Services!$A$1:$B$45,2)),"",VLOOKUP(Y9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA9" s="41"/>
       <c r="AB9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA9,Services!$A$1:$B$45,2)),"",VLOOKUP(AA9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC9" s="41"/>
@@ -8345,17 +8364,17 @@
       <c r="C10" s="42"/>
       <c r="D10" s="41"/>
       <c r="E10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D10,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D10,Region!$A$2:$B$11,2)),"",VLOOKUP(D10,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F10" s="41"/>
       <c r="G10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F10,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F10,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F10,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H10" s="41"/>
       <c r="I10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H10,'Base Locations'!A9:F349,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H10,'Base Locations'!A9:F349,2)),"",VLOOKUP(H10,'Base Locations'!A9:F349,2))</f>
         <v/>
       </c>
       <c r="J10" s="41"/>
@@ -8363,42 +8382,42 @@
       <c r="L10" s="41"/>
       <c r="M10" s="41"/>
       <c r="N10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M10,Services!$A$1:$B$45,2)),"",VLOOKUP(M10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O10" s="41"/>
       <c r="P10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O10,Services!$A$1:$B$45,2)),"",VLOOKUP(O10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q10" s="41"/>
       <c r="R10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q10,Services!$A$1:$B$45,2)),"",VLOOKUP(Q10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S10" s="41"/>
       <c r="T10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S10,Services!$A$1:$B$45,2)),"",VLOOKUP(S10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U10" s="41"/>
       <c r="V10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U10,Services!$A$1:$B$45,2)),"",VLOOKUP(U10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W10" s="41"/>
       <c r="X10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W10,Services!$A$1:$B$45,2)),"",VLOOKUP(W10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y10" s="41"/>
       <c r="Z10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y10,Services!$A$1:$B$45,2)),"",VLOOKUP(Y10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA10" s="41"/>
       <c r="AB10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA10,Services!$A$1:$B$45,2)),"",VLOOKUP(AA10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC10" s="41"/>
@@ -8410,17 +8429,17 @@
       <c r="C11" s="42"/>
       <c r="D11" s="41"/>
       <c r="E11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D11,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D11,Region!$A$2:$B$11,2)),"",VLOOKUP(D11,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F11" s="41"/>
       <c r="G11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F11,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F11,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F11,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H11" s="41"/>
       <c r="I11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H11,'Base Locations'!A10:F350,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H11,'Base Locations'!A10:F350,2)),"",VLOOKUP(H11,'Base Locations'!A10:F350,2))</f>
         <v/>
       </c>
       <c r="J11" s="41"/>
@@ -8428,42 +8447,42 @@
       <c r="L11" s="41"/>
       <c r="M11" s="41"/>
       <c r="N11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M11,Services!$A$1:$B$45,2)),"",VLOOKUP(M11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O11" s="41"/>
       <c r="P11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O11,Services!$A$1:$B$45,2)),"",VLOOKUP(O11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q11" s="41"/>
       <c r="R11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q11,Services!$A$1:$B$45,2)),"",VLOOKUP(Q11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S11" s="41"/>
       <c r="T11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S11,Services!$A$1:$B$45,2)),"",VLOOKUP(S11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U11" s="41"/>
       <c r="V11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U11,Services!$A$1:$B$45,2)),"",VLOOKUP(U11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W11" s="41"/>
       <c r="X11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W11,Services!$A$1:$B$45,2)),"",VLOOKUP(W11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y11" s="41"/>
       <c r="Z11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y11,Services!$A$1:$B$45,2)),"",VLOOKUP(Y11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA11" s="41"/>
       <c r="AB11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA11,Services!$A$1:$B$45,2)),"",VLOOKUP(AA11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC11" s="41"/>
@@ -8475,17 +8494,17 @@
       <c r="C12" s="42"/>
       <c r="D12" s="41"/>
       <c r="E12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D12,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D12,Region!$A$2:$B$11,2)),"",VLOOKUP(D12,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F12" s="41"/>
       <c r="G12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F12,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F12,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F12,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H12" s="41"/>
       <c r="I12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H12,'Base Locations'!A11:F351,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H12,'Base Locations'!A11:F351,2)),"",VLOOKUP(H12,'Base Locations'!A11:F351,2))</f>
         <v/>
       </c>
       <c r="J12" s="41"/>
@@ -8493,42 +8512,42 @@
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
       <c r="N12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M12,Services!$A$1:$B$45,2)),"",VLOOKUP(M12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O12" s="41"/>
       <c r="P12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O12,Services!$A$1:$B$45,2)),"",VLOOKUP(O12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q12" s="41"/>
       <c r="R12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q12,Services!$A$1:$B$45,2)),"",VLOOKUP(Q12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S12" s="41"/>
       <c r="T12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S12,Services!$A$1:$B$45,2)),"",VLOOKUP(S12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U12" s="41"/>
       <c r="V12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U12,Services!$A$1:$B$45,2)),"",VLOOKUP(U12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W12" s="41"/>
       <c r="X12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W12,Services!$A$1:$B$45,2)),"",VLOOKUP(W12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y12" s="41"/>
       <c r="Z12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y12,Services!$A$1:$B$45,2)),"",VLOOKUP(Y12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA12" s="41"/>
       <c r="AB12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA12,Services!$A$1:$B$45,2)),"",VLOOKUP(AA12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC12" s="41"/>
@@ -8540,17 +8559,17 @@
       <c r="C13" s="42"/>
       <c r="D13" s="41"/>
       <c r="E13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D13,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D13,Region!$A$2:$B$11,2)),"",VLOOKUP(D13,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F13" s="41"/>
       <c r="G13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F13,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F13,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F13,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H13" s="41"/>
       <c r="I13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H13,'Base Locations'!A12:F352,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H13,'Base Locations'!A12:F352,2)),"",VLOOKUP(H13,'Base Locations'!A12:F352,2))</f>
         <v/>
       </c>
       <c r="J13" s="41"/>
@@ -8558,42 +8577,42 @@
       <c r="L13" s="41"/>
       <c r="M13" s="41"/>
       <c r="N13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M13,Services!$A$1:$B$45,2)),"",VLOOKUP(M13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O13" s="41"/>
       <c r="P13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O13,Services!$A$1:$B$45,2)),"",VLOOKUP(O13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q13" s="41"/>
       <c r="R13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q13,Services!$A$1:$B$45,2)),"",VLOOKUP(Q13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S13" s="41"/>
       <c r="T13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S13,Services!$A$1:$B$45,2)),"",VLOOKUP(S13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U13" s="41"/>
       <c r="V13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U13,Services!$A$1:$B$45,2)),"",VLOOKUP(U13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W13" s="41"/>
       <c r="X13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W13,Services!$A$1:$B$45,2)),"",VLOOKUP(W13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y13" s="41"/>
       <c r="Z13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y13,Services!$A$1:$B$45,2)),"",VLOOKUP(Y13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA13" s="41"/>
       <c r="AB13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA13,Services!$A$1:$B$45,2)),"",VLOOKUP(AA13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC13" s="41"/>
@@ -8605,17 +8624,17 @@
       <c r="C14" s="42"/>
       <c r="D14" s="41"/>
       <c r="E14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D14,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D14,Region!$A$2:$B$11,2)),"",VLOOKUP(D14,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F14" s="41"/>
       <c r="G14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F14,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F14,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F14,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H14" s="41"/>
       <c r="I14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H14,'Base Locations'!A13:F353,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H14,'Base Locations'!A13:F353,2)),"",VLOOKUP(H14,'Base Locations'!A13:F353,2))</f>
         <v/>
       </c>
       <c r="J14" s="41"/>
@@ -8623,42 +8642,42 @@
       <c r="L14" s="41"/>
       <c r="M14" s="41"/>
       <c r="N14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M14,Services!$A$1:$B$45,2)),"",VLOOKUP(M14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O14" s="41"/>
       <c r="P14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O14,Services!$A$1:$B$45,2)),"",VLOOKUP(O14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q14" s="41"/>
       <c r="R14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q14,Services!$A$1:$B$45,2)),"",VLOOKUP(Q14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S14" s="41"/>
       <c r="T14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S14,Services!$A$1:$B$45,2)),"",VLOOKUP(S14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U14" s="41"/>
       <c r="V14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U14,Services!$A$1:$B$45,2)),"",VLOOKUP(U14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W14" s="41"/>
       <c r="X14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W14,Services!$A$1:$B$45,2)),"",VLOOKUP(W14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y14" s="41"/>
       <c r="Z14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y14,Services!$A$1:$B$45,2)),"",VLOOKUP(Y14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA14" s="41"/>
       <c r="AB14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA14,Services!$A$1:$B$45,2)),"",VLOOKUP(AA14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC14" s="41"/>
@@ -8670,17 +8689,17 @@
       <c r="C15" s="42"/>
       <c r="D15" s="41"/>
       <c r="E15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D15,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D15,Region!$A$2:$B$11,2)),"",VLOOKUP(D15,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F15" s="41"/>
       <c r="G15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F15,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F15,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F15,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H15" s="41"/>
       <c r="I15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H15,'Base Locations'!A14:F354,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H15,'Base Locations'!A14:F354,2)),"",VLOOKUP(H15,'Base Locations'!A14:F354,2))</f>
         <v/>
       </c>
       <c r="J15" s="41"/>
@@ -8688,42 +8707,42 @@
       <c r="L15" s="41"/>
       <c r="M15" s="41"/>
       <c r="N15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M15,Services!$A$1:$B$45,2)),"",VLOOKUP(M15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O15" s="41"/>
       <c r="P15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O15,Services!$A$1:$B$45,2)),"",VLOOKUP(O15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q15" s="41"/>
       <c r="R15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q15,Services!$A$1:$B$45,2)),"",VLOOKUP(Q15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S15" s="41"/>
       <c r="T15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S15,Services!$A$1:$B$45,2)),"",VLOOKUP(S15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U15" s="41"/>
       <c r="V15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U15,Services!$A$1:$B$45,2)),"",VLOOKUP(U15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W15" s="41"/>
       <c r="X15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W15,Services!$A$1:$B$45,2)),"",VLOOKUP(W15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y15" s="41"/>
       <c r="Z15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y15,Services!$A$1:$B$45,2)),"",VLOOKUP(Y15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA15" s="41"/>
       <c r="AB15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA15,Services!$A$1:$B$45,2)),"",VLOOKUP(AA15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC15" s="41"/>
@@ -8735,17 +8754,17 @@
       <c r="C16" s="42"/>
       <c r="D16" s="41"/>
       <c r="E16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D16,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D16,Region!$A$2:$B$11,2)),"",VLOOKUP(D16,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F16" s="41"/>
       <c r="G16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F16,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F16,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F16,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H16" s="41"/>
       <c r="I16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H16,'Base Locations'!A15:F355,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H16,'Base Locations'!A15:F355,2)),"",VLOOKUP(H16,'Base Locations'!A15:F355,2))</f>
         <v/>
       </c>
       <c r="J16" s="41"/>
@@ -8753,42 +8772,42 @@
       <c r="L16" s="41"/>
       <c r="M16" s="41"/>
       <c r="N16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M16,Services!$A$1:$B$45,2)),"",VLOOKUP(M16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O16" s="41"/>
       <c r="P16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O16,Services!$A$1:$B$45,2)),"",VLOOKUP(O16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q16" s="41"/>
       <c r="R16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q16,Services!$A$1:$B$45,2)),"",VLOOKUP(Q16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S16" s="41"/>
       <c r="T16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S16,Services!$A$1:$B$45,2)),"",VLOOKUP(S16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U16" s="41"/>
       <c r="V16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U16,Services!$A$1:$B$45,2)),"",VLOOKUP(U16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W16" s="41"/>
       <c r="X16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W16,Services!$A$1:$B$45,2)),"",VLOOKUP(W16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y16" s="41"/>
       <c r="Z16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y16,Services!$A$1:$B$45,2)),"",VLOOKUP(Y16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA16" s="41"/>
       <c r="AB16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA16,Services!$A$1:$B$45,2)),"",VLOOKUP(AA16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC16" s="41"/>
@@ -8800,17 +8819,17 @@
       <c r="C17" s="42"/>
       <c r="D17" s="41"/>
       <c r="E17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D17,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D17,Region!$A$2:$B$11,2)),"",VLOOKUP(D17,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F17" s="41"/>
       <c r="G17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F17,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F17,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F17,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H17" s="41"/>
       <c r="I17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H17,'Base Locations'!A16:F356,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H17,'Base Locations'!A16:F356,2)),"",VLOOKUP(H17,'Base Locations'!A16:F356,2))</f>
         <v/>
       </c>
       <c r="J17" s="41"/>
@@ -8818,42 +8837,42 @@
       <c r="L17" s="41"/>
       <c r="M17" s="41"/>
       <c r="N17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M17,Services!$A$1:$B$45,2)),"",VLOOKUP(M17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O17" s="41"/>
       <c r="P17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O17,Services!$A$1:$B$45,2)),"",VLOOKUP(O17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q17" s="41"/>
       <c r="R17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q17,Services!$A$1:$B$45,2)),"",VLOOKUP(Q17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S17" s="41"/>
       <c r="T17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S17,Services!$A$1:$B$45,2)),"",VLOOKUP(S17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U17" s="41"/>
       <c r="V17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U17,Services!$A$1:$B$45,2)),"",VLOOKUP(U17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W17" s="41"/>
       <c r="X17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W17,Services!$A$1:$B$45,2)),"",VLOOKUP(W17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y17" s="41"/>
       <c r="Z17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y17,Services!$A$1:$B$45,2)),"",VLOOKUP(Y17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA17" s="41"/>
       <c r="AB17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA17,Services!$A$1:$B$45,2)),"",VLOOKUP(AA17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC17" s="41"/>
@@ -8865,17 +8884,17 @@
       <c r="C18" s="42"/>
       <c r="D18" s="41"/>
       <c r="E18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D18,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D18,Region!$A$2:$B$11,2)),"",VLOOKUP(D18,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F18" s="41"/>
       <c r="G18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F18,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F18,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F18,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H18" s="41"/>
       <c r="I18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H18,'Base Locations'!A17:F357,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H18,'Base Locations'!A17:F357,2)),"",VLOOKUP(H18,'Base Locations'!A17:F357,2))</f>
         <v/>
       </c>
       <c r="J18" s="41"/>
@@ -8883,42 +8902,42 @@
       <c r="L18" s="41"/>
       <c r="M18" s="41"/>
       <c r="N18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M18,Services!$A$1:$B$45,2)),"",VLOOKUP(M18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O18" s="41"/>
       <c r="P18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O18,Services!$A$1:$B$45,2)),"",VLOOKUP(O18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q18" s="41"/>
       <c r="R18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q18,Services!$A$1:$B$45,2)),"",VLOOKUP(Q18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S18" s="41"/>
       <c r="T18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S18,Services!$A$1:$B$45,2)),"",VLOOKUP(S18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U18" s="41"/>
       <c r="V18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U18,Services!$A$1:$B$45,2)),"",VLOOKUP(U18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W18" s="41"/>
       <c r="X18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W18,Services!$A$1:$B$45,2)),"",VLOOKUP(W18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y18" s="41"/>
       <c r="Z18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y18,Services!$A$1:$B$45,2)),"",VLOOKUP(Y18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA18" s="41"/>
       <c r="AB18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA18,Services!$A$1:$B$45,2)),"",VLOOKUP(AA18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC18" s="41"/>
@@ -8930,17 +8949,17 @@
       <c r="C19" s="42"/>
       <c r="D19" s="41"/>
       <c r="E19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D19,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D19,Region!$A$2:$B$11,2)),"",VLOOKUP(D19,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F19" s="41"/>
       <c r="G19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F19,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F19,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F19,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H19" s="41"/>
       <c r="I19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H19,'Base Locations'!A18:F358,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H19,'Base Locations'!A18:F358,2)),"",VLOOKUP(H19,'Base Locations'!A18:F358,2))</f>
         <v/>
       </c>
       <c r="J19" s="41"/>
@@ -8948,42 +8967,42 @@
       <c r="L19" s="41"/>
       <c r="M19" s="41"/>
       <c r="N19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M19,Services!$A$1:$B$45,2)),"",VLOOKUP(M19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O19" s="41"/>
       <c r="P19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O19,Services!$A$1:$B$45,2)),"",VLOOKUP(O19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q19" s="41"/>
       <c r="R19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q19,Services!$A$1:$B$45,2)),"",VLOOKUP(Q19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S19" s="41"/>
       <c r="T19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S19,Services!$A$1:$B$45,2)),"",VLOOKUP(S19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U19" s="41"/>
       <c r="V19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U19,Services!$A$1:$B$45,2)),"",VLOOKUP(U19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W19" s="41"/>
       <c r="X19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W19,Services!$A$1:$B$45,2)),"",VLOOKUP(W19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y19" s="41"/>
       <c r="Z19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y19,Services!$A$1:$B$45,2)),"",VLOOKUP(Y19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA19" s="41"/>
       <c r="AB19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA19,Services!$A$1:$B$45,2)),"",VLOOKUP(AA19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC19" s="41"/>
@@ -8995,17 +9014,17 @@
       <c r="C20" s="42"/>
       <c r="D20" s="41"/>
       <c r="E20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D20,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D20,Region!$A$2:$B$11,2)),"",VLOOKUP(D20,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F20" s="41"/>
       <c r="G20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F20,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F20,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F20,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H20" s="41"/>
       <c r="I20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H20,'Base Locations'!A19:F359,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H20,'Base Locations'!A19:F359,2)),"",VLOOKUP(H20,'Base Locations'!A19:F359,2))</f>
         <v/>
       </c>
       <c r="J20" s="41"/>
@@ -9013,42 +9032,42 @@
       <c r="L20" s="41"/>
       <c r="M20" s="41"/>
       <c r="N20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M20,Services!$A$1:$B$45,2)),"",VLOOKUP(M20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O20" s="41"/>
       <c r="P20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O20,Services!$A$1:$B$45,2)),"",VLOOKUP(O20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q20" s="41"/>
       <c r="R20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q20,Services!$A$1:$B$45,2)),"",VLOOKUP(Q20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S20" s="41"/>
       <c r="T20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S20,Services!$A$1:$B$45,2)),"",VLOOKUP(S20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U20" s="41"/>
       <c r="V20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U20,Services!$A$1:$B$45,2)),"",VLOOKUP(U20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W20" s="41"/>
       <c r="X20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W20,Services!$A$1:$B$45,2)),"",VLOOKUP(W20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y20" s="41"/>
       <c r="Z20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y20,Services!$A$1:$B$45,2)),"",VLOOKUP(Y20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA20" s="41"/>
       <c r="AB20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA20,Services!$A$1:$B$45,2)),"",VLOOKUP(AA20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC20" s="41"/>
@@ -9060,17 +9079,17 @@
       <c r="C21" s="42"/>
       <c r="D21" s="41"/>
       <c r="E21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D21,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D21,Region!$A$2:$B$11,2)),"",VLOOKUP(D21,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F21" s="41"/>
       <c r="G21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F21,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F21,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F21,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H21" s="41"/>
       <c r="I21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H21,'Base Locations'!A20:F360,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H21,'Base Locations'!A20:F360,2)),"",VLOOKUP(H21,'Base Locations'!A20:F360,2))</f>
         <v/>
       </c>
       <c r="J21" s="41"/>
@@ -9078,42 +9097,42 @@
       <c r="L21" s="41"/>
       <c r="M21" s="41"/>
       <c r="N21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M21,Services!$A$1:$B$45,2)),"",VLOOKUP(M21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O21" s="41"/>
       <c r="P21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O21,Services!$A$1:$B$45,2)),"",VLOOKUP(O21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q21" s="41"/>
       <c r="R21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q21,Services!$A$1:$B$45,2)),"",VLOOKUP(Q21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S21" s="41"/>
       <c r="T21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S21,Services!$A$1:$B$45,2)),"",VLOOKUP(S21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U21" s="41"/>
       <c r="V21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U21,Services!$A$1:$B$45,2)),"",VLOOKUP(U21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W21" s="41"/>
       <c r="X21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W21,Services!$A$1:$B$45,2)),"",VLOOKUP(W21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y21" s="41"/>
       <c r="Z21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y21,Services!$A$1:$B$45,2)),"",VLOOKUP(Y21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA21" s="41"/>
       <c r="AB21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA21,Services!$A$1:$B$45,2)),"",VLOOKUP(AA21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC21" s="41"/>
@@ -9125,17 +9144,17 @@
       <c r="C22" s="42"/>
       <c r="D22" s="41"/>
       <c r="E22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D22,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D22,Region!$A$2:$B$11,2)),"",VLOOKUP(D22,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F22" s="41"/>
       <c r="G22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F22,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F22,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F22,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H22" s="41"/>
       <c r="I22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H22,'Base Locations'!A21:F361,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H22,'Base Locations'!A21:F361,2)),"",VLOOKUP(H22,'Base Locations'!A21:F361,2))</f>
         <v/>
       </c>
       <c r="J22" s="41"/>
@@ -9143,42 +9162,42 @@
       <c r="L22" s="41"/>
       <c r="M22" s="41"/>
       <c r="N22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M22,Services!$A$1:$B$45,2)),"",VLOOKUP(M22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O22" s="41"/>
       <c r="P22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O22,Services!$A$1:$B$45,2)),"",VLOOKUP(O22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q22" s="41"/>
       <c r="R22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q22,Services!$A$1:$B$45,2)),"",VLOOKUP(Q22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S22" s="41"/>
       <c r="T22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S22,Services!$A$1:$B$45,2)),"",VLOOKUP(S22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U22" s="41"/>
       <c r="V22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U22,Services!$A$1:$B$45,2)),"",VLOOKUP(U22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W22" s="41"/>
       <c r="X22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W22,Services!$A$1:$B$45,2)),"",VLOOKUP(W22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y22" s="41"/>
       <c r="Z22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y22,Services!$A$1:$B$45,2)),"",VLOOKUP(Y22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA22" s="41"/>
       <c r="AB22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA22,Services!$A$1:$B$45,2)),"",VLOOKUP(AA22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC22" s="41"/>
@@ -9190,17 +9209,17 @@
       <c r="C23" s="42"/>
       <c r="D23" s="41"/>
       <c r="E23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D23,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D23,Region!$A$2:$B$11,2)),"",VLOOKUP(D23,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F23" s="41"/>
       <c r="G23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F23,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F23,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F23,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H23" s="41"/>
       <c r="I23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H23,'Base Locations'!A22:F362,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H23,'Base Locations'!A22:F362,2)),"",VLOOKUP(H23,'Base Locations'!A22:F362,2))</f>
         <v/>
       </c>
       <c r="J23" s="41"/>
@@ -9208,42 +9227,42 @@
       <c r="L23" s="41"/>
       <c r="M23" s="41"/>
       <c r="N23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M23,Services!$A$1:$B$45,2)),"",VLOOKUP(M23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O23" s="41"/>
       <c r="P23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O23,Services!$A$1:$B$45,2)),"",VLOOKUP(O23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q23" s="41"/>
       <c r="R23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q23,Services!$A$1:$B$45,2)),"",VLOOKUP(Q23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S23" s="41"/>
       <c r="T23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S23,Services!$A$1:$B$45,2)),"",VLOOKUP(S23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U23" s="41"/>
       <c r="V23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U23,Services!$A$1:$B$45,2)),"",VLOOKUP(U23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W23" s="41"/>
       <c r="X23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W23,Services!$A$1:$B$45,2)),"",VLOOKUP(W23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y23" s="41"/>
       <c r="Z23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y23,Services!$A$1:$B$45,2)),"",VLOOKUP(Y23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA23" s="41"/>
       <c r="AB23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA23,Services!$A$1:$B$45,2)),"",VLOOKUP(AA23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC23" s="41"/>
@@ -9255,17 +9274,17 @@
       <c r="C24" s="42"/>
       <c r="D24" s="41"/>
       <c r="E24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D24,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D24,Region!$A$2:$B$11,2)),"",VLOOKUP(D24,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F24" s="41"/>
       <c r="G24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F24,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F24,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F24,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H24" s="41"/>
       <c r="I24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H24,'Base Locations'!A23:F363,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H24,'Base Locations'!A23:F363,2)),"",VLOOKUP(H24,'Base Locations'!A23:F363,2))</f>
         <v/>
       </c>
       <c r="J24" s="41"/>
@@ -9273,42 +9292,42 @@
       <c r="L24" s="41"/>
       <c r="M24" s="41"/>
       <c r="N24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M24,Services!$A$1:$B$45,2)),"",VLOOKUP(M24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O24" s="41"/>
       <c r="P24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O24,Services!$A$1:$B$45,2)),"",VLOOKUP(O24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q24" s="41"/>
       <c r="R24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q24,Services!$A$1:$B$45,2)),"",VLOOKUP(Q24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S24" s="41"/>
       <c r="T24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S24,Services!$A$1:$B$45,2)),"",VLOOKUP(S24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U24" s="41"/>
       <c r="V24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U24,Services!$A$1:$B$45,2)),"",VLOOKUP(U24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W24" s="41"/>
       <c r="X24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W24,Services!$A$1:$B$45,2)),"",VLOOKUP(W24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y24" s="41"/>
       <c r="Z24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y24,Services!$A$1:$B$45,2)),"",VLOOKUP(Y24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA24" s="41"/>
       <c r="AB24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA24,Services!$A$1:$B$45,2)),"",VLOOKUP(AA24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC24" s="41"/>
@@ -9320,17 +9339,17 @@
       <c r="C25" s="42"/>
       <c r="D25" s="41"/>
       <c r="E25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D25,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D25,Region!$A$2:$B$11,2)),"",VLOOKUP(D25,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F25" s="41"/>
       <c r="G25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F25,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F25,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F25,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H25" s="41"/>
       <c r="I25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H25,'Base Locations'!A24:F364,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H25,'Base Locations'!A24:F364,2)),"",VLOOKUP(H25,'Base Locations'!A24:F364,2))</f>
         <v/>
       </c>
       <c r="J25" s="41"/>
@@ -9338,42 +9357,42 @@
       <c r="L25" s="41"/>
       <c r="M25" s="41"/>
       <c r="N25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M25,Services!$A$1:$B$45,2)),"",VLOOKUP(M25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O25" s="41"/>
       <c r="P25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O25,Services!$A$1:$B$45,2)),"",VLOOKUP(O25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q25" s="41"/>
       <c r="R25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q25,Services!$A$1:$B$45,2)),"",VLOOKUP(Q25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S25" s="41"/>
       <c r="T25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S25,Services!$A$1:$B$45,2)),"",VLOOKUP(S25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U25" s="41"/>
       <c r="V25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U25,Services!$A$1:$B$45,2)),"",VLOOKUP(U25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W25" s="41"/>
       <c r="X25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W25,Services!$A$1:$B$45,2)),"",VLOOKUP(W25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y25" s="41"/>
       <c r="Z25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y25,Services!$A$1:$B$45,2)),"",VLOOKUP(Y25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA25" s="41"/>
       <c r="AB25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA25,Services!$A$1:$B$45,2)),"",VLOOKUP(AA25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC25" s="41"/>
@@ -9385,17 +9404,17 @@
       <c r="C26" s="42"/>
       <c r="D26" s="41"/>
       <c r="E26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D26,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D26,Region!$A$2:$B$11,2)),"",VLOOKUP(D26,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F26" s="41"/>
       <c r="G26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F26,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F26,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F26,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H26" s="41"/>
       <c r="I26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H26,'Base Locations'!A25:F365,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H26,'Base Locations'!A25:F365,2)),"",VLOOKUP(H26,'Base Locations'!A25:F365,2))</f>
         <v/>
       </c>
       <c r="J26" s="41"/>
@@ -9403,42 +9422,42 @@
       <c r="L26" s="41"/>
       <c r="M26" s="41"/>
       <c r="N26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M26,Services!$A$1:$B$45,2)),"",VLOOKUP(M26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O26" s="41"/>
       <c r="P26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O26,Services!$A$1:$B$45,2)),"",VLOOKUP(O26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q26" s="41"/>
       <c r="R26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q26,Services!$A$1:$B$45,2)),"",VLOOKUP(Q26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S26" s="41"/>
       <c r="T26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S26,Services!$A$1:$B$45,2)),"",VLOOKUP(S26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U26" s="41"/>
       <c r="V26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U26,Services!$A$1:$B$45,2)),"",VLOOKUP(U26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W26" s="41"/>
       <c r="X26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W26,Services!$A$1:$B$45,2)),"",VLOOKUP(W26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y26" s="41"/>
       <c r="Z26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y26,Services!$A$1:$B$45,2)),"",VLOOKUP(Y26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA26" s="41"/>
       <c r="AB26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA26,Services!$A$1:$B$45,2)),"",VLOOKUP(AA26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC26" s="41"/>
@@ -9450,17 +9469,17 @@
       <c r="C27" s="42"/>
       <c r="D27" s="41"/>
       <c r="E27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D27,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D27,Region!$A$2:$B$11,2)),"",VLOOKUP(D27,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F27" s="41"/>
       <c r="G27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F27,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F27,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F27,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H27" s="41"/>
       <c r="I27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H27,'Base Locations'!A26:F366,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H27,'Base Locations'!A26:F366,2)),"",VLOOKUP(H27,'Base Locations'!A26:F366,2))</f>
         <v/>
       </c>
       <c r="J27" s="41"/>
@@ -9468,42 +9487,42 @@
       <c r="L27" s="41"/>
       <c r="M27" s="41"/>
       <c r="N27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M27,Services!$A$1:$B$45,2)),"",VLOOKUP(M27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O27" s="41"/>
       <c r="P27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O27,Services!$A$1:$B$45,2)),"",VLOOKUP(O27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q27" s="41"/>
       <c r="R27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q27,Services!$A$1:$B$45,2)),"",VLOOKUP(Q27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S27" s="41"/>
       <c r="T27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S27,Services!$A$1:$B$45,2)),"",VLOOKUP(S27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U27" s="41"/>
       <c r="V27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U27,Services!$A$1:$B$45,2)),"",VLOOKUP(U27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W27" s="41"/>
       <c r="X27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W27,Services!$A$1:$B$45,2)),"",VLOOKUP(W27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y27" s="41"/>
       <c r="Z27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y27,Services!$A$1:$B$45,2)),"",VLOOKUP(Y27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA27" s="41"/>
       <c r="AB27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA27,Services!$A$1:$B$45,2)),"",VLOOKUP(AA27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC27" s="41"/>
@@ -9515,17 +9534,17 @@
       <c r="C28" s="42"/>
       <c r="D28" s="41"/>
       <c r="E28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D28,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D28,Region!$A$2:$B$11,2)),"",VLOOKUP(D28,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F28" s="41"/>
       <c r="G28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F28,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F28,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F28,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H28" s="41"/>
       <c r="I28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H28,'Base Locations'!A27:F367,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H28,'Base Locations'!A27:F367,2)),"",VLOOKUP(H28,'Base Locations'!A27:F367,2))</f>
         <v/>
       </c>
       <c r="J28" s="41"/>
@@ -9533,42 +9552,42 @@
       <c r="L28" s="41"/>
       <c r="M28" s="41"/>
       <c r="N28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M28,Services!$A$1:$B$45,2)),"",VLOOKUP(M28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O28" s="41"/>
       <c r="P28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O28,Services!$A$1:$B$45,2)),"",VLOOKUP(O28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q28" s="41"/>
       <c r="R28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q28,Services!$A$1:$B$45,2)),"",VLOOKUP(Q28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S28" s="41"/>
       <c r="T28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S28,Services!$A$1:$B$45,2)),"",VLOOKUP(S28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U28" s="41"/>
       <c r="V28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U28,Services!$A$1:$B$45,2)),"",VLOOKUP(U28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W28" s="41"/>
       <c r="X28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W28,Services!$A$1:$B$45,2)),"",VLOOKUP(W28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y28" s="41"/>
       <c r="Z28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y28,Services!$A$1:$B$45,2)),"",VLOOKUP(Y28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA28" s="41"/>
       <c r="AB28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA28,Services!$A$1:$B$45,2)),"",VLOOKUP(AA28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC28" s="41"/>
@@ -9580,17 +9599,17 @@
       <c r="C29" s="42"/>
       <c r="D29" s="41"/>
       <c r="E29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D29,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D29,Region!$A$2:$B$11,2)),"",VLOOKUP(D29,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F29" s="41"/>
       <c r="G29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F29,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F29,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F29,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H29" s="41"/>
       <c r="I29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H29,'Base Locations'!A28:F368,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H29,'Base Locations'!A28:F368,2)),"",VLOOKUP(H29,'Base Locations'!A28:F368,2))</f>
         <v/>
       </c>
       <c r="J29" s="41"/>
@@ -9598,42 +9617,42 @@
       <c r="L29" s="41"/>
       <c r="M29" s="41"/>
       <c r="N29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M29,Services!$A$1:$B$45,2)),"",VLOOKUP(M29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O29" s="41"/>
       <c r="P29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O29,Services!$A$1:$B$45,2)),"",VLOOKUP(O29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q29" s="41"/>
       <c r="R29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q29,Services!$A$1:$B$45,2)),"",VLOOKUP(Q29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S29" s="41"/>
       <c r="T29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S29,Services!$A$1:$B$45,2)),"",VLOOKUP(S29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U29" s="41"/>
       <c r="V29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U29,Services!$A$1:$B$45,2)),"",VLOOKUP(U29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W29" s="41"/>
       <c r="X29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W29,Services!$A$1:$B$45,2)),"",VLOOKUP(W29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y29" s="41"/>
       <c r="Z29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y29,Services!$A$1:$B$45,2)),"",VLOOKUP(Y29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA29" s="41"/>
       <c r="AB29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA29,Services!$A$1:$B$45,2)),"",VLOOKUP(AA29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC29" s="41"/>
@@ -9645,17 +9664,17 @@
       <c r="C30" s="42"/>
       <c r="D30" s="41"/>
       <c r="E30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D30,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D30,Region!$A$2:$B$11,2)),"",VLOOKUP(D30,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F30" s="41"/>
       <c r="G30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F30,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F30,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F30,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H30" s="41"/>
       <c r="I30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H30,'Base Locations'!A29:F369,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H30,'Base Locations'!A29:F369,2)),"",VLOOKUP(H30,'Base Locations'!A29:F369,2))</f>
         <v/>
       </c>
       <c r="J30" s="41"/>
@@ -9663,42 +9682,42 @@
       <c r="L30" s="41"/>
       <c r="M30" s="41"/>
       <c r="N30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M30,Services!$A$1:$B$45,2)),"",VLOOKUP(M30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O30" s="41"/>
       <c r="P30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O30,Services!$A$1:$B$45,2)),"",VLOOKUP(O30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q30" s="41"/>
       <c r="R30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q30,Services!$A$1:$B$45,2)),"",VLOOKUP(Q30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S30" s="41"/>
       <c r="T30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S30,Services!$A$1:$B$45,2)),"",VLOOKUP(S30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U30" s="41"/>
       <c r="V30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U30,Services!$A$1:$B$45,2)),"",VLOOKUP(U30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W30" s="41"/>
       <c r="X30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W30,Services!$A$1:$B$45,2)),"",VLOOKUP(W30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y30" s="41"/>
       <c r="Z30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y30,Services!$A$1:$B$45,2)),"",VLOOKUP(Y30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA30" s="41"/>
       <c r="AB30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA30,Services!$A$1:$B$45,2)),"",VLOOKUP(AA30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC30" s="41"/>
@@ -9710,17 +9729,17 @@
       <c r="C31" s="42"/>
       <c r="D31" s="41"/>
       <c r="E31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D31,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D31,Region!$A$2:$B$11,2)),"",VLOOKUP(D31,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F31" s="41"/>
       <c r="G31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F31,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F31,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F31,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H31" s="41"/>
       <c r="I31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H31,'Base Locations'!A30:F370,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H31,'Base Locations'!A30:F370,2)),"",VLOOKUP(H31,'Base Locations'!A30:F370,2))</f>
         <v/>
       </c>
       <c r="J31" s="41"/>
@@ -9728,42 +9747,42 @@
       <c r="L31" s="41"/>
       <c r="M31" s="41"/>
       <c r="N31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M31,Services!$A$1:$B$45,2)),"",VLOOKUP(M31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O31" s="41"/>
       <c r="P31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O31,Services!$A$1:$B$45,2)),"",VLOOKUP(O31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q31" s="41"/>
       <c r="R31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q31,Services!$A$1:$B$45,2)),"",VLOOKUP(Q31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S31" s="41"/>
       <c r="T31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S31,Services!$A$1:$B$45,2)),"",VLOOKUP(S31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U31" s="41"/>
       <c r="V31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U31,Services!$A$1:$B$45,2)),"",VLOOKUP(U31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W31" s="41"/>
       <c r="X31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W31,Services!$A$1:$B$45,2)),"",VLOOKUP(W31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y31" s="41"/>
       <c r="Z31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y31,Services!$A$1:$B$45,2)),"",VLOOKUP(Y31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA31" s="41"/>
       <c r="AB31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA31,Services!$A$1:$B$45,2)),"",VLOOKUP(AA31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC31" s="41"/>
@@ -9775,17 +9794,17 @@
       <c r="C32" s="42"/>
       <c r="D32" s="41"/>
       <c r="E32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D32,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D32,Region!$A$2:$B$11,2)),"",VLOOKUP(D32,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F32" s="41"/>
       <c r="G32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F32,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F32,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F32,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H32" s="41"/>
       <c r="I32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H32,'Base Locations'!A31:F371,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H32,'Base Locations'!A31:F371,2)),"",VLOOKUP(H32,'Base Locations'!A31:F371,2))</f>
         <v/>
       </c>
       <c r="J32" s="41"/>
@@ -9793,42 +9812,42 @@
       <c r="L32" s="41"/>
       <c r="M32" s="41"/>
       <c r="N32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M32,Services!$A$1:$B$45,2)),"",VLOOKUP(M32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O32" s="41"/>
       <c r="P32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O32,Services!$A$1:$B$45,2)),"",VLOOKUP(O32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q32" s="41"/>
       <c r="R32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q32,Services!$A$1:$B$45,2)),"",VLOOKUP(Q32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S32" s="41"/>
       <c r="T32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S32,Services!$A$1:$B$45,2)),"",VLOOKUP(S32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U32" s="41"/>
       <c r="V32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U32,Services!$A$1:$B$45,2)),"",VLOOKUP(U32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W32" s="41"/>
       <c r="X32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W32,Services!$A$1:$B$45,2)),"",VLOOKUP(W32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y32" s="41"/>
       <c r="Z32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y32,Services!$A$1:$B$45,2)),"",VLOOKUP(Y32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA32" s="41"/>
       <c r="AB32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA32,Services!$A$1:$B$45,2)),"",VLOOKUP(AA32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC32" s="41"/>
@@ -9840,17 +9859,17 @@
       <c r="C33" s="42"/>
       <c r="D33" s="41"/>
       <c r="E33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D33,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D33,Region!$A$2:$B$11,2)),"",VLOOKUP(D33,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F33" s="41"/>
       <c r="G33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F33,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F33,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F33,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H33" s="41"/>
       <c r="I33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H33,'Base Locations'!A32:F372,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H33,'Base Locations'!A32:F372,2)),"",VLOOKUP(H33,'Base Locations'!A32:F372,2))</f>
         <v/>
       </c>
       <c r="J33" s="41"/>
@@ -9858,42 +9877,42 @@
       <c r="L33" s="41"/>
       <c r="M33" s="41"/>
       <c r="N33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M33,Services!$A$1:$B$45,2)),"",VLOOKUP(M33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O33" s="41"/>
       <c r="P33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O33,Services!$A$1:$B$45,2)),"",VLOOKUP(O33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q33" s="41"/>
       <c r="R33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q33,Services!$A$1:$B$45,2)),"",VLOOKUP(Q33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S33" s="41"/>
       <c r="T33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S33,Services!$A$1:$B$45,2)),"",VLOOKUP(S33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U33" s="41"/>
       <c r="V33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U33,Services!$A$1:$B$45,2)),"",VLOOKUP(U33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W33" s="41"/>
       <c r="X33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W33,Services!$A$1:$B$45,2)),"",VLOOKUP(W33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y33" s="41"/>
       <c r="Z33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y33,Services!$A$1:$B$45,2)),"",VLOOKUP(Y33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA33" s="41"/>
       <c r="AB33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA33,Services!$A$1:$B$45,2)),"",VLOOKUP(AA33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC33" s="41"/>
@@ -9905,17 +9924,17 @@
       <c r="C34" s="42"/>
       <c r="D34" s="41"/>
       <c r="E34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D34,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D34,Region!$A$2:$B$11,2)),"",VLOOKUP(D34,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F34" s="41"/>
       <c r="G34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F34,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F34,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F34,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H34" s="41"/>
       <c r="I34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H34,'Base Locations'!A33:F373,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H34,'Base Locations'!A33:F373,2)),"",VLOOKUP(H34,'Base Locations'!A33:F373,2))</f>
         <v/>
       </c>
       <c r="J34" s="41"/>
@@ -9923,42 +9942,42 @@
       <c r="L34" s="41"/>
       <c r="M34" s="41"/>
       <c r="N34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M34,Services!$A$1:$B$45,2)),"",VLOOKUP(M34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O34" s="41"/>
       <c r="P34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O34,Services!$A$1:$B$45,2)),"",VLOOKUP(O34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q34" s="41"/>
       <c r="R34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q34,Services!$A$1:$B$45,2)),"",VLOOKUP(Q34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S34" s="41"/>
       <c r="T34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S34,Services!$A$1:$B$45,2)),"",VLOOKUP(S34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U34" s="41"/>
       <c r="V34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U34,Services!$A$1:$B$45,2)),"",VLOOKUP(U34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W34" s="41"/>
       <c r="X34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W34,Services!$A$1:$B$45,2)),"",VLOOKUP(W34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y34" s="41"/>
       <c r="Z34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y34,Services!$A$1:$B$45,2)),"",VLOOKUP(Y34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA34" s="41"/>
       <c r="AB34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA34,Services!$A$1:$B$45,2)),"",VLOOKUP(AA34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC34" s="41"/>
@@ -9970,17 +9989,17 @@
       <c r="C35" s="42"/>
       <c r="D35" s="41"/>
       <c r="E35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D35,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D35,Region!$A$2:$B$11,2)),"",VLOOKUP(D35,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F35" s="41"/>
       <c r="G35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F35,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F35,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F35,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H35" s="41"/>
       <c r="I35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H35,'Base Locations'!A34:F374,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H35,'Base Locations'!A34:F374,2)),"",VLOOKUP(H35,'Base Locations'!A34:F374,2))</f>
         <v/>
       </c>
       <c r="J35" s="41"/>
@@ -9988,42 +10007,42 @@
       <c r="L35" s="41"/>
       <c r="M35" s="41"/>
       <c r="N35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M35,Services!$A$1:$B$45,2)),"",VLOOKUP(M35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O35" s="41"/>
       <c r="P35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O35,Services!$A$1:$B$45,2)),"",VLOOKUP(O35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q35" s="41"/>
       <c r="R35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q35,Services!$A$1:$B$45,2)),"",VLOOKUP(Q35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S35" s="41"/>
       <c r="T35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S35,Services!$A$1:$B$45,2)),"",VLOOKUP(S35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U35" s="41"/>
       <c r="V35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U35,Services!$A$1:$B$45,2)),"",VLOOKUP(U35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W35" s="41"/>
       <c r="X35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W35,Services!$A$1:$B$45,2)),"",VLOOKUP(W35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y35" s="41"/>
       <c r="Z35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y35,Services!$A$1:$B$45,2)),"",VLOOKUP(Y35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA35" s="41"/>
       <c r="AB35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA35,Services!$A$1:$B$45,2)),"",VLOOKUP(AA35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC35" s="41"/>
@@ -10035,17 +10054,17 @@
       <c r="C36" s="42"/>
       <c r="D36" s="41"/>
       <c r="E36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D36,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D36,Region!$A$2:$B$11,2)),"",VLOOKUP(D36,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F36" s="41"/>
       <c r="G36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F36,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F36,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F36,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H36" s="41"/>
       <c r="I36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H36,'Base Locations'!A35:F375,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H36,'Base Locations'!A35:F375,2)),"",VLOOKUP(H36,'Base Locations'!A35:F375,2))</f>
         <v/>
       </c>
       <c r="J36" s="41"/>
@@ -10053,42 +10072,42 @@
       <c r="L36" s="41"/>
       <c r="M36" s="41"/>
       <c r="N36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M36,Services!$A$1:$B$45,2)),"",VLOOKUP(M36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O36" s="41"/>
       <c r="P36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O36,Services!$A$1:$B$45,2)),"",VLOOKUP(O36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q36" s="41"/>
       <c r="R36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q36,Services!$A$1:$B$45,2)),"",VLOOKUP(Q36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S36" s="41"/>
       <c r="T36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S36,Services!$A$1:$B$45,2)),"",VLOOKUP(S36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U36" s="41"/>
       <c r="V36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U36,Services!$A$1:$B$45,2)),"",VLOOKUP(U36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W36" s="41"/>
       <c r="X36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W36,Services!$A$1:$B$45,2)),"",VLOOKUP(W36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y36" s="41"/>
       <c r="Z36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y36,Services!$A$1:$B$45,2)),"",VLOOKUP(Y36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA36" s="41"/>
       <c r="AB36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA36,Services!$A$1:$B$45,2)),"",VLOOKUP(AA36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC36" s="41"/>
@@ -10100,17 +10119,17 @@
       <c r="C37" s="42"/>
       <c r="D37" s="41"/>
       <c r="E37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D37,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D37,Region!$A$2:$B$11,2)),"",VLOOKUP(D37,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F37" s="41"/>
       <c r="G37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F37,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F37,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F37,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H37" s="41"/>
       <c r="I37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H37,'Base Locations'!A36:F376,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H37,'Base Locations'!A36:F376,2)),"",VLOOKUP(H37,'Base Locations'!A36:F376,2))</f>
         <v/>
       </c>
       <c r="J37" s="41"/>
@@ -10118,42 +10137,42 @@
       <c r="L37" s="41"/>
       <c r="M37" s="41"/>
       <c r="N37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M37,Services!$A$1:$B$45,2)),"",VLOOKUP(M37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O37" s="41"/>
       <c r="P37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O37,Services!$A$1:$B$45,2)),"",VLOOKUP(O37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q37" s="41"/>
       <c r="R37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q37,Services!$A$1:$B$45,2)),"",VLOOKUP(Q37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S37" s="41"/>
       <c r="T37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S37,Services!$A$1:$B$45,2)),"",VLOOKUP(S37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U37" s="41"/>
       <c r="V37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U37,Services!$A$1:$B$45,2)),"",VLOOKUP(U37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W37" s="41"/>
       <c r="X37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W37,Services!$A$1:$B$45,2)),"",VLOOKUP(W37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y37" s="41"/>
       <c r="Z37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y37,Services!$A$1:$B$45,2)),"",VLOOKUP(Y37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA37" s="41"/>
       <c r="AB37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA37,Services!$A$1:$B$45,2)),"",VLOOKUP(AA37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC37" s="41"/>
@@ -10165,17 +10184,17 @@
       <c r="C38" s="42"/>
       <c r="D38" s="41"/>
       <c r="E38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D38,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D38,Region!$A$2:$B$11,2)),"",VLOOKUP(D38,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F38" s="41"/>
       <c r="G38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F38,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F38,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F38,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H38" s="41"/>
       <c r="I38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H38,'Base Locations'!A37:F377,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H38,'Base Locations'!A37:F377,2)),"",VLOOKUP(H38,'Base Locations'!A37:F377,2))</f>
         <v/>
       </c>
       <c r="J38" s="41"/>
@@ -10183,42 +10202,42 @@
       <c r="L38" s="41"/>
       <c r="M38" s="41"/>
       <c r="N38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M38,Services!$A$1:$B$45,2)),"",VLOOKUP(M38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O38" s="41"/>
       <c r="P38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O38,Services!$A$1:$B$45,2)),"",VLOOKUP(O38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q38" s="41"/>
       <c r="R38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q38,Services!$A$1:$B$45,2)),"",VLOOKUP(Q38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S38" s="41"/>
       <c r="T38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S38,Services!$A$1:$B$45,2)),"",VLOOKUP(S38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U38" s="41"/>
       <c r="V38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U38,Services!$A$1:$B$45,2)),"",VLOOKUP(U38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W38" s="41"/>
       <c r="X38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W38,Services!$A$1:$B$45,2)),"",VLOOKUP(W38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y38" s="41"/>
       <c r="Z38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y38,Services!$A$1:$B$45,2)),"",VLOOKUP(Y38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA38" s="41"/>
       <c r="AB38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA38,Services!$A$1:$B$45,2)),"",VLOOKUP(AA38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC38" s="41"/>
@@ -10230,17 +10249,17 @@
       <c r="C39" s="42"/>
       <c r="D39" s="41"/>
       <c r="E39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D39,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D39,Region!$A$2:$B$11,2)),"",VLOOKUP(D39,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F39" s="41"/>
       <c r="G39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F39,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F39,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F39,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H39" s="41"/>
       <c r="I39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H39,'Base Locations'!A38:F378,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H39,'Base Locations'!A38:F378,2)),"",VLOOKUP(H39,'Base Locations'!A38:F378,2))</f>
         <v/>
       </c>
       <c r="J39" s="41"/>
@@ -10248,42 +10267,42 @@
       <c r="L39" s="41"/>
       <c r="M39" s="41"/>
       <c r="N39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M39,Services!$A$1:$B$45,2)),"",VLOOKUP(M39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O39" s="41"/>
       <c r="P39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O39,Services!$A$1:$B$45,2)),"",VLOOKUP(O39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q39" s="41"/>
       <c r="R39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q39,Services!$A$1:$B$45,2)),"",VLOOKUP(Q39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S39" s="41"/>
       <c r="T39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S39,Services!$A$1:$B$45,2)),"",VLOOKUP(S39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U39" s="41"/>
       <c r="V39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U39,Services!$A$1:$B$45,2)),"",VLOOKUP(U39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W39" s="41"/>
       <c r="X39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W39,Services!$A$1:$B$45,2)),"",VLOOKUP(W39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y39" s="41"/>
       <c r="Z39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y39,Services!$A$1:$B$45,2)),"",VLOOKUP(Y39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA39" s="41"/>
       <c r="AB39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA39,Services!$A$1:$B$45,2)),"",VLOOKUP(AA39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC39" s="41"/>
@@ -10295,17 +10314,17 @@
       <c r="C40" s="42"/>
       <c r="D40" s="41"/>
       <c r="E40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D40,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D40,Region!$A$2:$B$11,2)),"",VLOOKUP(D40,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F40" s="41"/>
       <c r="G40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F40,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F40,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F40,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H40" s="41"/>
       <c r="I40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H40,'Base Locations'!A39:F379,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H40,'Base Locations'!A39:F379,2)),"",VLOOKUP(H40,'Base Locations'!A39:F379,2))</f>
         <v/>
       </c>
       <c r="J40" s="41"/>
@@ -10313,42 +10332,42 @@
       <c r="L40" s="41"/>
       <c r="M40" s="41"/>
       <c r="N40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M40,Services!$A$1:$B$45,2)),"",VLOOKUP(M40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O40" s="41"/>
       <c r="P40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O40,Services!$A$1:$B$45,2)),"",VLOOKUP(O40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q40" s="41"/>
       <c r="R40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q40,Services!$A$1:$B$45,2)),"",VLOOKUP(Q40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S40" s="41"/>
       <c r="T40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S40,Services!$A$1:$B$45,2)),"",VLOOKUP(S40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U40" s="41"/>
       <c r="V40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U40,Services!$A$1:$B$45,2)),"",VLOOKUP(U40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W40" s="41"/>
       <c r="X40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W40,Services!$A$1:$B$45,2)),"",VLOOKUP(W40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y40" s="41"/>
       <c r="Z40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y40,Services!$A$1:$B$45,2)),"",VLOOKUP(Y40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA40" s="41"/>
       <c r="AB40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA40,Services!$A$1:$B$45,2)),"",VLOOKUP(AA40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC40" s="41"/>
@@ -10360,17 +10379,17 @@
       <c r="C41" s="42"/>
       <c r="D41" s="41"/>
       <c r="E41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D41,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D41,Region!$A$2:$B$11,2)),"",VLOOKUP(D41,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F41" s="41"/>
       <c r="G41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F41,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F41,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F41,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H41" s="41"/>
       <c r="I41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H41,'Base Locations'!A40:F380,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H41,'Base Locations'!A40:F380,2)),"",VLOOKUP(H41,'Base Locations'!A40:F380,2))</f>
         <v/>
       </c>
       <c r="J41" s="41"/>
@@ -10378,42 +10397,42 @@
       <c r="L41" s="41"/>
       <c r="M41" s="41"/>
       <c r="N41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M41,Services!$A$1:$B$45,2)),"",VLOOKUP(M41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O41" s="41"/>
       <c r="P41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O41,Services!$A$1:$B$45,2)),"",VLOOKUP(O41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q41" s="41"/>
       <c r="R41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q41,Services!$A$1:$B$45,2)),"",VLOOKUP(Q41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S41" s="41"/>
       <c r="T41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S41,Services!$A$1:$B$45,2)),"",VLOOKUP(S41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U41" s="41"/>
       <c r="V41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U41,Services!$A$1:$B$45,2)),"",VLOOKUP(U41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W41" s="41"/>
       <c r="X41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W41,Services!$A$1:$B$45,2)),"",VLOOKUP(W41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y41" s="41"/>
       <c r="Z41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y41,Services!$A$1:$B$45,2)),"",VLOOKUP(Y41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA41" s="41"/>
       <c r="AB41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA41,Services!$A$1:$B$45,2)),"",VLOOKUP(AA41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC41" s="41"/>
@@ -10425,17 +10444,17 @@
       <c r="C42" s="42"/>
       <c r="D42" s="41"/>
       <c r="E42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D42,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D42,Region!$A$2:$B$11,2)),"",VLOOKUP(D42,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F42" s="41"/>
       <c r="G42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F42,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F42,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F42,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H42" s="41"/>
       <c r="I42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H42,'Base Locations'!A41:F381,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H42,'Base Locations'!A41:F381,2)),"",VLOOKUP(H42,'Base Locations'!A41:F381,2))</f>
         <v/>
       </c>
       <c r="J42" s="41"/>
@@ -10443,42 +10462,42 @@
       <c r="L42" s="41"/>
       <c r="M42" s="41"/>
       <c r="N42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M42,Services!$A$1:$B$45,2)),"",VLOOKUP(M42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O42" s="41"/>
       <c r="P42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O42,Services!$A$1:$B$45,2)),"",VLOOKUP(O42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q42" s="41"/>
       <c r="R42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q42,Services!$A$1:$B$45,2)),"",VLOOKUP(Q42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S42" s="41"/>
       <c r="T42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S42,Services!$A$1:$B$45,2)),"",VLOOKUP(S42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U42" s="41"/>
       <c r="V42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U42,Services!$A$1:$B$45,2)),"",VLOOKUP(U42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W42" s="41"/>
       <c r="X42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W42,Services!$A$1:$B$45,2)),"",VLOOKUP(W42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y42" s="41"/>
       <c r="Z42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y42,Services!$A$1:$B$45,2)),"",VLOOKUP(Y42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA42" s="41"/>
       <c r="AB42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA42,Services!$A$1:$B$45,2)),"",VLOOKUP(AA42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC42" s="41"/>
@@ -10490,17 +10509,17 @@
       <c r="C43" s="42"/>
       <c r="D43" s="41"/>
       <c r="E43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D43,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D43,Region!$A$2:$B$11,2)),"",VLOOKUP(D43,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F43" s="41"/>
       <c r="G43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F43,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F43,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F43,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H43" s="41"/>
       <c r="I43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H43,'Base Locations'!A42:F382,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H43,'Base Locations'!A42:F382,2)),"",VLOOKUP(H43,'Base Locations'!A42:F382,2))</f>
         <v/>
       </c>
       <c r="J43" s="41"/>
@@ -10508,42 +10527,42 @@
       <c r="L43" s="41"/>
       <c r="M43" s="41"/>
       <c r="N43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M43,Services!$A$1:$B$45,2)),"",VLOOKUP(M43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O43" s="41"/>
       <c r="P43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O43,Services!$A$1:$B$45,2)),"",VLOOKUP(O43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q43" s="41"/>
       <c r="R43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q43,Services!$A$1:$B$45,2)),"",VLOOKUP(Q43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S43" s="41"/>
       <c r="T43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S43,Services!$A$1:$B$45,2)),"",VLOOKUP(S43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U43" s="41"/>
       <c r="V43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U43,Services!$A$1:$B$45,2)),"",VLOOKUP(U43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W43" s="41"/>
       <c r="X43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W43,Services!$A$1:$B$45,2)),"",VLOOKUP(W43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y43" s="41"/>
       <c r="Z43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y43,Services!$A$1:$B$45,2)),"",VLOOKUP(Y43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA43" s="41"/>
       <c r="AB43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA43,Services!$A$1:$B$45,2)),"",VLOOKUP(AA43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC43" s="41"/>
@@ -10555,17 +10574,17 @@
       <c r="C44" s="42"/>
       <c r="D44" s="41"/>
       <c r="E44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D44,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D44,Region!$A$2:$B$11,2)),"",VLOOKUP(D44,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F44" s="41"/>
       <c r="G44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F44,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F44,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F44,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H44" s="41"/>
       <c r="I44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H44,'Base Locations'!A43:F383,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H44,'Base Locations'!A43:F383,2)),"",VLOOKUP(H44,'Base Locations'!A43:F383,2))</f>
         <v/>
       </c>
       <c r="J44" s="41"/>
@@ -10573,42 +10592,42 @@
       <c r="L44" s="41"/>
       <c r="M44" s="41"/>
       <c r="N44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M44,Services!$A$1:$B$45,2)),"",VLOOKUP(M44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O44" s="41"/>
       <c r="P44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O44,Services!$A$1:$B$45,2)),"",VLOOKUP(O44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q44" s="41"/>
       <c r="R44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q44,Services!$A$1:$B$45,2)),"",VLOOKUP(Q44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S44" s="41"/>
       <c r="T44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S44,Services!$A$1:$B$45,2)),"",VLOOKUP(S44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U44" s="41"/>
       <c r="V44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U44,Services!$A$1:$B$45,2)),"",VLOOKUP(U44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W44" s="41"/>
       <c r="X44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W44,Services!$A$1:$B$45,2)),"",VLOOKUP(W44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y44" s="41"/>
       <c r="Z44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y44,Services!$A$1:$B$45,2)),"",VLOOKUP(Y44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA44" s="41"/>
       <c r="AB44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA44,Services!$A$1:$B$45,2)),"",VLOOKUP(AA44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC44" s="41"/>
@@ -10620,17 +10639,17 @@
       <c r="C45" s="42"/>
       <c r="D45" s="41"/>
       <c r="E45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D45,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D45,Region!$A$2:$B$11,2)),"",VLOOKUP(D45,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F45" s="41"/>
       <c r="G45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F45,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F45,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F45,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H45" s="41"/>
       <c r="I45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H45,'Base Locations'!A44:F384,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H45,'Base Locations'!A44:F384,2)),"",VLOOKUP(H45,'Base Locations'!A44:F384,2))</f>
         <v/>
       </c>
       <c r="J45" s="41"/>
@@ -10638,42 +10657,42 @@
       <c r="L45" s="41"/>
       <c r="M45" s="41"/>
       <c r="N45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M45,Services!$A$1:$B$45,2)),"",VLOOKUP(M45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O45" s="41"/>
       <c r="P45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O45,Services!$A$1:$B$45,2)),"",VLOOKUP(O45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q45" s="41"/>
       <c r="R45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q45,Services!$A$1:$B$45,2)),"",VLOOKUP(Q45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S45" s="41"/>
       <c r="T45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S45,Services!$A$1:$B$45,2)),"",VLOOKUP(S45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U45" s="41"/>
       <c r="V45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U45,Services!$A$1:$B$45,2)),"",VLOOKUP(U45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W45" s="41"/>
       <c r="X45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W45,Services!$A$1:$B$45,2)),"",VLOOKUP(W45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y45" s="41"/>
       <c r="Z45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y45,Services!$A$1:$B$45,2)),"",VLOOKUP(Y45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA45" s="41"/>
       <c r="AB45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA45,Services!$A$1:$B$45,2)),"",VLOOKUP(AA45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC45" s="41"/>
@@ -10685,17 +10704,17 @@
       <c r="C46" s="42"/>
       <c r="D46" s="41"/>
       <c r="E46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D46,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D46,Region!$A$2:$B$11,2)),"",VLOOKUP(D46,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F46" s="41"/>
       <c r="G46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F46,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F46,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F46,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H46" s="41"/>
       <c r="I46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H46,'Base Locations'!A45:F385,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H46,'Base Locations'!A45:F385,2)),"",VLOOKUP(H46,'Base Locations'!A45:F385,2))</f>
         <v/>
       </c>
       <c r="J46" s="41"/>
@@ -10703,42 +10722,42 @@
       <c r="L46" s="41"/>
       <c r="M46" s="41"/>
       <c r="N46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M46,Services!$A$1:$B$45,2)),"",VLOOKUP(M46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O46" s="41"/>
       <c r="P46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O46,Services!$A$1:$B$45,2)),"",VLOOKUP(O46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q46" s="41"/>
       <c r="R46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q46,Services!$A$1:$B$45,2)),"",VLOOKUP(Q46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S46" s="41"/>
       <c r="T46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S46,Services!$A$1:$B$45,2)),"",VLOOKUP(S46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U46" s="41"/>
       <c r="V46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U46,Services!$A$1:$B$45,2)),"",VLOOKUP(U46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W46" s="41"/>
       <c r="X46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W46,Services!$A$1:$B$45,2)),"",VLOOKUP(W46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y46" s="41"/>
       <c r="Z46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y46,Services!$A$1:$B$45,2)),"",VLOOKUP(Y46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA46" s="41"/>
       <c r="AB46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA46,Services!$A$1:$B$45,2)),"",VLOOKUP(AA46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC46" s="41"/>
@@ -10750,17 +10769,17 @@
       <c r="C47" s="42"/>
       <c r="D47" s="41"/>
       <c r="E47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D47,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D47,Region!$A$2:$B$11,2)),"",VLOOKUP(D47,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F47" s="41"/>
       <c r="G47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F47,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F47,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F47,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H47" s="41"/>
       <c r="I47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H47,'Base Locations'!A46:F386,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H47,'Base Locations'!A46:F386,2)),"",VLOOKUP(H47,'Base Locations'!A46:F386,2))</f>
         <v/>
       </c>
       <c r="J47" s="41"/>
@@ -10768,42 +10787,42 @@
       <c r="L47" s="41"/>
       <c r="M47" s="41"/>
       <c r="N47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M47,Services!$A$1:$B$45,2)),"",VLOOKUP(M47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O47" s="41"/>
       <c r="P47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O47,Services!$A$1:$B$45,2)),"",VLOOKUP(O47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q47" s="41"/>
       <c r="R47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q47,Services!$A$1:$B$45,2)),"",VLOOKUP(Q47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S47" s="41"/>
       <c r="T47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S47,Services!$A$1:$B$45,2)),"",VLOOKUP(S47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U47" s="41"/>
       <c r="V47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U47,Services!$A$1:$B$45,2)),"",VLOOKUP(U47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W47" s="41"/>
       <c r="X47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W47,Services!$A$1:$B$45,2)),"",VLOOKUP(W47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y47" s="41"/>
       <c r="Z47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y47,Services!$A$1:$B$45,2)),"",VLOOKUP(Y47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA47" s="41"/>
       <c r="AB47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA47,Services!$A$1:$B$45,2)),"",VLOOKUP(AA47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC47" s="41"/>
@@ -10815,17 +10834,17 @@
       <c r="C48" s="42"/>
       <c r="D48" s="41"/>
       <c r="E48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D48,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D48,Region!$A$2:$B$11,2)),"",VLOOKUP(D48,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F48" s="41"/>
       <c r="G48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F48,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F48,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F48,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H48" s="41"/>
       <c r="I48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H48,'Base Locations'!A47:F387,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H48,'Base Locations'!A47:F387,2)),"",VLOOKUP(H48,'Base Locations'!A47:F387,2))</f>
         <v/>
       </c>
       <c r="J48" s="41"/>
@@ -10833,42 +10852,42 @@
       <c r="L48" s="41"/>
       <c r="M48" s="41"/>
       <c r="N48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M48,Services!$A$1:$B$45,2)),"",VLOOKUP(M48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O48" s="41"/>
       <c r="P48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O48,Services!$A$1:$B$45,2)),"",VLOOKUP(O48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q48" s="41"/>
       <c r="R48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q48,Services!$A$1:$B$45,2)),"",VLOOKUP(Q48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S48" s="41"/>
       <c r="T48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S48,Services!$A$1:$B$45,2)),"",VLOOKUP(S48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U48" s="41"/>
       <c r="V48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U48,Services!$A$1:$B$45,2)),"",VLOOKUP(U48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W48" s="41"/>
       <c r="X48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W48,Services!$A$1:$B$45,2)),"",VLOOKUP(W48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y48" s="41"/>
       <c r="Z48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y48,Services!$A$1:$B$45,2)),"",VLOOKUP(Y48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA48" s="41"/>
       <c r="AB48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA48,Services!$A$1:$B$45,2)),"",VLOOKUP(AA48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC48" s="41"/>
@@ -10880,17 +10899,17 @@
       <c r="C49" s="42"/>
       <c r="D49" s="41"/>
       <c r="E49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D49,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D49,Region!$A$2:$B$11,2)),"",VLOOKUP(D49,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F49" s="41"/>
       <c r="G49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F49,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F49,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F49,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H49" s="41"/>
       <c r="I49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H49,'Base Locations'!A48:F388,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H49,'Base Locations'!A48:F388,2)),"",VLOOKUP(H49,'Base Locations'!A48:F388,2))</f>
         <v/>
       </c>
       <c r="J49" s="41"/>
@@ -10898,42 +10917,42 @@
       <c r="L49" s="41"/>
       <c r="M49" s="41"/>
       <c r="N49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M49,Services!$A$1:$B$45,2)),"",VLOOKUP(M49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O49" s="41"/>
       <c r="P49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O49,Services!$A$1:$B$45,2)),"",VLOOKUP(O49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q49" s="41"/>
       <c r="R49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q49,Services!$A$1:$B$45,2)),"",VLOOKUP(Q49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S49" s="41"/>
       <c r="T49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S49,Services!$A$1:$B$45,2)),"",VLOOKUP(S49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U49" s="41"/>
       <c r="V49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U49,Services!$A$1:$B$45,2)),"",VLOOKUP(U49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W49" s="41"/>
       <c r="X49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W49,Services!$A$1:$B$45,2)),"",VLOOKUP(W49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y49" s="41"/>
       <c r="Z49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y49,Services!$A$1:$B$45,2)),"",VLOOKUP(Y49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA49" s="41"/>
       <c r="AB49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA49,Services!$A$1:$B$45,2)),"",VLOOKUP(AA49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC49" s="41"/>
@@ -10945,17 +10964,17 @@
       <c r="C50" s="42"/>
       <c r="D50" s="41"/>
       <c r="E50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D50,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D50,Region!$A$2:$B$11,2)),"",VLOOKUP(D50,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F50" s="41"/>
       <c r="G50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F50,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F50,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F50,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H50" s="41"/>
       <c r="I50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H50,'Base Locations'!A49:F389,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H50,'Base Locations'!A49:F389,2)),"",VLOOKUP(H50,'Base Locations'!A49:F389,2))</f>
         <v/>
       </c>
       <c r="J50" s="41"/>
@@ -10963,49 +10982,49 @@
       <c r="L50" s="41"/>
       <c r="M50" s="41"/>
       <c r="N50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M50,Services!$A$1:$B$45,2)),"",VLOOKUP(M50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O50" s="41"/>
       <c r="P50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O50,Services!$A$1:$B$45,2)),"",VLOOKUP(O50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q50" s="41"/>
       <c r="R50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q50,Services!$A$1:$B$45,2)),"",VLOOKUP(Q50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S50" s="41"/>
       <c r="T50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S50,Services!$A$1:$B$45,2)),"",VLOOKUP(S50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U50" s="41"/>
       <c r="V50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U50,Services!$A$1:$B$45,2)),"",VLOOKUP(U50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W50" s="41"/>
       <c r="X50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W50,Services!$A$1:$B$45,2)),"",VLOOKUP(W50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y50" s="41"/>
       <c r="Z50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y50,Services!$A$1:$B$45,2)),"",VLOOKUP(Y50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA50" s="41"/>
       <c r="AB50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA50,Services!$A$1:$B$45,2)),"",VLOOKUP(AA50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC50" s="41"/>
       <c r="AD50" s="41"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="WAaZ35wRl78ipiLsjfD57CyB3HV/XTkh+AkpuITrgzbsCulipizsGtzZA633/Z+avY7gs2bxn5onauLD9tGmuQ==" saltValue="T3F9NByxyx7ZjTQE4ykYyg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="6oyb3rRRfKDqti5GQJdNRgETALv5BhypIRzP7ad5VgVRdJpgy9LUEIpAIaOgXLHmnqidCaz2KGK7nd1sygRpVQ==" saltValue="jaug0yiNYL4uUSxB9UIkgQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -11066,7 +11085,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.5" collapsed="true"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -11112,7 +11131,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -11495,13 +11514,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="48.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="16" width="14.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="19" width="12.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="22" width="13.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="19" width="39.83203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="25" width="15.5" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="51.5" collapsed="true"/>
+    <col min="1" max="1" width="48.5" customWidth="1"/>
+    <col min="2" max="2" width="14" style="16" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="22" customWidth="1"/>
+    <col min="5" max="5" width="39.83203125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="25" customWidth="1"/>
+    <col min="7" max="7" width="51.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -18820,8 +18839,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.1640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="9.5" collapsed="true"/>
+    <col min="1" max="1" width="27.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: RDCC-2389 Updated code to align with the Latest Excel File (#168)
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE97A472-D0B0-1947-BA11-D62D757BD41E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8991DFDA-2383-614C-A1EB-BFD86ABD8430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19540" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="11" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="1199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="1200">
   <si>
     <t>Region</t>
   </si>
@@ -3641,13 +3641,15 @@
   </si>
   <si>
     <t>Future Operations</t>
+  </si>
+  <si>
+    <t>caseworker-iac</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4932,7 +4934,7 @@
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AB98"/>
+  <dimension ref="A1:AH98"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="X90" sqref="X90"/>
@@ -4940,7 +4942,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="29" max="34" style="32" width="9.1640625" collapsed="true"/>
+    <col min="29" max="34" width="9.1640625" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="26" x14ac:dyDescent="0.3">
@@ -7446,8 +7448,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="104.1640625" collapsed="true"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="104.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -7639,42 +7641,42 @@
   </sheetPr>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="40" width="21.83203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="40" width="24.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="40" width="30.1640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="40" width="20.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" hidden="true" width="20.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="40" width="62.5" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" hidden="true" width="33.83203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="40" width="49.83203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" hidden="true" width="32.1640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="40" width="15.5" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="40" width="25.5" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="40" width="19.5" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="40" width="24.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" hidden="true" width="24.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="40" width="21.33203125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" hidden="true" width="21.33203125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" style="40" width="19.1640625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" hidden="true" width="19.1640625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="40" width="19.1640625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" hidden="true" width="19.1640625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="40" width="16.0" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" hidden="true" width="16.0" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="40" width="14.5" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" hidden="true" width="14.5" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="40" width="17.33203125" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" hidden="true" width="17.33203125" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="40" width="14.5" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" hidden="true" width="14.5" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="40" width="25.5" collapsed="true"/>
-    <col min="30" max="30" style="40" width="9.1640625" collapsed="true"/>
+    <col min="1" max="1" width="21.83203125" style="40" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="40" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" style="40" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="40" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="62.5" style="40" customWidth="1"/>
+    <col min="7" max="7" width="33.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="49.83203125" style="40" customWidth="1"/>
+    <col min="9" max="9" width="32.1640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="40" customWidth="1"/>
+    <col min="11" max="11" width="25.5" style="40" customWidth="1"/>
+    <col min="12" max="12" width="19.5" style="40" customWidth="1"/>
+    <col min="13" max="13" width="24" style="40" customWidth="1"/>
+    <col min="14" max="14" width="24" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="21.33203125" style="40" customWidth="1"/>
+    <col min="16" max="16" width="21.33203125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="19.1640625" style="40" customWidth="1"/>
+    <col min="18" max="18" width="19.1640625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" style="40" customWidth="1"/>
+    <col min="20" max="20" width="19.1640625" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="16" style="40" customWidth="1"/>
+    <col min="22" max="22" width="16" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5" style="40" customWidth="1"/>
+    <col min="24" max="24" width="14.5" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" style="40" customWidth="1"/>
+    <col min="26" max="26" width="17.33203125" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5" style="40" customWidth="1"/>
+    <col min="28" max="28" width="14.5" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="25.5" style="40" customWidth="1"/>
+    <col min="30" max="30" width="9.1640625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -7772,89 +7774,89 @@
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>2240op</v>
+        <v>0851oe</v>
       </c>
       <c r="B2" s="41" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>2107nr</v>
+        <v>4676fi</v>
       </c>
       <c r="C2" s="42" t="str">
         <f ca="1">CONCATENATE(A2,".",B2,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>2240op.2107nr501320@justice.gov.uk</v>
+        <v>0851oe.4676fi511977@justice.gov.uk</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1">
-        <f>_xlfn.IFNA(VLOOKUP(D2,Region!$A$2:$B$11,2),"")</f>
-        <v>2</v>
+        <f>IF(ISNA(VLOOKUP(D2,Region!$A$2:$B$11,2)),"",VLOOKUP(D2,Region!$A$2:$B$11,2))</f>
+        <v>3</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G2" s="1">
-        <f>_xlfn.IFNA(VLOOKUP(F2,'Base Locations'!$A$1:$F$341,2),"")</f>
-        <v>219164</v>
+        <f>IF(ISNA(VLOOKUP(F2,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F2,'Base Locations'!$A$1:$F$341,2))</f>
+        <v>271588</v>
       </c>
       <c r="H2" s="41" t="s">
         <v>74</v>
       </c>
       <c r="I2" s="1">
-        <f>_xlfn.IFNA(VLOOKUP(H2,'Base Locations'!A1:F341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H2,'Base Locations'!A1:F341,2)),"",VLOOKUP(H2,'Base Locations'!A1:F341,2))</f>
         <v>817181</v>
       </c>
       <c r="J2" s="41" t="s">
         <v>52</v>
       </c>
       <c r="K2" s="41" t="s">
-        <v>408</v>
-      </c>
-      <c r="L2" s="41" t="s">
         <v>409</v>
       </c>
+      <c r="L2" s="41"/>
       <c r="M2" s="41" t="s">
-        <v>13</v>
+        <v>1169</v>
       </c>
       <c r="N2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M2,Services!$A$1:$B$45,2),"")</f>
-        <v>BAB1</v>
+        <f>IF(ISNA(VLOOKUP(M2,Services!$A$1:$B$45,2)),"",VLOOKUP(M2,Services!$A$1:$B$45,2))</f>
+        <v>BHA3</v>
       </c>
       <c r="O2" s="41"/>
       <c r="P2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O2,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O2,Services!$A$1:$B$45,2)),"",VLOOKUP(O2,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q2" s="41"/>
       <c r="R2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q2,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q2,Services!$A$1:$B$45,2)),"",VLOOKUP(Q2,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S2" s="41"/>
       <c r="T2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S2,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S2,Services!$A$1:$B$45,2)),"",VLOOKUP(S2,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U2" s="41"/>
       <c r="V2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U2,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U2,Services!$A$1:$B$45,2)),"",VLOOKUP(U2,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W2" s="41"/>
       <c r="X2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W2,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W2,Services!$A$1:$B$45,2)),"",VLOOKUP(W2,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y2" s="41"/>
       <c r="Z2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y2,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y2,Services!$A$1:$B$45,2)),"",VLOOKUP(Y2,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA2" s="41"/>
       <c r="AB2" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA2,Services!$A$1:$B$45,2),"")</f>
-        <v/>
-      </c>
-      <c r="AC2" s="41"/>
+        <f>IF(ISNA(VLOOKUP(AA2,Services!$A$1:$B$45,2)),"",VLOOKUP(AA2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AC2" s="41" t="s">
+        <v>1199</v>
+      </c>
       <c r="AD2" s="41" t="s">
         <v>1121</v>
       </c>
@@ -7862,86 +7864,82 @@
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>3809cc</v>
+        <v>0803pw</v>
       </c>
       <c r="B3" s="41" t="str">
         <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>9166tg</v>
+        <v>2686td</v>
       </c>
       <c r="C3" s="42" t="str">
         <f ca="1">CONCATENATE(A3,".",B3,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>3809cc.9166tg299028@justice.gov.uk</v>
+        <v>0803pw.2686td494233@justice.gov.uk</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1">
-        <f>_xlfn.IFNA(VLOOKUP(D3,Region!$A$2:$B$11,2),"")</f>
-        <v>3</v>
+        <f>IF(ISNA(VLOOKUP(D3,Region!$A$2:$B$11,2)),"",VLOOKUP(D3,Region!$A$2:$B$11,2))</f>
+        <v>4</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G3" s="1">
-        <f>_xlfn.IFNA(VLOOKUP(F3,'Base Locations'!$A$1:$F$341,2),"")</f>
-        <v>229786</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="1">
-        <f>_xlfn.IFNA(VLOOKUP(H3,'Base Locations'!A2:F342,2),"")</f>
-        <v>574546</v>
+        <f>IF(ISNA(VLOOKUP(F3,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F3,'Base Locations'!$A$1:$F$341,2))</f>
+        <v>206150</v>
+      </c>
+      <c r="H3" s="41"/>
+      <c r="I3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(H3,'Base Locations'!A2:F342,2)),"",VLOOKUP(H3,'Base Locations'!A2:F342,2))</f>
+        <v/>
       </c>
       <c r="J3" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="41" t="s">
-        <v>408</v>
-      </c>
+        <v>1198</v>
+      </c>
+      <c r="K3" s="41"/>
       <c r="L3" s="41" t="s">
         <v>409</v>
       </c>
-      <c r="M3" s="41" t="s">
-        <v>14</v>
-      </c>
+      <c r="M3" s="41"/>
       <c r="N3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M3,Services!$A$1:$B$45,2),"")</f>
-        <v>BAA4</v>
-      </c>
-      <c r="O3" s="41"/>
+        <f>IF(ISNA(VLOOKUP(M3,Services!$A$1:$B$45,2)),"",VLOOKUP(M3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="O3" s="41" t="s">
+        <v>1168</v>
+      </c>
       <c r="P3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O3,Services!$A$1:$B$45,2),"")</f>
-        <v/>
+        <f>IF(ISNA(VLOOKUP(O3,Services!$A$1:$B$45,2)),"",VLOOKUP(O3,Services!$A$1:$B$45,2))</f>
+        <v>BAB2</v>
       </c>
       <c r="Q3" s="41"/>
       <c r="R3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q3,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q3,Services!$A$1:$B$45,2)),"",VLOOKUP(Q3,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S3" s="41"/>
       <c r="T3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S3,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S3,Services!$A$1:$B$45,2)),"",VLOOKUP(S3,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U3" s="41"/>
       <c r="V3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U3,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U3,Services!$A$1:$B$45,2)),"",VLOOKUP(U3,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W3" s="41"/>
       <c r="X3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W3,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W3,Services!$A$1:$B$45,2)),"",VLOOKUP(W3,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y3" s="41"/>
       <c r="Z3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y3,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y3,Services!$A$1:$B$45,2)),"",VLOOKUP(Y3,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA3" s="41"/>
       <c r="AB3" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA3,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA3,Services!$A$1:$B$45,2)),"",VLOOKUP(AA3,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC3" s="41"/>
@@ -7950,65 +7948,86 @@
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D4,Region!$A$2:$B$11,2),"")</f>
-        <v/>
-      </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F4,'Base Locations'!$A$1:$F$341,2),"")</f>
-        <v/>
-      </c>
-      <c r="H4" s="41"/>
-      <c r="I4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H4,'Base Locations'!A3:F343,2),"")</f>
-        <v/>
-      </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
+      <c r="A4" s="41" t="str">
+        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
+        <v>5444qe</v>
+      </c>
+      <c r="B4" s="41" t="str">
+        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
+        <v>7318rb</v>
+      </c>
+      <c r="C4" s="42" t="str">
+        <f ca="1">CONCATENATE(A4,".",B4,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
+        <v>5444qe.7318rb44305@justice.gov.uk</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <f>IF(ISNA(VLOOKUP(D4,Region!$A$2:$B$11,2)),"",VLOOKUP(D4,Region!$A$2:$B$11,2))</f>
+        <v>5</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="1">
+        <f>IF(ISNA(VLOOKUP(F4,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F4,'Base Locations'!$A$1:$F$341,2))</f>
+        <v>574546</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="1">
+        <f>IF(ISNA(VLOOKUP(H4,'Base Locations'!A3:F343,2)),"",VLOOKUP(H4,'Base Locations'!A3:F343,2))</f>
+        <v>229786</v>
+      </c>
+      <c r="J4" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="41" t="s">
+        <v>408</v>
+      </c>
       <c r="L4" s="41"/>
       <c r="M4" s="41"/>
       <c r="N4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M4,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M4,Services!$A$1:$B$45,2)),"",VLOOKUP(M4,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O4" s="41"/>
       <c r="P4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O4,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O4,Services!$A$1:$B$45,2)),"",VLOOKUP(O4,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q4" s="41"/>
       <c r="R4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q4,Services!$A$1:$B$45,2),"")</f>
-        <v/>
-      </c>
-      <c r="S4" s="41"/>
+        <f>IF(ISNA(VLOOKUP(Q4,Services!$A$1:$B$45,2)),"",VLOOKUP(Q4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="S4" s="41" t="s">
+        <v>1167</v>
+      </c>
       <c r="T4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S4,Services!$A$1:$B$45,2),"")</f>
-        <v/>
+        <f>IF(ISNA(VLOOKUP(S4,Services!$A$1:$B$45,2)),"",VLOOKUP(S4,Services!$A$1:$B$45,2))</f>
+        <v>BAB2</v>
       </c>
       <c r="U4" s="41"/>
       <c r="V4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U4,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U4,Services!$A$1:$B$45,2)),"",VLOOKUP(U4,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W4" s="41"/>
       <c r="X4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W4,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W4,Services!$A$1:$B$45,2)),"",VLOOKUP(W4,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y4" s="41"/>
       <c r="Z4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y4,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y4,Services!$A$1:$B$45,2)),"",VLOOKUP(Y4,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA4" s="41"/>
       <c r="AB4" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA4,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA4,Services!$A$1:$B$45,2)),"",VLOOKUP(AA4,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC4" s="41"/>
@@ -8020,17 +8039,17 @@
       <c r="C5" s="42"/>
       <c r="D5" s="41"/>
       <c r="E5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D5,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D5,Region!$A$2:$B$11,2)),"",VLOOKUP(D5,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F5" s="41"/>
       <c r="G5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F5,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F5,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F5,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H5" s="41"/>
       <c r="I5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H5,'Base Locations'!A4:F344,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H5,'Base Locations'!A4:F344,2)),"",VLOOKUP(H5,'Base Locations'!A4:F344,2))</f>
         <v/>
       </c>
       <c r="J5" s="41"/>
@@ -8038,42 +8057,42 @@
       <c r="L5" s="41"/>
       <c r="M5" s="41"/>
       <c r="N5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M5,Services!$A$1:$B$45,2)),"",VLOOKUP(M5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O5,Services!$A$1:$B$45,2)),"",VLOOKUP(O5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q5" s="41"/>
       <c r="R5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q5,Services!$A$1:$B$45,2)),"",VLOOKUP(Q5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S5" s="41"/>
       <c r="T5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S5,Services!$A$1:$B$45,2)),"",VLOOKUP(S5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U5" s="41"/>
       <c r="V5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U5,Services!$A$1:$B$45,2)),"",VLOOKUP(U5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W5" s="41"/>
       <c r="X5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W5,Services!$A$1:$B$45,2)),"",VLOOKUP(W5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y5" s="41"/>
       <c r="Z5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y5,Services!$A$1:$B$45,2)),"",VLOOKUP(Y5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA5" s="41"/>
       <c r="AB5" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA5,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA5,Services!$A$1:$B$45,2)),"",VLOOKUP(AA5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC5" s="41"/>
@@ -8085,17 +8104,17 @@
       <c r="C6" s="42"/>
       <c r="D6" s="41"/>
       <c r="E6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D6,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D6,Region!$A$2:$B$11,2)),"",VLOOKUP(D6,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F6" s="41"/>
       <c r="G6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F6,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F6,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F6,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H6" s="41"/>
       <c r="I6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H6,'Base Locations'!A5:F345,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H6,'Base Locations'!A5:F345,2)),"",VLOOKUP(H6,'Base Locations'!A5:F345,2))</f>
         <v/>
       </c>
       <c r="J6" s="41"/>
@@ -8103,42 +8122,42 @@
       <c r="L6" s="41"/>
       <c r="M6" s="41"/>
       <c r="N6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M6,Services!$A$1:$B$45,2)),"",VLOOKUP(M6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O6" s="41"/>
       <c r="P6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O6,Services!$A$1:$B$45,2)),"",VLOOKUP(O6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q6" s="41"/>
       <c r="R6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q6,Services!$A$1:$B$45,2)),"",VLOOKUP(Q6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S6" s="41"/>
       <c r="T6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S6,Services!$A$1:$B$45,2)),"",VLOOKUP(S6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U6" s="41"/>
       <c r="V6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U6,Services!$A$1:$B$45,2)),"",VLOOKUP(U6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W6" s="41"/>
       <c r="X6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W6,Services!$A$1:$B$45,2)),"",VLOOKUP(W6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y6" s="41"/>
       <c r="Z6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y6,Services!$A$1:$B$45,2)),"",VLOOKUP(Y6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA6" s="41"/>
       <c r="AB6" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA6,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA6,Services!$A$1:$B$45,2)),"",VLOOKUP(AA6,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC6" s="41"/>
@@ -8150,17 +8169,17 @@
       <c r="C7" s="42"/>
       <c r="D7" s="41"/>
       <c r="E7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D7,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D7,Region!$A$2:$B$11,2)),"",VLOOKUP(D7,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F7" s="41"/>
       <c r="G7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F7,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F7,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F7,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H7" s="41"/>
       <c r="I7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H7,'Base Locations'!A6:F346,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H7,'Base Locations'!A6:F346,2)),"",VLOOKUP(H7,'Base Locations'!A6:F346,2))</f>
         <v/>
       </c>
       <c r="J7" s="41"/>
@@ -8168,42 +8187,42 @@
       <c r="L7" s="41"/>
       <c r="M7" s="41"/>
       <c r="N7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M7,Services!$A$1:$B$45,2)),"",VLOOKUP(M7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O7" s="41"/>
       <c r="P7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O7,Services!$A$1:$B$45,2)),"",VLOOKUP(O7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q7" s="41"/>
       <c r="R7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q7,Services!$A$1:$B$45,2)),"",VLOOKUP(Q7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S7" s="41"/>
       <c r="T7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S7,Services!$A$1:$B$45,2)),"",VLOOKUP(S7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U7" s="41"/>
       <c r="V7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U7,Services!$A$1:$B$45,2)),"",VLOOKUP(U7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W7" s="41"/>
       <c r="X7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W7,Services!$A$1:$B$45,2)),"",VLOOKUP(W7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y7" s="41"/>
       <c r="Z7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y7,Services!$A$1:$B$45,2)),"",VLOOKUP(Y7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA7" s="41"/>
       <c r="AB7" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA7,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA7,Services!$A$1:$B$45,2)),"",VLOOKUP(AA7,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC7" s="41"/>
@@ -8215,17 +8234,17 @@
       <c r="C8" s="42"/>
       <c r="D8" s="41"/>
       <c r="E8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D8,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D8,Region!$A$2:$B$11,2)),"",VLOOKUP(D8,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F8" s="41"/>
       <c r="G8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F8,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F8,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F8,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H8" s="41"/>
       <c r="I8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H8,'Base Locations'!A7:F347,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H8,'Base Locations'!A7:F347,2)),"",VLOOKUP(H8,'Base Locations'!A7:F347,2))</f>
         <v/>
       </c>
       <c r="J8" s="41"/>
@@ -8233,42 +8252,42 @@
       <c r="L8" s="41"/>
       <c r="M8" s="41"/>
       <c r="N8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M8,Services!$A$1:$B$45,2)),"",VLOOKUP(M8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O8" s="41"/>
       <c r="P8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O8,Services!$A$1:$B$45,2)),"",VLOOKUP(O8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q8" s="41"/>
       <c r="R8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q8,Services!$A$1:$B$45,2)),"",VLOOKUP(Q8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S8" s="41"/>
       <c r="T8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S8,Services!$A$1:$B$45,2)),"",VLOOKUP(S8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U8" s="41"/>
       <c r="V8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U8,Services!$A$1:$B$45,2)),"",VLOOKUP(U8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W8" s="41"/>
       <c r="X8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W8,Services!$A$1:$B$45,2)),"",VLOOKUP(W8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y8" s="41"/>
       <c r="Z8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y8,Services!$A$1:$B$45,2)),"",VLOOKUP(Y8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA8" s="41"/>
       <c r="AB8" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA8,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA8,Services!$A$1:$B$45,2)),"",VLOOKUP(AA8,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC8" s="41"/>
@@ -8280,17 +8299,17 @@
       <c r="C9" s="42"/>
       <c r="D9" s="41"/>
       <c r="E9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D9,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D9,Region!$A$2:$B$11,2)),"",VLOOKUP(D9,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F9" s="41"/>
       <c r="G9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F9,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F9,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F9,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H9" s="41"/>
       <c r="I9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H9,'Base Locations'!A8:F348,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H9,'Base Locations'!A8:F348,2)),"",VLOOKUP(H9,'Base Locations'!A8:F348,2))</f>
         <v/>
       </c>
       <c r="J9" s="41"/>
@@ -8298,42 +8317,42 @@
       <c r="L9" s="41"/>
       <c r="M9" s="41"/>
       <c r="N9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M9,Services!$A$1:$B$45,2)),"",VLOOKUP(M9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O9" s="41"/>
       <c r="P9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O9,Services!$A$1:$B$45,2)),"",VLOOKUP(O9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q9" s="41"/>
       <c r="R9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q9,Services!$A$1:$B$45,2)),"",VLOOKUP(Q9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S9" s="41"/>
       <c r="T9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S9,Services!$A$1:$B$45,2)),"",VLOOKUP(S9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U9" s="41"/>
       <c r="V9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U9,Services!$A$1:$B$45,2)),"",VLOOKUP(U9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W9" s="41"/>
       <c r="X9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W9,Services!$A$1:$B$45,2)),"",VLOOKUP(W9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y9" s="41"/>
       <c r="Z9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y9,Services!$A$1:$B$45,2)),"",VLOOKUP(Y9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA9" s="41"/>
       <c r="AB9" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA9,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA9,Services!$A$1:$B$45,2)),"",VLOOKUP(AA9,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC9" s="41"/>
@@ -8345,17 +8364,17 @@
       <c r="C10" s="42"/>
       <c r="D10" s="41"/>
       <c r="E10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D10,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D10,Region!$A$2:$B$11,2)),"",VLOOKUP(D10,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F10" s="41"/>
       <c r="G10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F10,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F10,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F10,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H10" s="41"/>
       <c r="I10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H10,'Base Locations'!A9:F349,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H10,'Base Locations'!A9:F349,2)),"",VLOOKUP(H10,'Base Locations'!A9:F349,2))</f>
         <v/>
       </c>
       <c r="J10" s="41"/>
@@ -8363,42 +8382,42 @@
       <c r="L10" s="41"/>
       <c r="M10" s="41"/>
       <c r="N10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M10,Services!$A$1:$B$45,2)),"",VLOOKUP(M10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O10" s="41"/>
       <c r="P10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O10,Services!$A$1:$B$45,2)),"",VLOOKUP(O10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q10" s="41"/>
       <c r="R10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q10,Services!$A$1:$B$45,2)),"",VLOOKUP(Q10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S10" s="41"/>
       <c r="T10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S10,Services!$A$1:$B$45,2)),"",VLOOKUP(S10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U10" s="41"/>
       <c r="V10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U10,Services!$A$1:$B$45,2)),"",VLOOKUP(U10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W10" s="41"/>
       <c r="X10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W10,Services!$A$1:$B$45,2)),"",VLOOKUP(W10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y10" s="41"/>
       <c r="Z10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y10,Services!$A$1:$B$45,2)),"",VLOOKUP(Y10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA10" s="41"/>
       <c r="AB10" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA10,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA10,Services!$A$1:$B$45,2)),"",VLOOKUP(AA10,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC10" s="41"/>
@@ -8410,17 +8429,17 @@
       <c r="C11" s="42"/>
       <c r="D11" s="41"/>
       <c r="E11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D11,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D11,Region!$A$2:$B$11,2)),"",VLOOKUP(D11,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F11" s="41"/>
       <c r="G11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F11,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F11,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F11,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H11" s="41"/>
       <c r="I11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H11,'Base Locations'!A10:F350,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H11,'Base Locations'!A10:F350,2)),"",VLOOKUP(H11,'Base Locations'!A10:F350,2))</f>
         <v/>
       </c>
       <c r="J11" s="41"/>
@@ -8428,42 +8447,42 @@
       <c r="L11" s="41"/>
       <c r="M11" s="41"/>
       <c r="N11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M11,Services!$A$1:$B$45,2)),"",VLOOKUP(M11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O11" s="41"/>
       <c r="P11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O11,Services!$A$1:$B$45,2)),"",VLOOKUP(O11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q11" s="41"/>
       <c r="R11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q11,Services!$A$1:$B$45,2)),"",VLOOKUP(Q11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S11" s="41"/>
       <c r="T11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S11,Services!$A$1:$B$45,2)),"",VLOOKUP(S11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U11" s="41"/>
       <c r="V11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U11,Services!$A$1:$B$45,2)),"",VLOOKUP(U11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W11" s="41"/>
       <c r="X11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W11,Services!$A$1:$B$45,2)),"",VLOOKUP(W11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y11" s="41"/>
       <c r="Z11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y11,Services!$A$1:$B$45,2)),"",VLOOKUP(Y11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA11" s="41"/>
       <c r="AB11" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA11,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA11,Services!$A$1:$B$45,2)),"",VLOOKUP(AA11,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC11" s="41"/>
@@ -8475,17 +8494,17 @@
       <c r="C12" s="42"/>
       <c r="D12" s="41"/>
       <c r="E12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D12,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D12,Region!$A$2:$B$11,2)),"",VLOOKUP(D12,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F12" s="41"/>
       <c r="G12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F12,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F12,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F12,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H12" s="41"/>
       <c r="I12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H12,'Base Locations'!A11:F351,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H12,'Base Locations'!A11:F351,2)),"",VLOOKUP(H12,'Base Locations'!A11:F351,2))</f>
         <v/>
       </c>
       <c r="J12" s="41"/>
@@ -8493,42 +8512,42 @@
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
       <c r="N12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M12,Services!$A$1:$B$45,2)),"",VLOOKUP(M12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O12" s="41"/>
       <c r="P12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O12,Services!$A$1:$B$45,2)),"",VLOOKUP(O12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q12" s="41"/>
       <c r="R12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q12,Services!$A$1:$B$45,2)),"",VLOOKUP(Q12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S12" s="41"/>
       <c r="T12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S12,Services!$A$1:$B$45,2)),"",VLOOKUP(S12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U12" s="41"/>
       <c r="V12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U12,Services!$A$1:$B$45,2)),"",VLOOKUP(U12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W12" s="41"/>
       <c r="X12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W12,Services!$A$1:$B$45,2)),"",VLOOKUP(W12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y12" s="41"/>
       <c r="Z12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y12,Services!$A$1:$B$45,2)),"",VLOOKUP(Y12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA12" s="41"/>
       <c r="AB12" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA12,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA12,Services!$A$1:$B$45,2)),"",VLOOKUP(AA12,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC12" s="41"/>
@@ -8540,17 +8559,17 @@
       <c r="C13" s="42"/>
       <c r="D13" s="41"/>
       <c r="E13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D13,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D13,Region!$A$2:$B$11,2)),"",VLOOKUP(D13,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F13" s="41"/>
       <c r="G13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F13,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F13,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F13,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H13" s="41"/>
       <c r="I13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H13,'Base Locations'!A12:F352,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H13,'Base Locations'!A12:F352,2)),"",VLOOKUP(H13,'Base Locations'!A12:F352,2))</f>
         <v/>
       </c>
       <c r="J13" s="41"/>
@@ -8558,42 +8577,42 @@
       <c r="L13" s="41"/>
       <c r="M13" s="41"/>
       <c r="N13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M13,Services!$A$1:$B$45,2)),"",VLOOKUP(M13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O13" s="41"/>
       <c r="P13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O13,Services!$A$1:$B$45,2)),"",VLOOKUP(O13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q13" s="41"/>
       <c r="R13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q13,Services!$A$1:$B$45,2)),"",VLOOKUP(Q13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S13" s="41"/>
       <c r="T13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S13,Services!$A$1:$B$45,2)),"",VLOOKUP(S13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U13" s="41"/>
       <c r="V13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U13,Services!$A$1:$B$45,2)),"",VLOOKUP(U13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W13" s="41"/>
       <c r="X13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W13,Services!$A$1:$B$45,2)),"",VLOOKUP(W13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y13" s="41"/>
       <c r="Z13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y13,Services!$A$1:$B$45,2)),"",VLOOKUP(Y13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA13" s="41"/>
       <c r="AB13" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA13,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA13,Services!$A$1:$B$45,2)),"",VLOOKUP(AA13,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC13" s="41"/>
@@ -8605,17 +8624,17 @@
       <c r="C14" s="42"/>
       <c r="D14" s="41"/>
       <c r="E14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D14,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D14,Region!$A$2:$B$11,2)),"",VLOOKUP(D14,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F14" s="41"/>
       <c r="G14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F14,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F14,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F14,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H14" s="41"/>
       <c r="I14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H14,'Base Locations'!A13:F353,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H14,'Base Locations'!A13:F353,2)),"",VLOOKUP(H14,'Base Locations'!A13:F353,2))</f>
         <v/>
       </c>
       <c r="J14" s="41"/>
@@ -8623,42 +8642,42 @@
       <c r="L14" s="41"/>
       <c r="M14" s="41"/>
       <c r="N14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M14,Services!$A$1:$B$45,2)),"",VLOOKUP(M14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O14" s="41"/>
       <c r="P14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O14,Services!$A$1:$B$45,2)),"",VLOOKUP(O14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q14" s="41"/>
       <c r="R14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q14,Services!$A$1:$B$45,2)),"",VLOOKUP(Q14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S14" s="41"/>
       <c r="T14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S14,Services!$A$1:$B$45,2)),"",VLOOKUP(S14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U14" s="41"/>
       <c r="V14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U14,Services!$A$1:$B$45,2)),"",VLOOKUP(U14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W14" s="41"/>
       <c r="X14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W14,Services!$A$1:$B$45,2)),"",VLOOKUP(W14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y14" s="41"/>
       <c r="Z14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y14,Services!$A$1:$B$45,2)),"",VLOOKUP(Y14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA14" s="41"/>
       <c r="AB14" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA14,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA14,Services!$A$1:$B$45,2)),"",VLOOKUP(AA14,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC14" s="41"/>
@@ -8670,17 +8689,17 @@
       <c r="C15" s="42"/>
       <c r="D15" s="41"/>
       <c r="E15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D15,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D15,Region!$A$2:$B$11,2)),"",VLOOKUP(D15,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F15" s="41"/>
       <c r="G15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F15,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F15,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F15,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H15" s="41"/>
       <c r="I15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H15,'Base Locations'!A14:F354,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H15,'Base Locations'!A14:F354,2)),"",VLOOKUP(H15,'Base Locations'!A14:F354,2))</f>
         <v/>
       </c>
       <c r="J15" s="41"/>
@@ -8688,42 +8707,42 @@
       <c r="L15" s="41"/>
       <c r="M15" s="41"/>
       <c r="N15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M15,Services!$A$1:$B$45,2)),"",VLOOKUP(M15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O15" s="41"/>
       <c r="P15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O15,Services!$A$1:$B$45,2)),"",VLOOKUP(O15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q15" s="41"/>
       <c r="R15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q15,Services!$A$1:$B$45,2)),"",VLOOKUP(Q15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S15" s="41"/>
       <c r="T15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S15,Services!$A$1:$B$45,2)),"",VLOOKUP(S15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U15" s="41"/>
       <c r="V15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U15,Services!$A$1:$B$45,2)),"",VLOOKUP(U15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W15" s="41"/>
       <c r="X15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W15,Services!$A$1:$B$45,2)),"",VLOOKUP(W15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y15" s="41"/>
       <c r="Z15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y15,Services!$A$1:$B$45,2)),"",VLOOKUP(Y15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA15" s="41"/>
       <c r="AB15" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA15,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA15,Services!$A$1:$B$45,2)),"",VLOOKUP(AA15,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC15" s="41"/>
@@ -8735,17 +8754,17 @@
       <c r="C16" s="42"/>
       <c r="D16" s="41"/>
       <c r="E16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D16,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D16,Region!$A$2:$B$11,2)),"",VLOOKUP(D16,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F16" s="41"/>
       <c r="G16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F16,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F16,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F16,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H16" s="41"/>
       <c r="I16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H16,'Base Locations'!A15:F355,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H16,'Base Locations'!A15:F355,2)),"",VLOOKUP(H16,'Base Locations'!A15:F355,2))</f>
         <v/>
       </c>
       <c r="J16" s="41"/>
@@ -8753,42 +8772,42 @@
       <c r="L16" s="41"/>
       <c r="M16" s="41"/>
       <c r="N16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M16,Services!$A$1:$B$45,2)),"",VLOOKUP(M16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O16" s="41"/>
       <c r="P16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O16,Services!$A$1:$B$45,2)),"",VLOOKUP(O16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q16" s="41"/>
       <c r="R16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q16,Services!$A$1:$B$45,2)),"",VLOOKUP(Q16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S16" s="41"/>
       <c r="T16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S16,Services!$A$1:$B$45,2)),"",VLOOKUP(S16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U16" s="41"/>
       <c r="V16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U16,Services!$A$1:$B$45,2)),"",VLOOKUP(U16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W16" s="41"/>
       <c r="X16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W16,Services!$A$1:$B$45,2)),"",VLOOKUP(W16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y16" s="41"/>
       <c r="Z16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y16,Services!$A$1:$B$45,2)),"",VLOOKUP(Y16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA16" s="41"/>
       <c r="AB16" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA16,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA16,Services!$A$1:$B$45,2)),"",VLOOKUP(AA16,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC16" s="41"/>
@@ -8800,17 +8819,17 @@
       <c r="C17" s="42"/>
       <c r="D17" s="41"/>
       <c r="E17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D17,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D17,Region!$A$2:$B$11,2)),"",VLOOKUP(D17,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F17" s="41"/>
       <c r="G17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F17,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F17,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F17,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H17" s="41"/>
       <c r="I17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H17,'Base Locations'!A16:F356,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H17,'Base Locations'!A16:F356,2)),"",VLOOKUP(H17,'Base Locations'!A16:F356,2))</f>
         <v/>
       </c>
       <c r="J17" s="41"/>
@@ -8818,42 +8837,42 @@
       <c r="L17" s="41"/>
       <c r="M17" s="41"/>
       <c r="N17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M17,Services!$A$1:$B$45,2)),"",VLOOKUP(M17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O17" s="41"/>
       <c r="P17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O17,Services!$A$1:$B$45,2)),"",VLOOKUP(O17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q17" s="41"/>
       <c r="R17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q17,Services!$A$1:$B$45,2)),"",VLOOKUP(Q17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S17" s="41"/>
       <c r="T17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S17,Services!$A$1:$B$45,2)),"",VLOOKUP(S17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U17" s="41"/>
       <c r="V17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U17,Services!$A$1:$B$45,2)),"",VLOOKUP(U17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W17" s="41"/>
       <c r="X17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W17,Services!$A$1:$B$45,2)),"",VLOOKUP(W17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y17" s="41"/>
       <c r="Z17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y17,Services!$A$1:$B$45,2)),"",VLOOKUP(Y17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA17" s="41"/>
       <c r="AB17" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA17,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA17,Services!$A$1:$B$45,2)),"",VLOOKUP(AA17,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC17" s="41"/>
@@ -8865,17 +8884,17 @@
       <c r="C18" s="42"/>
       <c r="D18" s="41"/>
       <c r="E18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D18,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D18,Region!$A$2:$B$11,2)),"",VLOOKUP(D18,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F18" s="41"/>
       <c r="G18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F18,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F18,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F18,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H18" s="41"/>
       <c r="I18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H18,'Base Locations'!A17:F357,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H18,'Base Locations'!A17:F357,2)),"",VLOOKUP(H18,'Base Locations'!A17:F357,2))</f>
         <v/>
       </c>
       <c r="J18" s="41"/>
@@ -8883,42 +8902,42 @@
       <c r="L18" s="41"/>
       <c r="M18" s="41"/>
       <c r="N18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M18,Services!$A$1:$B$45,2)),"",VLOOKUP(M18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O18" s="41"/>
       <c r="P18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O18,Services!$A$1:$B$45,2)),"",VLOOKUP(O18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q18" s="41"/>
       <c r="R18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q18,Services!$A$1:$B$45,2)),"",VLOOKUP(Q18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S18" s="41"/>
       <c r="T18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S18,Services!$A$1:$B$45,2)),"",VLOOKUP(S18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U18" s="41"/>
       <c r="V18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U18,Services!$A$1:$B$45,2)),"",VLOOKUP(U18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W18" s="41"/>
       <c r="X18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W18,Services!$A$1:$B$45,2)),"",VLOOKUP(W18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y18" s="41"/>
       <c r="Z18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y18,Services!$A$1:$B$45,2)),"",VLOOKUP(Y18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA18" s="41"/>
       <c r="AB18" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA18,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA18,Services!$A$1:$B$45,2)),"",VLOOKUP(AA18,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC18" s="41"/>
@@ -8930,17 +8949,17 @@
       <c r="C19" s="42"/>
       <c r="D19" s="41"/>
       <c r="E19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D19,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D19,Region!$A$2:$B$11,2)),"",VLOOKUP(D19,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F19" s="41"/>
       <c r="G19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F19,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F19,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F19,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H19" s="41"/>
       <c r="I19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H19,'Base Locations'!A18:F358,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H19,'Base Locations'!A18:F358,2)),"",VLOOKUP(H19,'Base Locations'!A18:F358,2))</f>
         <v/>
       </c>
       <c r="J19" s="41"/>
@@ -8948,42 +8967,42 @@
       <c r="L19" s="41"/>
       <c r="M19" s="41"/>
       <c r="N19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M19,Services!$A$1:$B$45,2)),"",VLOOKUP(M19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O19" s="41"/>
       <c r="P19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O19,Services!$A$1:$B$45,2)),"",VLOOKUP(O19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q19" s="41"/>
       <c r="R19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q19,Services!$A$1:$B$45,2)),"",VLOOKUP(Q19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S19" s="41"/>
       <c r="T19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S19,Services!$A$1:$B$45,2)),"",VLOOKUP(S19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U19" s="41"/>
       <c r="V19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U19,Services!$A$1:$B$45,2)),"",VLOOKUP(U19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W19" s="41"/>
       <c r="X19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W19,Services!$A$1:$B$45,2)),"",VLOOKUP(W19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y19" s="41"/>
       <c r="Z19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y19,Services!$A$1:$B$45,2)),"",VLOOKUP(Y19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA19" s="41"/>
       <c r="AB19" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA19,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA19,Services!$A$1:$B$45,2)),"",VLOOKUP(AA19,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC19" s="41"/>
@@ -8995,17 +9014,17 @@
       <c r="C20" s="42"/>
       <c r="D20" s="41"/>
       <c r="E20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D20,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D20,Region!$A$2:$B$11,2)),"",VLOOKUP(D20,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F20" s="41"/>
       <c r="G20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F20,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F20,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F20,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H20" s="41"/>
       <c r="I20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H20,'Base Locations'!A19:F359,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H20,'Base Locations'!A19:F359,2)),"",VLOOKUP(H20,'Base Locations'!A19:F359,2))</f>
         <v/>
       </c>
       <c r="J20" s="41"/>
@@ -9013,42 +9032,42 @@
       <c r="L20" s="41"/>
       <c r="M20" s="41"/>
       <c r="N20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M20,Services!$A$1:$B$45,2)),"",VLOOKUP(M20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O20" s="41"/>
       <c r="P20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O20,Services!$A$1:$B$45,2)),"",VLOOKUP(O20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q20" s="41"/>
       <c r="R20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q20,Services!$A$1:$B$45,2)),"",VLOOKUP(Q20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S20" s="41"/>
       <c r="T20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S20,Services!$A$1:$B$45,2)),"",VLOOKUP(S20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U20" s="41"/>
       <c r="V20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U20,Services!$A$1:$B$45,2)),"",VLOOKUP(U20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W20" s="41"/>
       <c r="X20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W20,Services!$A$1:$B$45,2)),"",VLOOKUP(W20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y20" s="41"/>
       <c r="Z20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y20,Services!$A$1:$B$45,2)),"",VLOOKUP(Y20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA20" s="41"/>
       <c r="AB20" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA20,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA20,Services!$A$1:$B$45,2)),"",VLOOKUP(AA20,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC20" s="41"/>
@@ -9060,17 +9079,17 @@
       <c r="C21" s="42"/>
       <c r="D21" s="41"/>
       <c r="E21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D21,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D21,Region!$A$2:$B$11,2)),"",VLOOKUP(D21,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F21" s="41"/>
       <c r="G21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F21,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F21,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F21,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H21" s="41"/>
       <c r="I21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H21,'Base Locations'!A20:F360,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H21,'Base Locations'!A20:F360,2)),"",VLOOKUP(H21,'Base Locations'!A20:F360,2))</f>
         <v/>
       </c>
       <c r="J21" s="41"/>
@@ -9078,42 +9097,42 @@
       <c r="L21" s="41"/>
       <c r="M21" s="41"/>
       <c r="N21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M21,Services!$A$1:$B$45,2)),"",VLOOKUP(M21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O21" s="41"/>
       <c r="P21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O21,Services!$A$1:$B$45,2)),"",VLOOKUP(O21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q21" s="41"/>
       <c r="R21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q21,Services!$A$1:$B$45,2)),"",VLOOKUP(Q21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S21" s="41"/>
       <c r="T21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S21,Services!$A$1:$B$45,2)),"",VLOOKUP(S21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U21" s="41"/>
       <c r="V21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U21,Services!$A$1:$B$45,2)),"",VLOOKUP(U21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W21" s="41"/>
       <c r="X21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W21,Services!$A$1:$B$45,2)),"",VLOOKUP(W21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y21" s="41"/>
       <c r="Z21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y21,Services!$A$1:$B$45,2)),"",VLOOKUP(Y21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA21" s="41"/>
       <c r="AB21" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA21,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA21,Services!$A$1:$B$45,2)),"",VLOOKUP(AA21,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC21" s="41"/>
@@ -9125,17 +9144,17 @@
       <c r="C22" s="42"/>
       <c r="D22" s="41"/>
       <c r="E22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D22,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D22,Region!$A$2:$B$11,2)),"",VLOOKUP(D22,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F22" s="41"/>
       <c r="G22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F22,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F22,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F22,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H22" s="41"/>
       <c r="I22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H22,'Base Locations'!A21:F361,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H22,'Base Locations'!A21:F361,2)),"",VLOOKUP(H22,'Base Locations'!A21:F361,2))</f>
         <v/>
       </c>
       <c r="J22" s="41"/>
@@ -9143,42 +9162,42 @@
       <c r="L22" s="41"/>
       <c r="M22" s="41"/>
       <c r="N22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M22,Services!$A$1:$B$45,2)),"",VLOOKUP(M22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O22" s="41"/>
       <c r="P22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O22,Services!$A$1:$B$45,2)),"",VLOOKUP(O22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q22" s="41"/>
       <c r="R22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q22,Services!$A$1:$B$45,2)),"",VLOOKUP(Q22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S22" s="41"/>
       <c r="T22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S22,Services!$A$1:$B$45,2)),"",VLOOKUP(S22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U22" s="41"/>
       <c r="V22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U22,Services!$A$1:$B$45,2)),"",VLOOKUP(U22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W22" s="41"/>
       <c r="X22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W22,Services!$A$1:$B$45,2)),"",VLOOKUP(W22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y22" s="41"/>
       <c r="Z22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y22,Services!$A$1:$B$45,2)),"",VLOOKUP(Y22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA22" s="41"/>
       <c r="AB22" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA22,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA22,Services!$A$1:$B$45,2)),"",VLOOKUP(AA22,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC22" s="41"/>
@@ -9190,17 +9209,17 @@
       <c r="C23" s="42"/>
       <c r="D23" s="41"/>
       <c r="E23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D23,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D23,Region!$A$2:$B$11,2)),"",VLOOKUP(D23,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F23" s="41"/>
       <c r="G23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F23,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F23,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F23,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H23" s="41"/>
       <c r="I23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H23,'Base Locations'!A22:F362,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H23,'Base Locations'!A22:F362,2)),"",VLOOKUP(H23,'Base Locations'!A22:F362,2))</f>
         <v/>
       </c>
       <c r="J23" s="41"/>
@@ -9208,42 +9227,42 @@
       <c r="L23" s="41"/>
       <c r="M23" s="41"/>
       <c r="N23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M23,Services!$A$1:$B$45,2)),"",VLOOKUP(M23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O23" s="41"/>
       <c r="P23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O23,Services!$A$1:$B$45,2)),"",VLOOKUP(O23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q23" s="41"/>
       <c r="R23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q23,Services!$A$1:$B$45,2)),"",VLOOKUP(Q23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S23" s="41"/>
       <c r="T23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S23,Services!$A$1:$B$45,2)),"",VLOOKUP(S23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U23" s="41"/>
       <c r="V23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U23,Services!$A$1:$B$45,2)),"",VLOOKUP(U23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W23" s="41"/>
       <c r="X23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W23,Services!$A$1:$B$45,2)),"",VLOOKUP(W23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y23" s="41"/>
       <c r="Z23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y23,Services!$A$1:$B$45,2)),"",VLOOKUP(Y23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA23" s="41"/>
       <c r="AB23" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA23,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA23,Services!$A$1:$B$45,2)),"",VLOOKUP(AA23,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC23" s="41"/>
@@ -9255,17 +9274,17 @@
       <c r="C24" s="42"/>
       <c r="D24" s="41"/>
       <c r="E24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D24,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D24,Region!$A$2:$B$11,2)),"",VLOOKUP(D24,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F24" s="41"/>
       <c r="G24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F24,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F24,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F24,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H24" s="41"/>
       <c r="I24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H24,'Base Locations'!A23:F363,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H24,'Base Locations'!A23:F363,2)),"",VLOOKUP(H24,'Base Locations'!A23:F363,2))</f>
         <v/>
       </c>
       <c r="J24" s="41"/>
@@ -9273,42 +9292,42 @@
       <c r="L24" s="41"/>
       <c r="M24" s="41"/>
       <c r="N24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M24,Services!$A$1:$B$45,2)),"",VLOOKUP(M24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O24" s="41"/>
       <c r="P24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O24,Services!$A$1:$B$45,2)),"",VLOOKUP(O24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q24" s="41"/>
       <c r="R24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q24,Services!$A$1:$B$45,2)),"",VLOOKUP(Q24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S24" s="41"/>
       <c r="T24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S24,Services!$A$1:$B$45,2)),"",VLOOKUP(S24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U24" s="41"/>
       <c r="V24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U24,Services!$A$1:$B$45,2)),"",VLOOKUP(U24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W24" s="41"/>
       <c r="X24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W24,Services!$A$1:$B$45,2)),"",VLOOKUP(W24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y24" s="41"/>
       <c r="Z24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y24,Services!$A$1:$B$45,2)),"",VLOOKUP(Y24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA24" s="41"/>
       <c r="AB24" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA24,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA24,Services!$A$1:$B$45,2)),"",VLOOKUP(AA24,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC24" s="41"/>
@@ -9320,17 +9339,17 @@
       <c r="C25" s="42"/>
       <c r="D25" s="41"/>
       <c r="E25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D25,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D25,Region!$A$2:$B$11,2)),"",VLOOKUP(D25,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F25" s="41"/>
       <c r="G25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F25,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F25,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F25,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H25" s="41"/>
       <c r="I25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H25,'Base Locations'!A24:F364,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H25,'Base Locations'!A24:F364,2)),"",VLOOKUP(H25,'Base Locations'!A24:F364,2))</f>
         <v/>
       </c>
       <c r="J25" s="41"/>
@@ -9338,42 +9357,42 @@
       <c r="L25" s="41"/>
       <c r="M25" s="41"/>
       <c r="N25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M25,Services!$A$1:$B$45,2)),"",VLOOKUP(M25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O25" s="41"/>
       <c r="P25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O25,Services!$A$1:$B$45,2)),"",VLOOKUP(O25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q25" s="41"/>
       <c r="R25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q25,Services!$A$1:$B$45,2)),"",VLOOKUP(Q25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S25" s="41"/>
       <c r="T25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S25,Services!$A$1:$B$45,2)),"",VLOOKUP(S25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U25" s="41"/>
       <c r="V25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U25,Services!$A$1:$B$45,2)),"",VLOOKUP(U25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W25" s="41"/>
       <c r="X25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W25,Services!$A$1:$B$45,2)),"",VLOOKUP(W25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y25" s="41"/>
       <c r="Z25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y25,Services!$A$1:$B$45,2)),"",VLOOKUP(Y25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA25" s="41"/>
       <c r="AB25" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA25,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA25,Services!$A$1:$B$45,2)),"",VLOOKUP(AA25,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC25" s="41"/>
@@ -9385,17 +9404,17 @@
       <c r="C26" s="42"/>
       <c r="D26" s="41"/>
       <c r="E26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D26,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D26,Region!$A$2:$B$11,2)),"",VLOOKUP(D26,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F26" s="41"/>
       <c r="G26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F26,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F26,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F26,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H26" s="41"/>
       <c r="I26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H26,'Base Locations'!A25:F365,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H26,'Base Locations'!A25:F365,2)),"",VLOOKUP(H26,'Base Locations'!A25:F365,2))</f>
         <v/>
       </c>
       <c r="J26" s="41"/>
@@ -9403,42 +9422,42 @@
       <c r="L26" s="41"/>
       <c r="M26" s="41"/>
       <c r="N26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M26,Services!$A$1:$B$45,2)),"",VLOOKUP(M26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O26" s="41"/>
       <c r="P26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O26,Services!$A$1:$B$45,2)),"",VLOOKUP(O26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q26" s="41"/>
       <c r="R26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q26,Services!$A$1:$B$45,2)),"",VLOOKUP(Q26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S26" s="41"/>
       <c r="T26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S26,Services!$A$1:$B$45,2)),"",VLOOKUP(S26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U26" s="41"/>
       <c r="V26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U26,Services!$A$1:$B$45,2)),"",VLOOKUP(U26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W26" s="41"/>
       <c r="X26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W26,Services!$A$1:$B$45,2)),"",VLOOKUP(W26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y26" s="41"/>
       <c r="Z26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y26,Services!$A$1:$B$45,2)),"",VLOOKUP(Y26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA26" s="41"/>
       <c r="AB26" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA26,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA26,Services!$A$1:$B$45,2)),"",VLOOKUP(AA26,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC26" s="41"/>
@@ -9450,17 +9469,17 @@
       <c r="C27" s="42"/>
       <c r="D27" s="41"/>
       <c r="E27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D27,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D27,Region!$A$2:$B$11,2)),"",VLOOKUP(D27,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F27" s="41"/>
       <c r="G27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F27,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F27,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F27,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H27" s="41"/>
       <c r="I27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H27,'Base Locations'!A26:F366,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H27,'Base Locations'!A26:F366,2)),"",VLOOKUP(H27,'Base Locations'!A26:F366,2))</f>
         <v/>
       </c>
       <c r="J27" s="41"/>
@@ -9468,42 +9487,42 @@
       <c r="L27" s="41"/>
       <c r="M27" s="41"/>
       <c r="N27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M27,Services!$A$1:$B$45,2)),"",VLOOKUP(M27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O27" s="41"/>
       <c r="P27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O27,Services!$A$1:$B$45,2)),"",VLOOKUP(O27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q27" s="41"/>
       <c r="R27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q27,Services!$A$1:$B$45,2)),"",VLOOKUP(Q27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S27" s="41"/>
       <c r="T27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S27,Services!$A$1:$B$45,2)),"",VLOOKUP(S27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U27" s="41"/>
       <c r="V27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U27,Services!$A$1:$B$45,2)),"",VLOOKUP(U27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W27" s="41"/>
       <c r="X27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W27,Services!$A$1:$B$45,2)),"",VLOOKUP(W27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y27" s="41"/>
       <c r="Z27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y27,Services!$A$1:$B$45,2)),"",VLOOKUP(Y27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA27" s="41"/>
       <c r="AB27" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA27,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA27,Services!$A$1:$B$45,2)),"",VLOOKUP(AA27,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC27" s="41"/>
@@ -9515,17 +9534,17 @@
       <c r="C28" s="42"/>
       <c r="D28" s="41"/>
       <c r="E28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D28,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D28,Region!$A$2:$B$11,2)),"",VLOOKUP(D28,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F28" s="41"/>
       <c r="G28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F28,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F28,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F28,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H28" s="41"/>
       <c r="I28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H28,'Base Locations'!A27:F367,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H28,'Base Locations'!A27:F367,2)),"",VLOOKUP(H28,'Base Locations'!A27:F367,2))</f>
         <v/>
       </c>
       <c r="J28" s="41"/>
@@ -9533,42 +9552,42 @@
       <c r="L28" s="41"/>
       <c r="M28" s="41"/>
       <c r="N28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M28,Services!$A$1:$B$45,2)),"",VLOOKUP(M28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O28" s="41"/>
       <c r="P28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O28,Services!$A$1:$B$45,2)),"",VLOOKUP(O28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q28" s="41"/>
       <c r="R28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q28,Services!$A$1:$B$45,2)),"",VLOOKUP(Q28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S28" s="41"/>
       <c r="T28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S28,Services!$A$1:$B$45,2)),"",VLOOKUP(S28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U28" s="41"/>
       <c r="V28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U28,Services!$A$1:$B$45,2)),"",VLOOKUP(U28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W28" s="41"/>
       <c r="X28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W28,Services!$A$1:$B$45,2)),"",VLOOKUP(W28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y28" s="41"/>
       <c r="Z28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y28,Services!$A$1:$B$45,2)),"",VLOOKUP(Y28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA28" s="41"/>
       <c r="AB28" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA28,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA28,Services!$A$1:$B$45,2)),"",VLOOKUP(AA28,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC28" s="41"/>
@@ -9580,17 +9599,17 @@
       <c r="C29" s="42"/>
       <c r="D29" s="41"/>
       <c r="E29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D29,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D29,Region!$A$2:$B$11,2)),"",VLOOKUP(D29,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F29" s="41"/>
       <c r="G29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F29,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F29,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F29,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H29" s="41"/>
       <c r="I29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H29,'Base Locations'!A28:F368,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H29,'Base Locations'!A28:F368,2)),"",VLOOKUP(H29,'Base Locations'!A28:F368,2))</f>
         <v/>
       </c>
       <c r="J29" s="41"/>
@@ -9598,42 +9617,42 @@
       <c r="L29" s="41"/>
       <c r="M29" s="41"/>
       <c r="N29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M29,Services!$A$1:$B$45,2)),"",VLOOKUP(M29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O29" s="41"/>
       <c r="P29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O29,Services!$A$1:$B$45,2)),"",VLOOKUP(O29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q29" s="41"/>
       <c r="R29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q29,Services!$A$1:$B$45,2)),"",VLOOKUP(Q29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S29" s="41"/>
       <c r="T29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S29,Services!$A$1:$B$45,2)),"",VLOOKUP(S29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U29" s="41"/>
       <c r="V29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U29,Services!$A$1:$B$45,2)),"",VLOOKUP(U29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W29" s="41"/>
       <c r="X29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W29,Services!$A$1:$B$45,2)),"",VLOOKUP(W29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y29" s="41"/>
       <c r="Z29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y29,Services!$A$1:$B$45,2)),"",VLOOKUP(Y29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA29" s="41"/>
       <c r="AB29" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA29,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA29,Services!$A$1:$B$45,2)),"",VLOOKUP(AA29,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC29" s="41"/>
@@ -9645,17 +9664,17 @@
       <c r="C30" s="42"/>
       <c r="D30" s="41"/>
       <c r="E30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D30,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D30,Region!$A$2:$B$11,2)),"",VLOOKUP(D30,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F30" s="41"/>
       <c r="G30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F30,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F30,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F30,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H30" s="41"/>
       <c r="I30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H30,'Base Locations'!A29:F369,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H30,'Base Locations'!A29:F369,2)),"",VLOOKUP(H30,'Base Locations'!A29:F369,2))</f>
         <v/>
       </c>
       <c r="J30" s="41"/>
@@ -9663,42 +9682,42 @@
       <c r="L30" s="41"/>
       <c r="M30" s="41"/>
       <c r="N30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M30,Services!$A$1:$B$45,2)),"",VLOOKUP(M30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O30" s="41"/>
       <c r="P30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O30,Services!$A$1:$B$45,2)),"",VLOOKUP(O30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q30" s="41"/>
       <c r="R30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q30,Services!$A$1:$B$45,2)),"",VLOOKUP(Q30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S30" s="41"/>
       <c r="T30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S30,Services!$A$1:$B$45,2)),"",VLOOKUP(S30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U30" s="41"/>
       <c r="V30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U30,Services!$A$1:$B$45,2)),"",VLOOKUP(U30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W30" s="41"/>
       <c r="X30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W30,Services!$A$1:$B$45,2)),"",VLOOKUP(W30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y30" s="41"/>
       <c r="Z30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y30,Services!$A$1:$B$45,2)),"",VLOOKUP(Y30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA30" s="41"/>
       <c r="AB30" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA30,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA30,Services!$A$1:$B$45,2)),"",VLOOKUP(AA30,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC30" s="41"/>
@@ -9710,17 +9729,17 @@
       <c r="C31" s="42"/>
       <c r="D31" s="41"/>
       <c r="E31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D31,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D31,Region!$A$2:$B$11,2)),"",VLOOKUP(D31,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F31" s="41"/>
       <c r="G31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F31,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F31,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F31,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H31" s="41"/>
       <c r="I31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H31,'Base Locations'!A30:F370,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H31,'Base Locations'!A30:F370,2)),"",VLOOKUP(H31,'Base Locations'!A30:F370,2))</f>
         <v/>
       </c>
       <c r="J31" s="41"/>
@@ -9728,42 +9747,42 @@
       <c r="L31" s="41"/>
       <c r="M31" s="41"/>
       <c r="N31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M31,Services!$A$1:$B$45,2)),"",VLOOKUP(M31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O31" s="41"/>
       <c r="P31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O31,Services!$A$1:$B$45,2)),"",VLOOKUP(O31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q31" s="41"/>
       <c r="R31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q31,Services!$A$1:$B$45,2)),"",VLOOKUP(Q31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S31" s="41"/>
       <c r="T31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S31,Services!$A$1:$B$45,2)),"",VLOOKUP(S31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U31" s="41"/>
       <c r="V31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U31,Services!$A$1:$B$45,2)),"",VLOOKUP(U31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W31" s="41"/>
       <c r="X31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W31,Services!$A$1:$B$45,2)),"",VLOOKUP(W31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y31" s="41"/>
       <c r="Z31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y31,Services!$A$1:$B$45,2)),"",VLOOKUP(Y31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA31" s="41"/>
       <c r="AB31" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA31,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA31,Services!$A$1:$B$45,2)),"",VLOOKUP(AA31,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC31" s="41"/>
@@ -9775,17 +9794,17 @@
       <c r="C32" s="42"/>
       <c r="D32" s="41"/>
       <c r="E32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D32,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D32,Region!$A$2:$B$11,2)),"",VLOOKUP(D32,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F32" s="41"/>
       <c r="G32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F32,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F32,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F32,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H32" s="41"/>
       <c r="I32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H32,'Base Locations'!A31:F371,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H32,'Base Locations'!A31:F371,2)),"",VLOOKUP(H32,'Base Locations'!A31:F371,2))</f>
         <v/>
       </c>
       <c r="J32" s="41"/>
@@ -9793,42 +9812,42 @@
       <c r="L32" s="41"/>
       <c r="M32" s="41"/>
       <c r="N32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M32,Services!$A$1:$B$45,2)),"",VLOOKUP(M32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O32" s="41"/>
       <c r="P32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O32,Services!$A$1:$B$45,2)),"",VLOOKUP(O32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q32" s="41"/>
       <c r="R32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q32,Services!$A$1:$B$45,2)),"",VLOOKUP(Q32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S32" s="41"/>
       <c r="T32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S32,Services!$A$1:$B$45,2)),"",VLOOKUP(S32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U32" s="41"/>
       <c r="V32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U32,Services!$A$1:$B$45,2)),"",VLOOKUP(U32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W32" s="41"/>
       <c r="X32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W32,Services!$A$1:$B$45,2)),"",VLOOKUP(W32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y32" s="41"/>
       <c r="Z32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y32,Services!$A$1:$B$45,2)),"",VLOOKUP(Y32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA32" s="41"/>
       <c r="AB32" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA32,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA32,Services!$A$1:$B$45,2)),"",VLOOKUP(AA32,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC32" s="41"/>
@@ -9840,17 +9859,17 @@
       <c r="C33" s="42"/>
       <c r="D33" s="41"/>
       <c r="E33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D33,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D33,Region!$A$2:$B$11,2)),"",VLOOKUP(D33,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F33" s="41"/>
       <c r="G33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F33,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F33,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F33,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H33" s="41"/>
       <c r="I33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H33,'Base Locations'!A32:F372,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H33,'Base Locations'!A32:F372,2)),"",VLOOKUP(H33,'Base Locations'!A32:F372,2))</f>
         <v/>
       </c>
       <c r="J33" s="41"/>
@@ -9858,42 +9877,42 @@
       <c r="L33" s="41"/>
       <c r="M33" s="41"/>
       <c r="N33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M33,Services!$A$1:$B$45,2)),"",VLOOKUP(M33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O33" s="41"/>
       <c r="P33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O33,Services!$A$1:$B$45,2)),"",VLOOKUP(O33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q33" s="41"/>
       <c r="R33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q33,Services!$A$1:$B$45,2)),"",VLOOKUP(Q33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S33" s="41"/>
       <c r="T33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S33,Services!$A$1:$B$45,2)),"",VLOOKUP(S33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U33" s="41"/>
       <c r="V33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U33,Services!$A$1:$B$45,2)),"",VLOOKUP(U33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W33" s="41"/>
       <c r="X33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W33,Services!$A$1:$B$45,2)),"",VLOOKUP(W33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y33" s="41"/>
       <c r="Z33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y33,Services!$A$1:$B$45,2)),"",VLOOKUP(Y33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA33" s="41"/>
       <c r="AB33" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA33,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA33,Services!$A$1:$B$45,2)),"",VLOOKUP(AA33,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC33" s="41"/>
@@ -9905,17 +9924,17 @@
       <c r="C34" s="42"/>
       <c r="D34" s="41"/>
       <c r="E34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D34,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D34,Region!$A$2:$B$11,2)),"",VLOOKUP(D34,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F34" s="41"/>
       <c r="G34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F34,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F34,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F34,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H34" s="41"/>
       <c r="I34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H34,'Base Locations'!A33:F373,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H34,'Base Locations'!A33:F373,2)),"",VLOOKUP(H34,'Base Locations'!A33:F373,2))</f>
         <v/>
       </c>
       <c r="J34" s="41"/>
@@ -9923,42 +9942,42 @@
       <c r="L34" s="41"/>
       <c r="M34" s="41"/>
       <c r="N34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M34,Services!$A$1:$B$45,2)),"",VLOOKUP(M34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O34" s="41"/>
       <c r="P34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O34,Services!$A$1:$B$45,2)),"",VLOOKUP(O34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q34" s="41"/>
       <c r="R34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q34,Services!$A$1:$B$45,2)),"",VLOOKUP(Q34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S34" s="41"/>
       <c r="T34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S34,Services!$A$1:$B$45,2)),"",VLOOKUP(S34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U34" s="41"/>
       <c r="V34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U34,Services!$A$1:$B$45,2)),"",VLOOKUP(U34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W34" s="41"/>
       <c r="X34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W34,Services!$A$1:$B$45,2)),"",VLOOKUP(W34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y34" s="41"/>
       <c r="Z34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y34,Services!$A$1:$B$45,2)),"",VLOOKUP(Y34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA34" s="41"/>
       <c r="AB34" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA34,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA34,Services!$A$1:$B$45,2)),"",VLOOKUP(AA34,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC34" s="41"/>
@@ -9970,17 +9989,17 @@
       <c r="C35" s="42"/>
       <c r="D35" s="41"/>
       <c r="E35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D35,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D35,Region!$A$2:$B$11,2)),"",VLOOKUP(D35,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F35" s="41"/>
       <c r="G35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F35,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F35,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F35,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H35" s="41"/>
       <c r="I35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H35,'Base Locations'!A34:F374,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H35,'Base Locations'!A34:F374,2)),"",VLOOKUP(H35,'Base Locations'!A34:F374,2))</f>
         <v/>
       </c>
       <c r="J35" s="41"/>
@@ -9988,42 +10007,42 @@
       <c r="L35" s="41"/>
       <c r="M35" s="41"/>
       <c r="N35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M35,Services!$A$1:$B$45,2)),"",VLOOKUP(M35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O35" s="41"/>
       <c r="P35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O35,Services!$A$1:$B$45,2)),"",VLOOKUP(O35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q35" s="41"/>
       <c r="R35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q35,Services!$A$1:$B$45,2)),"",VLOOKUP(Q35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S35" s="41"/>
       <c r="T35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S35,Services!$A$1:$B$45,2)),"",VLOOKUP(S35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U35" s="41"/>
       <c r="V35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U35,Services!$A$1:$B$45,2)),"",VLOOKUP(U35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W35" s="41"/>
       <c r="X35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W35,Services!$A$1:$B$45,2)),"",VLOOKUP(W35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y35" s="41"/>
       <c r="Z35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y35,Services!$A$1:$B$45,2)),"",VLOOKUP(Y35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA35" s="41"/>
       <c r="AB35" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA35,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA35,Services!$A$1:$B$45,2)),"",VLOOKUP(AA35,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC35" s="41"/>
@@ -10035,17 +10054,17 @@
       <c r="C36" s="42"/>
       <c r="D36" s="41"/>
       <c r="E36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D36,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D36,Region!$A$2:$B$11,2)),"",VLOOKUP(D36,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F36" s="41"/>
       <c r="G36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F36,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F36,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F36,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H36" s="41"/>
       <c r="I36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H36,'Base Locations'!A35:F375,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H36,'Base Locations'!A35:F375,2)),"",VLOOKUP(H36,'Base Locations'!A35:F375,2))</f>
         <v/>
       </c>
       <c r="J36" s="41"/>
@@ -10053,42 +10072,42 @@
       <c r="L36" s="41"/>
       <c r="M36" s="41"/>
       <c r="N36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M36,Services!$A$1:$B$45,2)),"",VLOOKUP(M36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O36" s="41"/>
       <c r="P36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O36,Services!$A$1:$B$45,2)),"",VLOOKUP(O36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q36" s="41"/>
       <c r="R36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q36,Services!$A$1:$B$45,2)),"",VLOOKUP(Q36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S36" s="41"/>
       <c r="T36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S36,Services!$A$1:$B$45,2)),"",VLOOKUP(S36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U36" s="41"/>
       <c r="V36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U36,Services!$A$1:$B$45,2)),"",VLOOKUP(U36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W36" s="41"/>
       <c r="X36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W36,Services!$A$1:$B$45,2)),"",VLOOKUP(W36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y36" s="41"/>
       <c r="Z36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y36,Services!$A$1:$B$45,2)),"",VLOOKUP(Y36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA36" s="41"/>
       <c r="AB36" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA36,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA36,Services!$A$1:$B$45,2)),"",VLOOKUP(AA36,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC36" s="41"/>
@@ -10100,17 +10119,17 @@
       <c r="C37" s="42"/>
       <c r="D37" s="41"/>
       <c r="E37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D37,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D37,Region!$A$2:$B$11,2)),"",VLOOKUP(D37,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F37" s="41"/>
       <c r="G37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F37,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F37,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F37,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H37" s="41"/>
       <c r="I37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H37,'Base Locations'!A36:F376,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H37,'Base Locations'!A36:F376,2)),"",VLOOKUP(H37,'Base Locations'!A36:F376,2))</f>
         <v/>
       </c>
       <c r="J37" s="41"/>
@@ -10118,42 +10137,42 @@
       <c r="L37" s="41"/>
       <c r="M37" s="41"/>
       <c r="N37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M37,Services!$A$1:$B$45,2)),"",VLOOKUP(M37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O37" s="41"/>
       <c r="P37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O37,Services!$A$1:$B$45,2)),"",VLOOKUP(O37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q37" s="41"/>
       <c r="R37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q37,Services!$A$1:$B$45,2)),"",VLOOKUP(Q37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S37" s="41"/>
       <c r="T37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S37,Services!$A$1:$B$45,2)),"",VLOOKUP(S37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U37" s="41"/>
       <c r="V37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U37,Services!$A$1:$B$45,2)),"",VLOOKUP(U37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W37" s="41"/>
       <c r="X37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W37,Services!$A$1:$B$45,2)),"",VLOOKUP(W37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y37" s="41"/>
       <c r="Z37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y37,Services!$A$1:$B$45,2)),"",VLOOKUP(Y37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA37" s="41"/>
       <c r="AB37" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA37,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA37,Services!$A$1:$B$45,2)),"",VLOOKUP(AA37,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC37" s="41"/>
@@ -10165,17 +10184,17 @@
       <c r="C38" s="42"/>
       <c r="D38" s="41"/>
       <c r="E38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D38,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D38,Region!$A$2:$B$11,2)),"",VLOOKUP(D38,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F38" s="41"/>
       <c r="G38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F38,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F38,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F38,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H38" s="41"/>
       <c r="I38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H38,'Base Locations'!A37:F377,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H38,'Base Locations'!A37:F377,2)),"",VLOOKUP(H38,'Base Locations'!A37:F377,2))</f>
         <v/>
       </c>
       <c r="J38" s="41"/>
@@ -10183,42 +10202,42 @@
       <c r="L38" s="41"/>
       <c r="M38" s="41"/>
       <c r="N38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M38,Services!$A$1:$B$45,2)),"",VLOOKUP(M38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O38" s="41"/>
       <c r="P38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O38,Services!$A$1:$B$45,2)),"",VLOOKUP(O38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q38" s="41"/>
       <c r="R38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q38,Services!$A$1:$B$45,2)),"",VLOOKUP(Q38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S38" s="41"/>
       <c r="T38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S38,Services!$A$1:$B$45,2)),"",VLOOKUP(S38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U38" s="41"/>
       <c r="V38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U38,Services!$A$1:$B$45,2)),"",VLOOKUP(U38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W38" s="41"/>
       <c r="X38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W38,Services!$A$1:$B$45,2)),"",VLOOKUP(W38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y38" s="41"/>
       <c r="Z38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y38,Services!$A$1:$B$45,2)),"",VLOOKUP(Y38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA38" s="41"/>
       <c r="AB38" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA38,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA38,Services!$A$1:$B$45,2)),"",VLOOKUP(AA38,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC38" s="41"/>
@@ -10230,17 +10249,17 @@
       <c r="C39" s="42"/>
       <c r="D39" s="41"/>
       <c r="E39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D39,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D39,Region!$A$2:$B$11,2)),"",VLOOKUP(D39,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F39" s="41"/>
       <c r="G39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F39,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F39,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F39,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H39" s="41"/>
       <c r="I39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H39,'Base Locations'!A38:F378,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H39,'Base Locations'!A38:F378,2)),"",VLOOKUP(H39,'Base Locations'!A38:F378,2))</f>
         <v/>
       </c>
       <c r="J39" s="41"/>
@@ -10248,42 +10267,42 @@
       <c r="L39" s="41"/>
       <c r="M39" s="41"/>
       <c r="N39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M39,Services!$A$1:$B$45,2)),"",VLOOKUP(M39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O39" s="41"/>
       <c r="P39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O39,Services!$A$1:$B$45,2)),"",VLOOKUP(O39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q39" s="41"/>
       <c r="R39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q39,Services!$A$1:$B$45,2)),"",VLOOKUP(Q39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S39" s="41"/>
       <c r="T39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S39,Services!$A$1:$B$45,2)),"",VLOOKUP(S39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U39" s="41"/>
       <c r="V39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U39,Services!$A$1:$B$45,2)),"",VLOOKUP(U39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W39" s="41"/>
       <c r="X39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W39,Services!$A$1:$B$45,2)),"",VLOOKUP(W39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y39" s="41"/>
       <c r="Z39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y39,Services!$A$1:$B$45,2)),"",VLOOKUP(Y39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA39" s="41"/>
       <c r="AB39" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA39,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA39,Services!$A$1:$B$45,2)),"",VLOOKUP(AA39,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC39" s="41"/>
@@ -10295,17 +10314,17 @@
       <c r="C40" s="42"/>
       <c r="D40" s="41"/>
       <c r="E40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D40,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D40,Region!$A$2:$B$11,2)),"",VLOOKUP(D40,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F40" s="41"/>
       <c r="G40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F40,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F40,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F40,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H40" s="41"/>
       <c r="I40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H40,'Base Locations'!A39:F379,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H40,'Base Locations'!A39:F379,2)),"",VLOOKUP(H40,'Base Locations'!A39:F379,2))</f>
         <v/>
       </c>
       <c r="J40" s="41"/>
@@ -10313,42 +10332,42 @@
       <c r="L40" s="41"/>
       <c r="M40" s="41"/>
       <c r="N40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M40,Services!$A$1:$B$45,2)),"",VLOOKUP(M40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O40" s="41"/>
       <c r="P40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O40,Services!$A$1:$B$45,2)),"",VLOOKUP(O40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q40" s="41"/>
       <c r="R40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q40,Services!$A$1:$B$45,2)),"",VLOOKUP(Q40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S40" s="41"/>
       <c r="T40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S40,Services!$A$1:$B$45,2)),"",VLOOKUP(S40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U40" s="41"/>
       <c r="V40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U40,Services!$A$1:$B$45,2)),"",VLOOKUP(U40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W40" s="41"/>
       <c r="X40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W40,Services!$A$1:$B$45,2)),"",VLOOKUP(W40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y40" s="41"/>
       <c r="Z40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y40,Services!$A$1:$B$45,2)),"",VLOOKUP(Y40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA40" s="41"/>
       <c r="AB40" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA40,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA40,Services!$A$1:$B$45,2)),"",VLOOKUP(AA40,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC40" s="41"/>
@@ -10360,17 +10379,17 @@
       <c r="C41" s="42"/>
       <c r="D41" s="41"/>
       <c r="E41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D41,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D41,Region!$A$2:$B$11,2)),"",VLOOKUP(D41,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F41" s="41"/>
       <c r="G41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F41,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F41,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F41,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H41" s="41"/>
       <c r="I41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H41,'Base Locations'!A40:F380,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H41,'Base Locations'!A40:F380,2)),"",VLOOKUP(H41,'Base Locations'!A40:F380,2))</f>
         <v/>
       </c>
       <c r="J41" s="41"/>
@@ -10378,42 +10397,42 @@
       <c r="L41" s="41"/>
       <c r="M41" s="41"/>
       <c r="N41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M41,Services!$A$1:$B$45,2)),"",VLOOKUP(M41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O41" s="41"/>
       <c r="P41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O41,Services!$A$1:$B$45,2)),"",VLOOKUP(O41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q41" s="41"/>
       <c r="R41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q41,Services!$A$1:$B$45,2)),"",VLOOKUP(Q41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S41" s="41"/>
       <c r="T41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S41,Services!$A$1:$B$45,2)),"",VLOOKUP(S41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U41" s="41"/>
       <c r="V41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U41,Services!$A$1:$B$45,2)),"",VLOOKUP(U41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W41" s="41"/>
       <c r="X41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W41,Services!$A$1:$B$45,2)),"",VLOOKUP(W41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y41" s="41"/>
       <c r="Z41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y41,Services!$A$1:$B$45,2)),"",VLOOKUP(Y41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA41" s="41"/>
       <c r="AB41" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA41,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA41,Services!$A$1:$B$45,2)),"",VLOOKUP(AA41,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC41" s="41"/>
@@ -10425,17 +10444,17 @@
       <c r="C42" s="42"/>
       <c r="D42" s="41"/>
       <c r="E42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D42,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D42,Region!$A$2:$B$11,2)),"",VLOOKUP(D42,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F42" s="41"/>
       <c r="G42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F42,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F42,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F42,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H42" s="41"/>
       <c r="I42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H42,'Base Locations'!A41:F381,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H42,'Base Locations'!A41:F381,2)),"",VLOOKUP(H42,'Base Locations'!A41:F381,2))</f>
         <v/>
       </c>
       <c r="J42" s="41"/>
@@ -10443,42 +10462,42 @@
       <c r="L42" s="41"/>
       <c r="M42" s="41"/>
       <c r="N42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M42,Services!$A$1:$B$45,2)),"",VLOOKUP(M42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O42" s="41"/>
       <c r="P42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O42,Services!$A$1:$B$45,2)),"",VLOOKUP(O42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q42" s="41"/>
       <c r="R42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q42,Services!$A$1:$B$45,2)),"",VLOOKUP(Q42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S42" s="41"/>
       <c r="T42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S42,Services!$A$1:$B$45,2)),"",VLOOKUP(S42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U42" s="41"/>
       <c r="V42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U42,Services!$A$1:$B$45,2)),"",VLOOKUP(U42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W42" s="41"/>
       <c r="X42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W42,Services!$A$1:$B$45,2)),"",VLOOKUP(W42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y42" s="41"/>
       <c r="Z42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y42,Services!$A$1:$B$45,2)),"",VLOOKUP(Y42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA42" s="41"/>
       <c r="AB42" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA42,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA42,Services!$A$1:$B$45,2)),"",VLOOKUP(AA42,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC42" s="41"/>
@@ -10490,17 +10509,17 @@
       <c r="C43" s="42"/>
       <c r="D43" s="41"/>
       <c r="E43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D43,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D43,Region!$A$2:$B$11,2)),"",VLOOKUP(D43,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F43" s="41"/>
       <c r="G43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F43,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F43,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F43,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H43" s="41"/>
       <c r="I43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H43,'Base Locations'!A42:F382,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H43,'Base Locations'!A42:F382,2)),"",VLOOKUP(H43,'Base Locations'!A42:F382,2))</f>
         <v/>
       </c>
       <c r="J43" s="41"/>
@@ -10508,42 +10527,42 @@
       <c r="L43" s="41"/>
       <c r="M43" s="41"/>
       <c r="N43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M43,Services!$A$1:$B$45,2)),"",VLOOKUP(M43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O43" s="41"/>
       <c r="P43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O43,Services!$A$1:$B$45,2)),"",VLOOKUP(O43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q43" s="41"/>
       <c r="R43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q43,Services!$A$1:$B$45,2)),"",VLOOKUP(Q43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S43" s="41"/>
       <c r="T43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S43,Services!$A$1:$B$45,2)),"",VLOOKUP(S43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U43" s="41"/>
       <c r="V43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U43,Services!$A$1:$B$45,2)),"",VLOOKUP(U43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W43" s="41"/>
       <c r="X43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W43,Services!$A$1:$B$45,2)),"",VLOOKUP(W43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y43" s="41"/>
       <c r="Z43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y43,Services!$A$1:$B$45,2)),"",VLOOKUP(Y43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA43" s="41"/>
       <c r="AB43" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA43,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA43,Services!$A$1:$B$45,2)),"",VLOOKUP(AA43,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC43" s="41"/>
@@ -10555,17 +10574,17 @@
       <c r="C44" s="42"/>
       <c r="D44" s="41"/>
       <c r="E44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D44,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D44,Region!$A$2:$B$11,2)),"",VLOOKUP(D44,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F44" s="41"/>
       <c r="G44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F44,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F44,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F44,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H44" s="41"/>
       <c r="I44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H44,'Base Locations'!A43:F383,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H44,'Base Locations'!A43:F383,2)),"",VLOOKUP(H44,'Base Locations'!A43:F383,2))</f>
         <v/>
       </c>
       <c r="J44" s="41"/>
@@ -10573,42 +10592,42 @@
       <c r="L44" s="41"/>
       <c r="M44" s="41"/>
       <c r="N44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M44,Services!$A$1:$B$45,2)),"",VLOOKUP(M44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O44" s="41"/>
       <c r="P44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O44,Services!$A$1:$B$45,2)),"",VLOOKUP(O44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q44" s="41"/>
       <c r="R44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q44,Services!$A$1:$B$45,2)),"",VLOOKUP(Q44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S44" s="41"/>
       <c r="T44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S44,Services!$A$1:$B$45,2)),"",VLOOKUP(S44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U44" s="41"/>
       <c r="V44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U44,Services!$A$1:$B$45,2)),"",VLOOKUP(U44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W44" s="41"/>
       <c r="X44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W44,Services!$A$1:$B$45,2)),"",VLOOKUP(W44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y44" s="41"/>
       <c r="Z44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y44,Services!$A$1:$B$45,2)),"",VLOOKUP(Y44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA44" s="41"/>
       <c r="AB44" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA44,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA44,Services!$A$1:$B$45,2)),"",VLOOKUP(AA44,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC44" s="41"/>
@@ -10620,17 +10639,17 @@
       <c r="C45" s="42"/>
       <c r="D45" s="41"/>
       <c r="E45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D45,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D45,Region!$A$2:$B$11,2)),"",VLOOKUP(D45,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F45" s="41"/>
       <c r="G45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F45,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F45,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F45,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H45" s="41"/>
       <c r="I45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H45,'Base Locations'!A44:F384,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H45,'Base Locations'!A44:F384,2)),"",VLOOKUP(H45,'Base Locations'!A44:F384,2))</f>
         <v/>
       </c>
       <c r="J45" s="41"/>
@@ -10638,42 +10657,42 @@
       <c r="L45" s="41"/>
       <c r="M45" s="41"/>
       <c r="N45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M45,Services!$A$1:$B$45,2)),"",VLOOKUP(M45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O45" s="41"/>
       <c r="P45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O45,Services!$A$1:$B$45,2)),"",VLOOKUP(O45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q45" s="41"/>
       <c r="R45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q45,Services!$A$1:$B$45,2)),"",VLOOKUP(Q45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S45" s="41"/>
       <c r="T45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S45,Services!$A$1:$B$45,2)),"",VLOOKUP(S45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U45" s="41"/>
       <c r="V45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U45,Services!$A$1:$B$45,2)),"",VLOOKUP(U45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W45" s="41"/>
       <c r="X45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W45,Services!$A$1:$B$45,2)),"",VLOOKUP(W45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y45" s="41"/>
       <c r="Z45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y45,Services!$A$1:$B$45,2)),"",VLOOKUP(Y45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA45" s="41"/>
       <c r="AB45" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA45,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA45,Services!$A$1:$B$45,2)),"",VLOOKUP(AA45,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC45" s="41"/>
@@ -10685,17 +10704,17 @@
       <c r="C46" s="42"/>
       <c r="D46" s="41"/>
       <c r="E46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D46,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D46,Region!$A$2:$B$11,2)),"",VLOOKUP(D46,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F46" s="41"/>
       <c r="G46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F46,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F46,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F46,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H46" s="41"/>
       <c r="I46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H46,'Base Locations'!A45:F385,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H46,'Base Locations'!A45:F385,2)),"",VLOOKUP(H46,'Base Locations'!A45:F385,2))</f>
         <v/>
       </c>
       <c r="J46" s="41"/>
@@ -10703,42 +10722,42 @@
       <c r="L46" s="41"/>
       <c r="M46" s="41"/>
       <c r="N46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M46,Services!$A$1:$B$45,2)),"",VLOOKUP(M46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O46" s="41"/>
       <c r="P46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O46,Services!$A$1:$B$45,2)),"",VLOOKUP(O46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q46" s="41"/>
       <c r="R46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q46,Services!$A$1:$B$45,2)),"",VLOOKUP(Q46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S46" s="41"/>
       <c r="T46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S46,Services!$A$1:$B$45,2)),"",VLOOKUP(S46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U46" s="41"/>
       <c r="V46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U46,Services!$A$1:$B$45,2)),"",VLOOKUP(U46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W46" s="41"/>
       <c r="X46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W46,Services!$A$1:$B$45,2)),"",VLOOKUP(W46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y46" s="41"/>
       <c r="Z46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y46,Services!$A$1:$B$45,2)),"",VLOOKUP(Y46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA46" s="41"/>
       <c r="AB46" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA46,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA46,Services!$A$1:$B$45,2)),"",VLOOKUP(AA46,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC46" s="41"/>
@@ -10750,17 +10769,17 @@
       <c r="C47" s="42"/>
       <c r="D47" s="41"/>
       <c r="E47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D47,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D47,Region!$A$2:$B$11,2)),"",VLOOKUP(D47,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F47" s="41"/>
       <c r="G47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F47,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F47,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F47,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H47" s="41"/>
       <c r="I47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H47,'Base Locations'!A46:F386,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H47,'Base Locations'!A46:F386,2)),"",VLOOKUP(H47,'Base Locations'!A46:F386,2))</f>
         <v/>
       </c>
       <c r="J47" s="41"/>
@@ -10768,42 +10787,42 @@
       <c r="L47" s="41"/>
       <c r="M47" s="41"/>
       <c r="N47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M47,Services!$A$1:$B$45,2)),"",VLOOKUP(M47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O47" s="41"/>
       <c r="P47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O47,Services!$A$1:$B$45,2)),"",VLOOKUP(O47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q47" s="41"/>
       <c r="R47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q47,Services!$A$1:$B$45,2)),"",VLOOKUP(Q47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S47" s="41"/>
       <c r="T47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S47,Services!$A$1:$B$45,2)),"",VLOOKUP(S47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U47" s="41"/>
       <c r="V47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U47,Services!$A$1:$B$45,2)),"",VLOOKUP(U47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W47" s="41"/>
       <c r="X47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W47,Services!$A$1:$B$45,2)),"",VLOOKUP(W47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y47" s="41"/>
       <c r="Z47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y47,Services!$A$1:$B$45,2)),"",VLOOKUP(Y47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA47" s="41"/>
       <c r="AB47" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA47,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA47,Services!$A$1:$B$45,2)),"",VLOOKUP(AA47,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC47" s="41"/>
@@ -10815,17 +10834,17 @@
       <c r="C48" s="42"/>
       <c r="D48" s="41"/>
       <c r="E48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D48,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D48,Region!$A$2:$B$11,2)),"",VLOOKUP(D48,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F48" s="41"/>
       <c r="G48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F48,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F48,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F48,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H48" s="41"/>
       <c r="I48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H48,'Base Locations'!A47:F387,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H48,'Base Locations'!A47:F387,2)),"",VLOOKUP(H48,'Base Locations'!A47:F387,2))</f>
         <v/>
       </c>
       <c r="J48" s="41"/>
@@ -10833,42 +10852,42 @@
       <c r="L48" s="41"/>
       <c r="M48" s="41"/>
       <c r="N48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M48,Services!$A$1:$B$45,2)),"",VLOOKUP(M48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O48" s="41"/>
       <c r="P48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O48,Services!$A$1:$B$45,2)),"",VLOOKUP(O48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q48" s="41"/>
       <c r="R48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q48,Services!$A$1:$B$45,2)),"",VLOOKUP(Q48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S48" s="41"/>
       <c r="T48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S48,Services!$A$1:$B$45,2)),"",VLOOKUP(S48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U48" s="41"/>
       <c r="V48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U48,Services!$A$1:$B$45,2)),"",VLOOKUP(U48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W48" s="41"/>
       <c r="X48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W48,Services!$A$1:$B$45,2)),"",VLOOKUP(W48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y48" s="41"/>
       <c r="Z48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y48,Services!$A$1:$B$45,2)),"",VLOOKUP(Y48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA48" s="41"/>
       <c r="AB48" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA48,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA48,Services!$A$1:$B$45,2)),"",VLOOKUP(AA48,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC48" s="41"/>
@@ -10880,17 +10899,17 @@
       <c r="C49" s="42"/>
       <c r="D49" s="41"/>
       <c r="E49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D49,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D49,Region!$A$2:$B$11,2)),"",VLOOKUP(D49,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F49" s="41"/>
       <c r="G49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F49,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F49,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F49,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H49" s="41"/>
       <c r="I49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H49,'Base Locations'!A48:F388,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H49,'Base Locations'!A48:F388,2)),"",VLOOKUP(H49,'Base Locations'!A48:F388,2))</f>
         <v/>
       </c>
       <c r="J49" s="41"/>
@@ -10898,42 +10917,42 @@
       <c r="L49" s="41"/>
       <c r="M49" s="41"/>
       <c r="N49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M49,Services!$A$1:$B$45,2)),"",VLOOKUP(M49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O49" s="41"/>
       <c r="P49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O49,Services!$A$1:$B$45,2)),"",VLOOKUP(O49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q49" s="41"/>
       <c r="R49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q49,Services!$A$1:$B$45,2)),"",VLOOKUP(Q49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S49" s="41"/>
       <c r="T49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S49,Services!$A$1:$B$45,2)),"",VLOOKUP(S49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U49" s="41"/>
       <c r="V49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U49,Services!$A$1:$B$45,2)),"",VLOOKUP(U49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W49" s="41"/>
       <c r="X49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W49,Services!$A$1:$B$45,2)),"",VLOOKUP(W49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y49" s="41"/>
       <c r="Z49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y49,Services!$A$1:$B$45,2)),"",VLOOKUP(Y49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA49" s="41"/>
       <c r="AB49" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA49,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA49,Services!$A$1:$B$45,2)),"",VLOOKUP(AA49,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC49" s="41"/>
@@ -10945,17 +10964,17 @@
       <c r="C50" s="42"/>
       <c r="D50" s="41"/>
       <c r="E50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(D50,Region!$A$2:$B$11,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(D50,Region!$A$2:$B$11,2)),"",VLOOKUP(D50,Region!$A$2:$B$11,2))</f>
         <v/>
       </c>
       <c r="F50" s="41"/>
       <c r="G50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(F50,'Base Locations'!$A$1:$F$341,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(F50,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F50,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
       <c r="H50" s="41"/>
       <c r="I50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(H50,'Base Locations'!A49:F389,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(H50,'Base Locations'!A49:F389,2)),"",VLOOKUP(H50,'Base Locations'!A49:F389,2))</f>
         <v/>
       </c>
       <c r="J50" s="41"/>
@@ -10963,49 +10982,49 @@
       <c r="L50" s="41"/>
       <c r="M50" s="41"/>
       <c r="N50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(M50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(M50,Services!$A$1:$B$45,2)),"",VLOOKUP(M50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="O50" s="41"/>
       <c r="P50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(O50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(O50,Services!$A$1:$B$45,2)),"",VLOOKUP(O50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Q50" s="41"/>
       <c r="R50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Q50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Q50,Services!$A$1:$B$45,2)),"",VLOOKUP(Q50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="S50" s="41"/>
       <c r="T50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(S50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(S50,Services!$A$1:$B$45,2)),"",VLOOKUP(S50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="U50" s="41"/>
       <c r="V50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(U50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(U50,Services!$A$1:$B$45,2)),"",VLOOKUP(U50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="W50" s="41"/>
       <c r="X50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(W50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(W50,Services!$A$1:$B$45,2)),"",VLOOKUP(W50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="Y50" s="41"/>
       <c r="Z50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(Y50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(Y50,Services!$A$1:$B$45,2)),"",VLOOKUP(Y50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AA50" s="41"/>
       <c r="AB50" s="1" t="str">
-        <f>_xlfn.IFNA(VLOOKUP(AA50,Services!$A$1:$B$45,2),"")</f>
+        <f>IF(ISNA(VLOOKUP(AA50,Services!$A$1:$B$45,2)),"",VLOOKUP(AA50,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
       <c r="AC50" s="41"/>
       <c r="AD50" s="41"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="WAaZ35wRl78ipiLsjfD57CyB3HV/XTkh+AkpuITrgzbsCulipizsGtzZA633/Z+avY7gs2bxn5onauLD9tGmuQ==" saltValue="T3F9NByxyx7ZjTQE4ykYyg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="6oyb3rRRfKDqti5GQJdNRgETALv5BhypIRzP7ad5VgVRdJpgy9LUEIpAIaOgXLHmnqidCaz2KGK7nd1sygRpVQ==" saltValue="jaug0yiNYL4uUSxB9UIkgQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -11066,7 +11085,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.5" collapsed="true"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -11112,7 +11131,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -11495,13 +11514,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="48.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="16" width="14.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="19" width="12.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="22" width="13.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="19" width="39.83203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="25" width="15.5" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="51.5" collapsed="true"/>
+    <col min="1" max="1" width="48.5" customWidth="1"/>
+    <col min="2" max="2" width="14" style="16" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="22" customWidth="1"/>
+    <col min="5" max="5" width="39.83203125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="25" customWidth="1"/>
+    <col min="7" max="7" width="51.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -18820,8 +18839,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.1640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="9.5" collapsed="true"/>
+    <col min="1" max="1" width="27.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: changed user type in excel files
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8991DFDA-2383-614C-A1EB-BFD86ABD8430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A898B29D-EE2A-BD49-95F4-F018BBA68441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19540" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -7641,8 +7641,8 @@
   </sheetPr>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7773,16 +7773,16 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="str">
-        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>0851oe</v>
+        <f t="shared" ref="A2:B4" ca="1" si="0">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
+        <v>8889wl</v>
       </c>
       <c r="B2" s="41" t="str">
-        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>4676fi</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1326al</v>
       </c>
       <c r="C2" s="42" t="str">
         <f ca="1">CONCATENATE(A2,".",B2,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>0851oe.4676fi511977@justice.gov.uk</v>
+        <v>8889wl.1326al984383@justice.gov.uk</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>5</v>
@@ -7863,16 +7863,16 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="str">
-        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>0803pw</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6774va</v>
       </c>
       <c r="B3" s="41" t="str">
-        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>2686td</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3128af</v>
       </c>
       <c r="C3" s="42" t="str">
         <f ca="1">CONCATENATE(A3,".",B3,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>0803pw.2686td494233@justice.gov.uk</v>
+        <v>6774va.3128af186327@justice.gov.uk</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>6</v>
@@ -7894,7 +7894,7 @@
         <v/>
       </c>
       <c r="J3" s="41" t="s">
-        <v>1198</v>
+        <v>52</v>
       </c>
       <c r="K3" s="41"/>
       <c r="L3" s="41" t="s">
@@ -7949,16 +7949,16 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="str">
-        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>5444qe</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3603th</v>
       </c>
       <c r="B4" s="41" t="str">
-        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>7318rb</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4205ir</v>
       </c>
       <c r="C4" s="42" t="str">
         <f ca="1">CONCATENATE(A4,".",B4,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>5444qe.7318rb44305@justice.gov.uk</v>
+        <v>3603th.4205ir919482@justice.gov.uk</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>9</v>
@@ -7982,7 +7982,7 @@
         <v>229786</v>
       </c>
       <c r="J4" s="41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K4" s="41" t="s">
         <v>408</v>

</xml_diff>

<commit_message>
feat: changed user type in excel files (#169)
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8991DFDA-2383-614C-A1EB-BFD86ABD8430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A898B29D-EE2A-BD49-95F4-F018BBA68441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19540" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -7641,8 +7641,8 @@
   </sheetPr>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7773,16 +7773,16 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="str">
-        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>0851oe</v>
+        <f t="shared" ref="A2:B4" ca="1" si="0">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
+        <v>8889wl</v>
       </c>
       <c r="B2" s="41" t="str">
-        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>4676fi</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1326al</v>
       </c>
       <c r="C2" s="42" t="str">
         <f ca="1">CONCATENATE(A2,".",B2,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>0851oe.4676fi511977@justice.gov.uk</v>
+        <v>8889wl.1326al984383@justice.gov.uk</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>5</v>
@@ -7863,16 +7863,16 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="str">
-        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>0803pw</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6774va</v>
       </c>
       <c r="B3" s="41" t="str">
-        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>2686td</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3128af</v>
       </c>
       <c r="C3" s="42" t="str">
         <f ca="1">CONCATENATE(A3,".",B3,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>0803pw.2686td494233@justice.gov.uk</v>
+        <v>6774va.3128af186327@justice.gov.uk</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>6</v>
@@ -7894,7 +7894,7 @@
         <v/>
       </c>
       <c r="J3" s="41" t="s">
-        <v>1198</v>
+        <v>52</v>
       </c>
       <c r="K3" s="41"/>
       <c r="L3" s="41" t="s">
@@ -7949,16 +7949,16 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="str">
-        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>5444qe</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3603th</v>
       </c>
       <c r="B4" s="41" t="str">
-        <f ca="1">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>7318rb</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4205ir</v>
       </c>
       <c r="C4" s="42" t="str">
         <f ca="1">CONCATENATE(A4,".",B4,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>5444qe.7318rb44305@justice.gov.uk</v>
+        <v>3603th.4205ir919482@justice.gov.uk</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>9</v>
@@ -7982,7 +7982,7 @@
         <v>229786</v>
       </c>
       <c r="J4" s="41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K4" s="41" t="s">
         <v>408</v>

</xml_diff>

<commit_message>
RDCC-2371 - trim flow- updated functional and junits
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/429962/hmcts/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A898B29D-EE2A-BD49-95F4-F018BBA68441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8A00FC-B75C-8547-B920-834EDAD380F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19540" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="1200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="1202">
   <si>
     <t>Region</t>
   </si>
@@ -3644,6 +3644,12 @@
   </si>
   <si>
     <t>caseworker-iac</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> untrimmed </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> caseworker-iac, caseworker-iac-dwp, </t>
   </si>
 </sst>
 </file>
@@ -7641,8 +7647,8 @@
   </sheetPr>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7773,16 +7779,16 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="str">
-        <f t="shared" ref="A2:B4" ca="1" si="0">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>8889wl</v>
+        <f t="shared" ref="A2:B5" ca="1" si="0">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
+        <v>4994oe</v>
       </c>
       <c r="B2" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>1326al</v>
+        <v>3250fd</v>
       </c>
       <c r="C2" s="42" t="str">
-        <f ca="1">CONCATENATE(A2,".",B2,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>8889wl.1326al984383@justice.gov.uk</v>
+        <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
+        <v>CWR-func-test-user-3142954156@justice.gov.uk</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>5</v>
@@ -7864,15 +7870,15 @@
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>6774va</v>
+        <v>8629jd</v>
       </c>
       <c r="B3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3128af</v>
+        <v>8318vk</v>
       </c>
       <c r="C3" s="42" t="str">
-        <f ca="1">CONCATENATE(A3,".",B3,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>6774va.3128af186327@justice.gov.uk</v>
+        <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
+        <v>CWR-func-test-user-3006812824@justice.gov.uk</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>6</v>
@@ -7950,15 +7956,15 @@
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>3603th</v>
+        <v>0768nk</v>
       </c>
       <c r="B4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>4205ir</v>
+        <v>2284ga</v>
       </c>
       <c r="C4" s="42" t="str">
-        <f ca="1">CONCATENATE(A4,".",B4,RANDBETWEEN(1,999999),"@","justice.gov.uk")</f>
-        <v>3603th.4205ir919482@justice.gov.uk</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>CWR-func-test-user-1681855941@justice.gov.uk</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>9</v>
@@ -8031,34 +8037,57 @@
         <v/>
       </c>
       <c r="AC4" s="41"/>
-      <c r="AD4" s="41"/>
+      <c r="AD4" s="41" t="s">
+        <v>1121</v>
+      </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="1" t="str">
+      <c r="A5" s="41" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C5" s="42" t="str">
+        <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
+        <v>CWR-func-test-user-4001221951@justice.gov.uk</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
         <f>IF(ISNA(VLOOKUP(D5,Region!$A$2:$B$11,2)),"",VLOOKUP(D5,Region!$A$2:$B$11,2))</f>
-        <v/>
-      </c>
-      <c r="F5" s="41"/>
-      <c r="G5" s="1" t="str">
+        <v>2</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="1">
         <f>IF(ISNA(VLOOKUP(F5,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F5,'Base Locations'!$A$1:$F$341,2))</f>
-        <v/>
-      </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="1" t="str">
+        <v>206150</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="1">
         <f>IF(ISNA(VLOOKUP(H5,'Base Locations'!A4:F344,2)),"",VLOOKUP(H5,'Base Locations'!A4:F344,2))</f>
-        <v/>
-      </c>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
+        <v>271588</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="41" t="s">
+        <v>408</v>
+      </c>
+      <c r="L5" s="41" t="s">
+        <v>409</v>
+      </c>
+      <c r="M5" s="41" t="s">
+        <v>1169</v>
+      </c>
       <c r="N5" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M5,Services!$A$1:$B$45,2)),"",VLOOKUP(M5,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BHA3</v>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="1" t="str">
@@ -8095,8 +8124,12 @@
         <f>IF(ISNA(VLOOKUP(AA5,Services!$A$1:$B$45,2)),"",VLOOKUP(AA5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
-      <c r="AC5" s="41"/>
-      <c r="AD5" s="41"/>
+      <c r="AC5" s="41" t="s">
+        <v>1201</v>
+      </c>
+      <c r="AD5" s="41" t="s">
+        <v>1121</v>
+      </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="41"/>

</xml_diff>

<commit_message>
RDCC-2509: updating excel to not have numbers in names for FTs
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/429962/hmcts/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/778425/Projects/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8A00FC-B75C-8547-B920-834EDAD380F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5C364A-3D47-7940-8583-5AAFB24B83D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -7647,8 +7647,8 @@
   </sheetPr>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7779,16 +7779,16 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="str">
-        <f t="shared" ref="A2:B5" ca="1" si="0">TEXT(RANDBETWEEN(0,9999),"0000")&amp;CHAR(RANDBETWEEN(97,122))&amp;CHAR(RANDBETWEEN(97,122))</f>
-        <v>4994oe</v>
+        <f ca="1">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
+        <v>Cjde</v>
       </c>
       <c r="B2" s="41" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>3250fd</v>
+        <f ca="1">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
+        <v>Zopd</v>
       </c>
       <c r="C2" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-3142954156@justice.gov.uk</v>
+        <v>CWR-func-test-user-1573471325@justice.gov.uk</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>5</v>
@@ -7869,16 +7869,16 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>8629jd</v>
+        <f ca="1">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
+        <v>Gwpn</v>
       </c>
       <c r="B3" s="41" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>8318vk</v>
+        <f ca="1">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
+        <v>Bdnm</v>
       </c>
       <c r="C3" s="42" t="str">
-        <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-3006812824@justice.gov.uk</v>
+        <f t="shared" ref="C3:C4" ca="1" si="0">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
+        <v>CWR-func-test-user-1455990037@justice.gov.uk</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>6</v>
@@ -7955,16 +7955,16 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="str">
+        <f ca="1">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
+        <v>Nina</v>
+      </c>
+      <c r="B4" s="41" t="str">
+        <f ca="1">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
+        <v>Secg</v>
+      </c>
+      <c r="C4" s="42" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>0768nk</v>
-      </c>
-      <c r="B4" s="41" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2284ga</v>
-      </c>
-      <c r="C4" s="42" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-1681855941@justice.gov.uk</v>
+        <v>CWR-func-test-user-2400670545@justice.gov.uk</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>9</v>
@@ -8050,7 +8050,7 @@
       </c>
       <c r="C5" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-4001221951@justice.gov.uk</v>
+        <v>CWR-func-test-user-8944558260@justice.gov.uk</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
feat: RDCC-3540 removed case allocator and task supervisor header validation
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893419B9-84BE-774B-BBF6-457AD03808D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A574EF62-AC2D-DC4A-8DAB-3046A4F05BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="1212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="1210">
   <si>
     <t>Region</t>
   </si>
@@ -3626,12 +3626,6 @@
   </si>
   <si>
     <t xml:space="preserve"> caseworker-iac, caseworker-iac-dwp, </t>
-  </si>
-  <si>
-    <t>Case Allocator</t>
-  </si>
-  <si>
-    <t>Task Supervisor</t>
   </si>
   <si>
     <t>Service1</t>
@@ -7675,7 +7669,7 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AF50"/>
+  <dimension ref="A1:AD50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="AE2" sqref="AE2"/>
@@ -7715,7 +7709,7 @@
     <col min="30" max="30" width="9.1640625" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="36" t="s">
         <v>1107</v>
       </c>
@@ -7753,52 +7747,52 @@
         <v>411</v>
       </c>
       <c r="M1" s="38" t="s">
+        <v>1194</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>1195</v>
+      </c>
+      <c r="O1" s="36" t="s">
         <v>1196</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="P1" s="29" t="s">
         <v>1197</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="Q1" s="39" t="s">
         <v>1198</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="R1" s="29" t="s">
         <v>1199</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="S1" s="38" t="s">
         <v>1200</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="T1" s="29" t="s">
         <v>1201</v>
       </c>
-      <c r="S1" s="38" t="s">
+      <c r="U1" s="38" t="s">
         <v>1202</v>
       </c>
-      <c r="T1" s="29" t="s">
+      <c r="V1" s="28" t="s">
         <v>1203</v>
       </c>
-      <c r="U1" s="38" t="s">
+      <c r="W1" s="38" t="s">
         <v>1204</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="X1" s="28" t="s">
         <v>1205</v>
       </c>
-      <c r="W1" s="38" t="s">
+      <c r="Y1" s="38" t="s">
         <v>1206</v>
       </c>
-      <c r="X1" s="28" t="s">
+      <c r="Z1" s="28" t="s">
         <v>1207</v>
       </c>
-      <c r="Y1" s="38" t="s">
+      <c r="AA1" s="38" t="s">
         <v>1208</v>
       </c>
-      <c r="Z1" s="28" t="s">
+      <c r="AB1" s="28" t="s">
         <v>1209</v>
-      </c>
-      <c r="AA1" s="38" t="s">
-        <v>1210</v>
-      </c>
-      <c r="AB1" s="28" t="s">
-        <v>1211</v>
       </c>
       <c r="AC1" s="38" t="s">
         <v>2</v>
@@ -7806,25 +7800,19 @@
       <c r="AD1" s="43" t="s">
         <v>1112</v>
       </c>
-      <c r="AE1" s="43" t="s">
-        <v>1194</v>
-      </c>
-      <c r="AF1" s="43" t="s">
-        <v>1195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="str">
         <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Jesy</v>
+        <v>Yeka</v>
       </c>
       <c r="B2" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Wdzf</v>
+        <v>Lubb</v>
       </c>
       <c r="C2" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-8466589903@justice.gov.uk</v>
+        <v>CWR-func-test-user-7973693164@justice.gov.uk</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>5</v>
@@ -7903,18 +7891,18 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Lcko</v>
+        <v>Seia</v>
       </c>
       <c r="B3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Uspq</v>
+        <v>Gnvt</v>
       </c>
       <c r="C3" s="42" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-9020055654@justice.gov.uk</v>
+        <v>CWR-func-test-user-6688385739@justice.gov.uk</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>6</v>
@@ -7989,18 +7977,18 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Mmij</v>
+        <v>Ukru</v>
       </c>
       <c r="B4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ggdr</v>
+        <v>Srhr</v>
       </c>
       <c r="C4" s="42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-7899977346@justice.gov.uk</v>
+        <v>CWR-func-test-user-8813178468@justice.gov.uk</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>9</v>
@@ -8077,7 +8065,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
         <v>1192</v>
       </c>
@@ -8086,7 +8074,7 @@
       </c>
       <c r="C5" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-5947612411@justice.gov.uk</v>
+        <v>CWR-func-test-user-7422657295@justice.gov.uk</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>4</v>
@@ -8167,7 +8155,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="41"/>
       <c r="B6" s="41"/>
       <c r="C6" s="42"/>
@@ -8232,7 +8220,7 @@
       <c r="AC6" s="41"/>
       <c r="AD6" s="41"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="41"/>
       <c r="B7" s="41"/>
       <c r="C7" s="42"/>
@@ -8297,7 +8285,7 @@
       <c r="AC7" s="41"/>
       <c r="AD7" s="41"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="41"/>
       <c r="B8" s="41"/>
       <c r="C8" s="42"/>
@@ -8362,7 +8350,7 @@
       <c r="AC8" s="41"/>
       <c r="AD8" s="41"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="41"/>
       <c r="B9" s="41"/>
       <c r="C9" s="42"/>
@@ -8427,7 +8415,7 @@
       <c r="AC9" s="41"/>
       <c r="AD9" s="41"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="41"/>
       <c r="B10" s="41"/>
       <c r="C10" s="42"/>
@@ -8492,7 +8480,7 @@
       <c r="AC10" s="41"/>
       <c r="AD10" s="41"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="41"/>
       <c r="B11" s="41"/>
       <c r="C11" s="42"/>
@@ -8557,7 +8545,7 @@
       <c r="AC11" s="41"/>
       <c r="AD11" s="41"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="41"/>
       <c r="B12" s="41"/>
       <c r="C12" s="42"/>
@@ -8622,7 +8610,7 @@
       <c r="AC12" s="41"/>
       <c r="AD12" s="41"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="41"/>
       <c r="B13" s="41"/>
       <c r="C13" s="42"/>
@@ -8687,7 +8675,7 @@
       <c r="AC13" s="41"/>
       <c r="AD13" s="41"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="41"/>
       <c r="B14" s="41"/>
       <c r="C14" s="42"/>
@@ -8752,7 +8740,7 @@
       <c r="AC14" s="41"/>
       <c r="AD14" s="41"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="41"/>
       <c r="B15" s="41"/>
       <c r="C15" s="42"/>
@@ -8817,7 +8805,7 @@
       <c r="AC15" s="41"/>
       <c r="AD15" s="41"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="41"/>
       <c r="B16" s="41"/>
       <c r="C16" s="42"/>

</xml_diff>

<commit_message>
Added with Updated Functional Test (#433)
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_2109032/RDCC4025/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A574EF62-AC2D-DC4A-8DAB-3046A4F05BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1943D1-4BDA-3642-9763-573B81B92472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19520" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="11" r:id="rId1"/>
     <sheet name="Terminology" sheetId="12" r:id="rId2"/>
     <sheet name="Staff Data" sheetId="1" r:id="rId3"/>
-    <sheet name="User Type" sheetId="9" state="hidden" r:id="rId4"/>
-    <sheet name="Services" sheetId="7" state="hidden" r:id="rId5"/>
-    <sheet name="Base Locations" sheetId="6" state="hidden" r:id="rId6"/>
-    <sheet name="Region" sheetId="3" state="hidden" r:id="rId7"/>
-    <sheet name="Roles" sheetId="4" state="hidden" r:id="rId8"/>
-    <sheet name="Validations" sheetId="10" state="hidden" r:id="rId9"/>
+    <sheet name="User Type" sheetId="9" r:id="rId4"/>
+    <sheet name="Services" sheetId="7" r:id="rId5"/>
+    <sheet name="Base Locations" sheetId="6" r:id="rId6"/>
+    <sheet name="Region" sheetId="3" r:id="rId7"/>
+    <sheet name="Roles" sheetId="4" r:id="rId8"/>
+    <sheet name="Validations" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="1210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="1218">
   <si>
     <t>Region</t>
   </si>
@@ -3674,6 +3674,30 @@
   </si>
   <si>
     <t>Service8 ID</t>
+  </si>
+  <si>
+    <t>Hearing Centre Team Leader </t>
+  </si>
+  <si>
+    <t>Hearing Centre Administrator</t>
+  </si>
+  <si>
+    <t>Court Clerk</t>
+  </si>
+  <si>
+    <t>National Business Centre Team leader</t>
+  </si>
+  <si>
+    <t>National Business Centre Listing team</t>
+  </si>
+  <si>
+    <t>National Business Centre Payments team</t>
+  </si>
+  <si>
+    <t>CTSC team leader</t>
+  </si>
+  <si>
+    <t>CTSC Administrator</t>
   </si>
 </sst>
 </file>
@@ -7671,8 +7695,8 @@
   </sheetPr>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7689,24 +7713,24 @@
     <col min="10" max="10" width="15.5" style="40" customWidth="1"/>
     <col min="11" max="11" width="25.5" style="40" customWidth="1"/>
     <col min="12" max="12" width="19.5" style="40" customWidth="1"/>
-    <col min="13" max="13" width="24" style="40" customWidth="1"/>
-    <col min="14" max="14" width="24" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="21.33203125" style="40" customWidth="1"/>
-    <col min="16" max="16" width="21.33203125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="19.1640625" style="40" customWidth="1"/>
-    <col min="18" max="18" width="19.1640625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="19.1640625" style="40" customWidth="1"/>
-    <col min="20" max="20" width="19.1640625" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="16" style="40" customWidth="1"/>
-    <col min="22" max="22" width="16" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="14.5" style="40" customWidth="1"/>
-    <col min="24" max="24" width="14.5" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" style="40" customWidth="1"/>
-    <col min="26" max="26" width="17.33203125" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="14.5" style="40" customWidth="1"/>
-    <col min="28" max="28" width="14.5" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="25.5" style="40" customWidth="1"/>
-    <col min="30" max="30" width="9.1640625" style="40"/>
+    <col min="13" max="13" width="8.83203125" style="40"/>
+    <col min="14" max="14" width="24" style="40" customWidth="1"/>
+    <col min="15" max="15" width="24" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="21.33203125" style="40" customWidth="1"/>
+    <col min="17" max="17" width="21.33203125" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="19.1640625" style="40" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="19.1640625" style="40" customWidth="1"/>
+    <col min="21" max="21" width="19.1640625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="16" style="40" customWidth="1"/>
+    <col min="23" max="23" width="16" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="14.5" style="40" customWidth="1"/>
+    <col min="25" max="25" width="14.5" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="17.33203125" style="40" customWidth="1"/>
+    <col min="27" max="27" width="17.33203125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="14.5" style="40" customWidth="1"/>
+    <col min="29" max="29" width="14.5" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="25.5" style="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -7746,73 +7770,73 @@
       <c r="L1" s="37" t="s">
         <v>411</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="43" t="s">
+        <v>1112</v>
+      </c>
+      <c r="N1" s="38" t="s">
         <v>1194</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="O1" s="27" t="s">
         <v>1195</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="P1" s="36" t="s">
         <v>1196</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="Q1" s="29" t="s">
         <v>1197</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="R1" s="39" t="s">
         <v>1198</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="S1" s="29" t="s">
         <v>1199</v>
       </c>
-      <c r="S1" s="38" t="s">
+      <c r="T1" s="38" t="s">
         <v>1200</v>
       </c>
-      <c r="T1" s="29" t="s">
+      <c r="U1" s="29" t="s">
         <v>1201</v>
       </c>
-      <c r="U1" s="38" t="s">
+      <c r="V1" s="38" t="s">
         <v>1202</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="W1" s="28" t="s">
         <v>1203</v>
       </c>
-      <c r="W1" s="38" t="s">
+      <c r="X1" s="38" t="s">
         <v>1204</v>
       </c>
-      <c r="X1" s="28" t="s">
+      <c r="Y1" s="28" t="s">
         <v>1205</v>
       </c>
-      <c r="Y1" s="38" t="s">
+      <c r="Z1" s="38" t="s">
         <v>1206</v>
       </c>
-      <c r="Z1" s="28" t="s">
+      <c r="AA1" s="28" t="s">
         <v>1207</v>
       </c>
-      <c r="AA1" s="38" t="s">
+      <c r="AB1" s="38" t="s">
         <v>1208</v>
       </c>
-      <c r="AB1" s="28" t="s">
+      <c r="AC1" s="28" t="s">
         <v>1209</v>
       </c>
-      <c r="AC1" s="38" t="s">
+      <c r="AD1" s="38" t="s">
         <v>2</v>
-      </c>
-      <c r="AD1" s="43" t="s">
-        <v>1112</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="str">
         <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Yeka</v>
+        <v>Aiij</v>
       </c>
       <c r="B2" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Lubb</v>
+        <v>Qsey</v>
       </c>
       <c r="C2" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-7973693164@justice.gov.uk</v>
+        <v>CWR-func-test-user-2237320615@justice.gov.uk</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>5</v>
@@ -7843,66 +7867,66 @@
       </c>
       <c r="L2" s="41"/>
       <c r="M2" s="41" t="s">
+        <v>1113</v>
+      </c>
+      <c r="N2" s="41" t="s">
         <v>1161</v>
       </c>
-      <c r="N2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M2,Services!$A$1:$B$45,2)),"",VLOOKUP(M2,Services!$A$1:$B$45,2))</f>
+      <c r="O2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N2,Services!$A$1:$B$45,2)),"",VLOOKUP(N2,Services!$A$1:$B$45,2))</f>
         <v>BHA3</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O2,Services!$A$1:$B$45,2)),"",VLOOKUP(O2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q2,Services!$A$1:$B$45,2)),"",VLOOKUP(Q2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S2" s="41"/>
-      <c r="T2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S2,Services!$A$1:$B$45,2)),"",VLOOKUP(S2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U2" s="41"/>
-      <c r="V2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U2,Services!$A$1:$B$45,2)),"",VLOOKUP(U2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W2" s="41"/>
-      <c r="X2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W2,Services!$A$1:$B$45,2)),"",VLOOKUP(W2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y2,Services!$A$1:$B$45,2)),"",VLOOKUP(Y2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA2,Services!$A$1:$B$45,2)),"",VLOOKUP(AA2,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC2" s="41" t="s">
+      <c r="P2" s="41"/>
+      <c r="Q2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P2,Services!$A$1:$B$45,2)),"",VLOOKUP(P2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R2" s="41"/>
+      <c r="S2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R2,Services!$A$1:$B$45,2)),"",VLOOKUP(R2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T2" s="41"/>
+      <c r="U2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T2,Services!$A$1:$B$45,2)),"",VLOOKUP(T2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V2" s="41"/>
+      <c r="W2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V2,Services!$A$1:$B$45,2)),"",VLOOKUP(V2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X2,Services!$A$1:$B$45,2)),"",VLOOKUP(X2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z2" s="41"/>
+      <c r="AA2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z2,Services!$A$1:$B$45,2)),"",VLOOKUP(Z2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB2,Services!$A$1:$B$45,2)),"",VLOOKUP(AB2,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AD2" s="41" t="s">
         <v>1191</v>
-      </c>
-      <c r="AD2" s="41" t="s">
-        <v>1113</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Seia</v>
+        <v>Tqlo</v>
       </c>
       <c r="B3" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gnvt</v>
+        <v>Bhgg</v>
       </c>
       <c r="C3" s="42" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-6688385739@justice.gov.uk</v>
+        <v>CWR-func-test-user-5238904422@justice.gov.uk</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>6</v>
@@ -7930,65 +7954,65 @@
       <c r="L3" s="41" t="s">
         <v>409</v>
       </c>
-      <c r="M3" s="41"/>
-      <c r="N3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M3,Services!$A$1:$B$45,2)),"",VLOOKUP(M3,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O3" s="41" t="s">
+      <c r="M3" s="41" t="s">
+        <v>1113</v>
+      </c>
+      <c r="N3" s="41"/>
+      <c r="O3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N3,Services!$A$1:$B$45,2)),"",VLOOKUP(N3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P3" s="41" t="s">
         <v>1160</v>
       </c>
-      <c r="P3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O3,Services!$A$1:$B$45,2)),"",VLOOKUP(O3,Services!$A$1:$B$45,2))</f>
+      <c r="Q3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P3,Services!$A$1:$B$45,2)),"",VLOOKUP(P3,Services!$A$1:$B$45,2))</f>
         <v>BAB2</v>
       </c>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q3,Services!$A$1:$B$45,2)),"",VLOOKUP(Q3,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S3" s="41"/>
-      <c r="T3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S3,Services!$A$1:$B$45,2)),"",VLOOKUP(S3,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U3" s="41"/>
-      <c r="V3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U3,Services!$A$1:$B$45,2)),"",VLOOKUP(U3,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W3" s="41"/>
-      <c r="X3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W3,Services!$A$1:$B$45,2)),"",VLOOKUP(W3,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y3,Services!$A$1:$B$45,2)),"",VLOOKUP(Y3,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA3" s="41"/>
-      <c r="AB3" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA3,Services!$A$1:$B$45,2)),"",VLOOKUP(AA3,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC3" s="41"/>
-      <c r="AD3" s="41" t="s">
-        <v>1113</v>
-      </c>
+      <c r="R3" s="41"/>
+      <c r="S3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R3,Services!$A$1:$B$45,2)),"",VLOOKUP(R3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T3" s="41"/>
+      <c r="U3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T3,Services!$A$1:$B$45,2)),"",VLOOKUP(T3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V3" s="41"/>
+      <c r="W3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V3,Services!$A$1:$B$45,2)),"",VLOOKUP(V3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X3,Services!$A$1:$B$45,2)),"",VLOOKUP(X3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z3,Services!$A$1:$B$45,2)),"",VLOOKUP(Z3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB3,Services!$A$1:$B$45,2)),"",VLOOKUP(AB3,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AD3" s="41"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ukru</v>
+        <v>Gtix</v>
       </c>
       <c r="B4" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Srhr</v>
+        <v>Fyct</v>
       </c>
       <c r="C4" s="42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-8813178468@justice.gov.uk</v>
+        <v>CWR-func-test-user-5583400545@justice.gov.uk</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>9</v>
@@ -8018,52 +8042,52 @@
         <v>408</v>
       </c>
       <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M4,Services!$A$1:$B$45,2)),"",VLOOKUP(M4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O4" s="41"/>
-      <c r="P4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O4,Services!$A$1:$B$45,2)),"",VLOOKUP(O4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q4,Services!$A$1:$B$45,2)),"",VLOOKUP(Q4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S4" s="41" t="s">
+      <c r="M4" s="41" t="s">
+        <v>1113</v>
+      </c>
+      <c r="N4" s="41"/>
+      <c r="O4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N4,Services!$A$1:$B$45,2)),"",VLOOKUP(N4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P4,Services!$A$1:$B$45,2)),"",VLOOKUP(P4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R4" s="41"/>
+      <c r="S4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R4,Services!$A$1:$B$45,2)),"",VLOOKUP(R4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T4" s="41" t="s">
         <v>1159</v>
       </c>
-      <c r="T4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S4,Services!$A$1:$B$45,2)),"",VLOOKUP(S4,Services!$A$1:$B$45,2))</f>
+      <c r="U4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T4,Services!$A$1:$B$45,2)),"",VLOOKUP(T4,Services!$A$1:$B$45,2))</f>
         <v>BAB2</v>
       </c>
-      <c r="U4" s="41"/>
-      <c r="V4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U4,Services!$A$1:$B$45,2)),"",VLOOKUP(U4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W4" s="41"/>
-      <c r="X4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W4,Services!$A$1:$B$45,2)),"",VLOOKUP(W4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y4" s="41"/>
-      <c r="Z4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y4,Services!$A$1:$B$45,2)),"",VLOOKUP(Y4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA4" s="41"/>
-      <c r="AB4" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA4,Services!$A$1:$B$45,2)),"",VLOOKUP(AA4,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC4" s="41"/>
-      <c r="AD4" s="41" t="s">
-        <v>1113</v>
-      </c>
+      <c r="V4" s="41"/>
+      <c r="W4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V4,Services!$A$1:$B$45,2)),"",VLOOKUP(V4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X4,Services!$A$1:$B$45,2)),"",VLOOKUP(X4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z4,Services!$A$1:$B$45,2)),"",VLOOKUP(Z4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB4" s="41"/>
+      <c r="AC4" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB4,Services!$A$1:$B$45,2)),"",VLOOKUP(AB4,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AD4" s="41"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
@@ -8074,7 +8098,7 @@
       </c>
       <c r="C5" s="42" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-7422657295@justice.gov.uk</v>
+        <v>CWR-func-test-user-9987389828@justice.gov.uk</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>4</v>
@@ -8107,52 +8131,52 @@
         <v>409</v>
       </c>
       <c r="M5" s="41" t="s">
+        <v>1113</v>
+      </c>
+      <c r="N5" s="41" t="s">
         <v>1161</v>
       </c>
-      <c r="N5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M5,Services!$A$1:$B$45,2)),"",VLOOKUP(M5,Services!$A$1:$B$45,2))</f>
+      <c r="O5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N5,Services!$A$1:$B$45,2)),"",VLOOKUP(N5,Services!$A$1:$B$45,2))</f>
         <v>BHA3</v>
       </c>
-      <c r="O5" s="41"/>
-      <c r="P5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O5,Services!$A$1:$B$45,2)),"",VLOOKUP(O5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q5,Services!$A$1:$B$45,2)),"",VLOOKUP(Q5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S5" s="41"/>
-      <c r="T5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S5,Services!$A$1:$B$45,2)),"",VLOOKUP(S5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U5" s="41"/>
-      <c r="V5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U5,Services!$A$1:$B$45,2)),"",VLOOKUP(U5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W5" s="41"/>
-      <c r="X5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W5,Services!$A$1:$B$45,2)),"",VLOOKUP(W5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y5" s="41"/>
-      <c r="Z5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y5,Services!$A$1:$B$45,2)),"",VLOOKUP(Y5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA5" s="41"/>
-      <c r="AB5" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA5,Services!$A$1:$B$45,2)),"",VLOOKUP(AA5,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC5" s="41" t="s">
+      <c r="P5" s="41"/>
+      <c r="Q5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P5,Services!$A$1:$B$45,2)),"",VLOOKUP(P5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R5" s="41"/>
+      <c r="S5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R5,Services!$A$1:$B$45,2)),"",VLOOKUP(R5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T5" s="41"/>
+      <c r="U5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T5,Services!$A$1:$B$45,2)),"",VLOOKUP(T5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V5" s="41"/>
+      <c r="W5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V5,Services!$A$1:$B$45,2)),"",VLOOKUP(V5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X5,Services!$A$1:$B$45,2)),"",VLOOKUP(X5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z5" s="41"/>
+      <c r="AA5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z5,Services!$A$1:$B$45,2)),"",VLOOKUP(Z5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB5" s="41"/>
+      <c r="AC5" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB5,Services!$A$1:$B$45,2)),"",VLOOKUP(AB5,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AD5" s="41" t="s">
         <v>1193</v>
-      </c>
-      <c r="AD5" s="41" t="s">
-        <v>1113</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
@@ -8178,46 +8202,46 @@
       <c r="K6" s="41"/>
       <c r="L6" s="41"/>
       <c r="M6" s="41"/>
-      <c r="N6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M6,Services!$A$1:$B$45,2)),"",VLOOKUP(M6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O6" s="41"/>
-      <c r="P6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O6,Services!$A$1:$B$45,2)),"",VLOOKUP(O6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q6,Services!$A$1:$B$45,2)),"",VLOOKUP(Q6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S6" s="41"/>
-      <c r="T6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S6,Services!$A$1:$B$45,2)),"",VLOOKUP(S6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U6" s="41"/>
-      <c r="V6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U6,Services!$A$1:$B$45,2)),"",VLOOKUP(U6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W6" s="41"/>
-      <c r="X6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W6,Services!$A$1:$B$45,2)),"",VLOOKUP(W6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y6,Services!$A$1:$B$45,2)),"",VLOOKUP(Y6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA6" s="41"/>
-      <c r="AB6" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA6,Services!$A$1:$B$45,2)),"",VLOOKUP(AA6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N6,Services!$A$1:$B$45,2)),"",VLOOKUP(N6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P6,Services!$A$1:$B$45,2)),"",VLOOKUP(P6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R6" s="41"/>
+      <c r="S6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R6,Services!$A$1:$B$45,2)),"",VLOOKUP(R6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T6" s="41"/>
+      <c r="U6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T6,Services!$A$1:$B$45,2)),"",VLOOKUP(T6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V6" s="41"/>
+      <c r="W6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V6,Services!$A$1:$B$45,2)),"",VLOOKUP(V6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X6,Services!$A$1:$B$45,2)),"",VLOOKUP(X6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z6" s="41"/>
+      <c r="AA6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z6,Services!$A$1:$B$45,2)),"",VLOOKUP(Z6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB6" s="41"/>
+      <c r="AC6" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB6,Services!$A$1:$B$45,2)),"",VLOOKUP(AB6,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD6" s="41"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
@@ -8243,46 +8267,46 @@
       <c r="K7" s="41"/>
       <c r="L7" s="41"/>
       <c r="M7" s="41"/>
-      <c r="N7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M7,Services!$A$1:$B$45,2)),"",VLOOKUP(M7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O7" s="41"/>
-      <c r="P7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O7,Services!$A$1:$B$45,2)),"",VLOOKUP(O7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q7,Services!$A$1:$B$45,2)),"",VLOOKUP(Q7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S7" s="41"/>
-      <c r="T7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S7,Services!$A$1:$B$45,2)),"",VLOOKUP(S7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U7" s="41"/>
-      <c r="V7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U7,Services!$A$1:$B$45,2)),"",VLOOKUP(U7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W7" s="41"/>
-      <c r="X7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W7,Services!$A$1:$B$45,2)),"",VLOOKUP(W7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y7" s="41"/>
-      <c r="Z7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y7,Services!$A$1:$B$45,2)),"",VLOOKUP(Y7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA7" s="41"/>
-      <c r="AB7" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA7,Services!$A$1:$B$45,2)),"",VLOOKUP(AA7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N7,Services!$A$1:$B$45,2)),"",VLOOKUP(N7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P7,Services!$A$1:$B$45,2)),"",VLOOKUP(P7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R7" s="41"/>
+      <c r="S7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R7,Services!$A$1:$B$45,2)),"",VLOOKUP(R7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T7" s="41"/>
+      <c r="U7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T7,Services!$A$1:$B$45,2)),"",VLOOKUP(T7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V7" s="41"/>
+      <c r="W7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V7,Services!$A$1:$B$45,2)),"",VLOOKUP(V7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X7,Services!$A$1:$B$45,2)),"",VLOOKUP(X7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z7,Services!$A$1:$B$45,2)),"",VLOOKUP(Z7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB7" s="41"/>
+      <c r="AC7" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB7,Services!$A$1:$B$45,2)),"",VLOOKUP(AB7,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD7" s="41"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
@@ -8308,46 +8332,46 @@
       <c r="K8" s="41"/>
       <c r="L8" s="41"/>
       <c r="M8" s="41"/>
-      <c r="N8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M8,Services!$A$1:$B$45,2)),"",VLOOKUP(M8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O8" s="41"/>
-      <c r="P8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O8,Services!$A$1:$B$45,2)),"",VLOOKUP(O8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q8,Services!$A$1:$B$45,2)),"",VLOOKUP(Q8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S8" s="41"/>
-      <c r="T8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S8,Services!$A$1:$B$45,2)),"",VLOOKUP(S8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U8" s="41"/>
-      <c r="V8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U8,Services!$A$1:$B$45,2)),"",VLOOKUP(U8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W8" s="41"/>
-      <c r="X8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W8,Services!$A$1:$B$45,2)),"",VLOOKUP(W8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y8,Services!$A$1:$B$45,2)),"",VLOOKUP(Y8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA8" s="41"/>
-      <c r="AB8" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA8,Services!$A$1:$B$45,2)),"",VLOOKUP(AA8,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N8,Services!$A$1:$B$45,2)),"",VLOOKUP(N8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P8,Services!$A$1:$B$45,2)),"",VLOOKUP(P8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R8" s="41"/>
+      <c r="S8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R8,Services!$A$1:$B$45,2)),"",VLOOKUP(R8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T8" s="41"/>
+      <c r="U8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T8,Services!$A$1:$B$45,2)),"",VLOOKUP(T8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V8" s="41"/>
+      <c r="W8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V8,Services!$A$1:$B$45,2)),"",VLOOKUP(V8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X8,Services!$A$1:$B$45,2)),"",VLOOKUP(X8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z8,Services!$A$1:$B$45,2)),"",VLOOKUP(Z8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB8" s="41"/>
+      <c r="AC8" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB8,Services!$A$1:$B$45,2)),"",VLOOKUP(AB8,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD8" s="41"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
@@ -8373,46 +8397,46 @@
       <c r="K9" s="41"/>
       <c r="L9" s="41"/>
       <c r="M9" s="41"/>
-      <c r="N9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M9,Services!$A$1:$B$45,2)),"",VLOOKUP(M9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O9" s="41"/>
-      <c r="P9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O9,Services!$A$1:$B$45,2)),"",VLOOKUP(O9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q9,Services!$A$1:$B$45,2)),"",VLOOKUP(Q9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S9" s="41"/>
-      <c r="T9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S9,Services!$A$1:$B$45,2)),"",VLOOKUP(S9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U9" s="41"/>
-      <c r="V9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U9,Services!$A$1:$B$45,2)),"",VLOOKUP(U9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W9" s="41"/>
-      <c r="X9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W9,Services!$A$1:$B$45,2)),"",VLOOKUP(W9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y9" s="41"/>
-      <c r="Z9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y9,Services!$A$1:$B$45,2)),"",VLOOKUP(Y9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA9" s="41"/>
-      <c r="AB9" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA9,Services!$A$1:$B$45,2)),"",VLOOKUP(AA9,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N9,Services!$A$1:$B$45,2)),"",VLOOKUP(N9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P9,Services!$A$1:$B$45,2)),"",VLOOKUP(P9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R9" s="41"/>
+      <c r="S9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R9,Services!$A$1:$B$45,2)),"",VLOOKUP(R9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T9" s="41"/>
+      <c r="U9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T9,Services!$A$1:$B$45,2)),"",VLOOKUP(T9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V9" s="41"/>
+      <c r="W9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V9,Services!$A$1:$B$45,2)),"",VLOOKUP(V9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X9,Services!$A$1:$B$45,2)),"",VLOOKUP(X9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z9" s="41"/>
+      <c r="AA9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z9,Services!$A$1:$B$45,2)),"",VLOOKUP(Z9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB9" s="41"/>
+      <c r="AC9" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB9,Services!$A$1:$B$45,2)),"",VLOOKUP(AB9,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD9" s="41"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
@@ -8438,46 +8462,46 @@
       <c r="K10" s="41"/>
       <c r="L10" s="41"/>
       <c r="M10" s="41"/>
-      <c r="N10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M10,Services!$A$1:$B$45,2)),"",VLOOKUP(M10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O10" s="41"/>
-      <c r="P10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O10,Services!$A$1:$B$45,2)),"",VLOOKUP(O10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q10,Services!$A$1:$B$45,2)),"",VLOOKUP(Q10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S10" s="41"/>
-      <c r="T10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S10,Services!$A$1:$B$45,2)),"",VLOOKUP(S10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U10" s="41"/>
-      <c r="V10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U10,Services!$A$1:$B$45,2)),"",VLOOKUP(U10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W10" s="41"/>
-      <c r="X10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W10,Services!$A$1:$B$45,2)),"",VLOOKUP(W10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y10" s="41"/>
-      <c r="Z10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y10,Services!$A$1:$B$45,2)),"",VLOOKUP(Y10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA10" s="41"/>
-      <c r="AB10" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA10,Services!$A$1:$B$45,2)),"",VLOOKUP(AA10,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N10,Services!$A$1:$B$45,2)),"",VLOOKUP(N10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P10,Services!$A$1:$B$45,2)),"",VLOOKUP(P10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R10" s="41"/>
+      <c r="S10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R10,Services!$A$1:$B$45,2)),"",VLOOKUP(R10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T10" s="41"/>
+      <c r="U10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T10,Services!$A$1:$B$45,2)),"",VLOOKUP(T10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V10" s="41"/>
+      <c r="W10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V10,Services!$A$1:$B$45,2)),"",VLOOKUP(V10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X10,Services!$A$1:$B$45,2)),"",VLOOKUP(X10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z10" s="41"/>
+      <c r="AA10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z10,Services!$A$1:$B$45,2)),"",VLOOKUP(Z10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB10" s="41"/>
+      <c r="AC10" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB10,Services!$A$1:$B$45,2)),"",VLOOKUP(AB10,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD10" s="41"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
@@ -8503,46 +8527,46 @@
       <c r="K11" s="41"/>
       <c r="L11" s="41"/>
       <c r="M11" s="41"/>
-      <c r="N11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M11,Services!$A$1:$B$45,2)),"",VLOOKUP(M11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O11" s="41"/>
-      <c r="P11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O11,Services!$A$1:$B$45,2)),"",VLOOKUP(O11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q11,Services!$A$1:$B$45,2)),"",VLOOKUP(Q11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S11" s="41"/>
-      <c r="T11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S11,Services!$A$1:$B$45,2)),"",VLOOKUP(S11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U11" s="41"/>
-      <c r="V11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U11,Services!$A$1:$B$45,2)),"",VLOOKUP(U11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W11" s="41"/>
-      <c r="X11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W11,Services!$A$1:$B$45,2)),"",VLOOKUP(W11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y11" s="41"/>
-      <c r="Z11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y11,Services!$A$1:$B$45,2)),"",VLOOKUP(Y11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA11" s="41"/>
-      <c r="AB11" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA11,Services!$A$1:$B$45,2)),"",VLOOKUP(AA11,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N11,Services!$A$1:$B$45,2)),"",VLOOKUP(N11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P11,Services!$A$1:$B$45,2)),"",VLOOKUP(P11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R11" s="41"/>
+      <c r="S11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R11,Services!$A$1:$B$45,2)),"",VLOOKUP(R11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T11" s="41"/>
+      <c r="U11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T11,Services!$A$1:$B$45,2)),"",VLOOKUP(T11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V11" s="41"/>
+      <c r="W11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V11,Services!$A$1:$B$45,2)),"",VLOOKUP(V11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X11,Services!$A$1:$B$45,2)),"",VLOOKUP(X11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z11" s="41"/>
+      <c r="AA11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z11,Services!$A$1:$B$45,2)),"",VLOOKUP(Z11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB11" s="41"/>
+      <c r="AC11" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB11,Services!$A$1:$B$45,2)),"",VLOOKUP(AB11,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD11" s="41"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
@@ -8568,46 +8592,46 @@
       <c r="K12" s="41"/>
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
-      <c r="N12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M12,Services!$A$1:$B$45,2)),"",VLOOKUP(M12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O12" s="41"/>
-      <c r="P12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O12,Services!$A$1:$B$45,2)),"",VLOOKUP(O12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q12,Services!$A$1:$B$45,2)),"",VLOOKUP(Q12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S12" s="41"/>
-      <c r="T12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S12,Services!$A$1:$B$45,2)),"",VLOOKUP(S12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U12" s="41"/>
-      <c r="V12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U12,Services!$A$1:$B$45,2)),"",VLOOKUP(U12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W12" s="41"/>
-      <c r="X12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W12,Services!$A$1:$B$45,2)),"",VLOOKUP(W12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y12" s="41"/>
-      <c r="Z12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y12,Services!$A$1:$B$45,2)),"",VLOOKUP(Y12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA12" s="41"/>
-      <c r="AB12" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA12,Services!$A$1:$B$45,2)),"",VLOOKUP(AA12,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N12,Services!$A$1:$B$45,2)),"",VLOOKUP(N12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P12,Services!$A$1:$B$45,2)),"",VLOOKUP(P12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R12" s="41"/>
+      <c r="S12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R12,Services!$A$1:$B$45,2)),"",VLOOKUP(R12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T12" s="41"/>
+      <c r="U12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T12,Services!$A$1:$B$45,2)),"",VLOOKUP(T12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V12" s="41"/>
+      <c r="W12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V12,Services!$A$1:$B$45,2)),"",VLOOKUP(V12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X12,Services!$A$1:$B$45,2)),"",VLOOKUP(X12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z12" s="41"/>
+      <c r="AA12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z12,Services!$A$1:$B$45,2)),"",VLOOKUP(Z12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB12" s="41"/>
+      <c r="AC12" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB12,Services!$A$1:$B$45,2)),"",VLOOKUP(AB12,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD12" s="41"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
@@ -8633,46 +8657,46 @@
       <c r="K13" s="41"/>
       <c r="L13" s="41"/>
       <c r="M13" s="41"/>
-      <c r="N13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M13,Services!$A$1:$B$45,2)),"",VLOOKUP(M13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O13" s="41"/>
-      <c r="P13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O13,Services!$A$1:$B$45,2)),"",VLOOKUP(O13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q13,Services!$A$1:$B$45,2)),"",VLOOKUP(Q13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S13" s="41"/>
-      <c r="T13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S13,Services!$A$1:$B$45,2)),"",VLOOKUP(S13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U13" s="41"/>
-      <c r="V13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U13,Services!$A$1:$B$45,2)),"",VLOOKUP(U13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W13" s="41"/>
-      <c r="X13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W13,Services!$A$1:$B$45,2)),"",VLOOKUP(W13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y13" s="41"/>
-      <c r="Z13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y13,Services!$A$1:$B$45,2)),"",VLOOKUP(Y13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA13" s="41"/>
-      <c r="AB13" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA13,Services!$A$1:$B$45,2)),"",VLOOKUP(AA13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N13,Services!$A$1:$B$45,2)),"",VLOOKUP(N13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P13,Services!$A$1:$B$45,2)),"",VLOOKUP(P13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R13" s="41"/>
+      <c r="S13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R13,Services!$A$1:$B$45,2)),"",VLOOKUP(R13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T13" s="41"/>
+      <c r="U13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T13,Services!$A$1:$B$45,2)),"",VLOOKUP(T13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V13" s="41"/>
+      <c r="W13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V13,Services!$A$1:$B$45,2)),"",VLOOKUP(V13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X13,Services!$A$1:$B$45,2)),"",VLOOKUP(X13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z13" s="41"/>
+      <c r="AA13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z13,Services!$A$1:$B$45,2)),"",VLOOKUP(Z13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB13" s="41"/>
+      <c r="AC13" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB13,Services!$A$1:$B$45,2)),"",VLOOKUP(AB13,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD13" s="41"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
@@ -8698,46 +8722,46 @@
       <c r="K14" s="41"/>
       <c r="L14" s="41"/>
       <c r="M14" s="41"/>
-      <c r="N14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M14,Services!$A$1:$B$45,2)),"",VLOOKUP(M14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O14" s="41"/>
-      <c r="P14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O14,Services!$A$1:$B$45,2)),"",VLOOKUP(O14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q14,Services!$A$1:$B$45,2)),"",VLOOKUP(Q14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S14" s="41"/>
-      <c r="T14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S14,Services!$A$1:$B$45,2)),"",VLOOKUP(S14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U14" s="41"/>
-      <c r="V14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U14,Services!$A$1:$B$45,2)),"",VLOOKUP(U14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W14" s="41"/>
-      <c r="X14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W14,Services!$A$1:$B$45,2)),"",VLOOKUP(W14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y14" s="41"/>
-      <c r="Z14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y14,Services!$A$1:$B$45,2)),"",VLOOKUP(Y14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA14" s="41"/>
-      <c r="AB14" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA14,Services!$A$1:$B$45,2)),"",VLOOKUP(AA14,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N14,Services!$A$1:$B$45,2)),"",VLOOKUP(N14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P14,Services!$A$1:$B$45,2)),"",VLOOKUP(P14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R14" s="41"/>
+      <c r="S14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R14,Services!$A$1:$B$45,2)),"",VLOOKUP(R14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T14" s="41"/>
+      <c r="U14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T14,Services!$A$1:$B$45,2)),"",VLOOKUP(T14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V14" s="41"/>
+      <c r="W14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V14,Services!$A$1:$B$45,2)),"",VLOOKUP(V14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X14,Services!$A$1:$B$45,2)),"",VLOOKUP(X14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z14" s="41"/>
+      <c r="AA14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z14,Services!$A$1:$B$45,2)),"",VLOOKUP(Z14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB14" s="41"/>
+      <c r="AC14" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB14,Services!$A$1:$B$45,2)),"",VLOOKUP(AB14,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD14" s="41"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
@@ -8763,46 +8787,46 @@
       <c r="K15" s="41"/>
       <c r="L15" s="41"/>
       <c r="M15" s="41"/>
-      <c r="N15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M15,Services!$A$1:$B$45,2)),"",VLOOKUP(M15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O15" s="41"/>
-      <c r="P15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O15,Services!$A$1:$B$45,2)),"",VLOOKUP(O15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q15,Services!$A$1:$B$45,2)),"",VLOOKUP(Q15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S15" s="41"/>
-      <c r="T15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S15,Services!$A$1:$B$45,2)),"",VLOOKUP(S15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U15" s="41"/>
-      <c r="V15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U15,Services!$A$1:$B$45,2)),"",VLOOKUP(U15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W15" s="41"/>
-      <c r="X15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W15,Services!$A$1:$B$45,2)),"",VLOOKUP(W15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y15" s="41"/>
-      <c r="Z15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y15,Services!$A$1:$B$45,2)),"",VLOOKUP(Y15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA15" s="41"/>
-      <c r="AB15" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA15,Services!$A$1:$B$45,2)),"",VLOOKUP(AA15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N15,Services!$A$1:$B$45,2)),"",VLOOKUP(N15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P15,Services!$A$1:$B$45,2)),"",VLOOKUP(P15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R15" s="41"/>
+      <c r="S15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R15,Services!$A$1:$B$45,2)),"",VLOOKUP(R15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T15" s="41"/>
+      <c r="U15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T15,Services!$A$1:$B$45,2)),"",VLOOKUP(T15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V15" s="41"/>
+      <c r="W15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V15,Services!$A$1:$B$45,2)),"",VLOOKUP(V15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X15" s="41"/>
+      <c r="Y15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X15,Services!$A$1:$B$45,2)),"",VLOOKUP(X15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z15" s="41"/>
+      <c r="AA15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z15,Services!$A$1:$B$45,2)),"",VLOOKUP(Z15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB15" s="41"/>
+      <c r="AC15" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB15,Services!$A$1:$B$45,2)),"",VLOOKUP(AB15,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD15" s="41"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
@@ -8828,46 +8852,46 @@
       <c r="K16" s="41"/>
       <c r="L16" s="41"/>
       <c r="M16" s="41"/>
-      <c r="N16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M16,Services!$A$1:$B$45,2)),"",VLOOKUP(M16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O16" s="41"/>
-      <c r="P16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O16,Services!$A$1:$B$45,2)),"",VLOOKUP(O16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q16" s="41"/>
-      <c r="R16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q16,Services!$A$1:$B$45,2)),"",VLOOKUP(Q16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S16" s="41"/>
-      <c r="T16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S16,Services!$A$1:$B$45,2)),"",VLOOKUP(S16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U16" s="41"/>
-      <c r="V16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U16,Services!$A$1:$B$45,2)),"",VLOOKUP(U16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W16" s="41"/>
-      <c r="X16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W16,Services!$A$1:$B$45,2)),"",VLOOKUP(W16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y16" s="41"/>
-      <c r="Z16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y16,Services!$A$1:$B$45,2)),"",VLOOKUP(Y16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA16" s="41"/>
-      <c r="AB16" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA16,Services!$A$1:$B$45,2)),"",VLOOKUP(AA16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N16,Services!$A$1:$B$45,2)),"",VLOOKUP(N16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P16,Services!$A$1:$B$45,2)),"",VLOOKUP(P16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R16" s="41"/>
+      <c r="S16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R16,Services!$A$1:$B$45,2)),"",VLOOKUP(R16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T16" s="41"/>
+      <c r="U16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T16,Services!$A$1:$B$45,2)),"",VLOOKUP(T16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V16" s="41"/>
+      <c r="W16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V16,Services!$A$1:$B$45,2)),"",VLOOKUP(V16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X16" s="41"/>
+      <c r="Y16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X16,Services!$A$1:$B$45,2)),"",VLOOKUP(X16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z16" s="41"/>
+      <c r="AA16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z16,Services!$A$1:$B$45,2)),"",VLOOKUP(Z16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB16" s="41"/>
+      <c r="AC16" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB16,Services!$A$1:$B$45,2)),"",VLOOKUP(AB16,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD16" s="41"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
@@ -8893,46 +8917,46 @@
       <c r="K17" s="41"/>
       <c r="L17" s="41"/>
       <c r="M17" s="41"/>
-      <c r="N17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M17,Services!$A$1:$B$45,2)),"",VLOOKUP(M17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O17" s="41"/>
-      <c r="P17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O17,Services!$A$1:$B$45,2)),"",VLOOKUP(O17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q17,Services!$A$1:$B$45,2)),"",VLOOKUP(Q17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S17" s="41"/>
-      <c r="T17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S17,Services!$A$1:$B$45,2)),"",VLOOKUP(S17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U17" s="41"/>
-      <c r="V17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U17,Services!$A$1:$B$45,2)),"",VLOOKUP(U17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W17" s="41"/>
-      <c r="X17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W17,Services!$A$1:$B$45,2)),"",VLOOKUP(W17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y17" s="41"/>
-      <c r="Z17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y17,Services!$A$1:$B$45,2)),"",VLOOKUP(Y17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA17" s="41"/>
-      <c r="AB17" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA17,Services!$A$1:$B$45,2)),"",VLOOKUP(AA17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N17,Services!$A$1:$B$45,2)),"",VLOOKUP(N17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P17,Services!$A$1:$B$45,2)),"",VLOOKUP(P17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R17" s="41"/>
+      <c r="S17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R17,Services!$A$1:$B$45,2)),"",VLOOKUP(R17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T17" s="41"/>
+      <c r="U17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T17,Services!$A$1:$B$45,2)),"",VLOOKUP(T17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V17" s="41"/>
+      <c r="W17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V17,Services!$A$1:$B$45,2)),"",VLOOKUP(V17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X17" s="41"/>
+      <c r="Y17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X17,Services!$A$1:$B$45,2)),"",VLOOKUP(X17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z17" s="41"/>
+      <c r="AA17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z17,Services!$A$1:$B$45,2)),"",VLOOKUP(Z17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB17" s="41"/>
+      <c r="AC17" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB17,Services!$A$1:$B$45,2)),"",VLOOKUP(AB17,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD17" s="41"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
@@ -8958,46 +8982,46 @@
       <c r="K18" s="41"/>
       <c r="L18" s="41"/>
       <c r="M18" s="41"/>
-      <c r="N18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M18,Services!$A$1:$B$45,2)),"",VLOOKUP(M18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O18" s="41"/>
-      <c r="P18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O18,Services!$A$1:$B$45,2)),"",VLOOKUP(O18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q18,Services!$A$1:$B$45,2)),"",VLOOKUP(Q18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S18" s="41"/>
-      <c r="T18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S18,Services!$A$1:$B$45,2)),"",VLOOKUP(S18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U18" s="41"/>
-      <c r="V18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U18,Services!$A$1:$B$45,2)),"",VLOOKUP(U18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W18" s="41"/>
-      <c r="X18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W18,Services!$A$1:$B$45,2)),"",VLOOKUP(W18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y18" s="41"/>
-      <c r="Z18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y18,Services!$A$1:$B$45,2)),"",VLOOKUP(Y18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA18" s="41"/>
-      <c r="AB18" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA18,Services!$A$1:$B$45,2)),"",VLOOKUP(AA18,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N18,Services!$A$1:$B$45,2)),"",VLOOKUP(N18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P18,Services!$A$1:$B$45,2)),"",VLOOKUP(P18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R18" s="41"/>
+      <c r="S18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R18,Services!$A$1:$B$45,2)),"",VLOOKUP(R18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T18" s="41"/>
+      <c r="U18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T18,Services!$A$1:$B$45,2)),"",VLOOKUP(T18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V18" s="41"/>
+      <c r="W18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V18,Services!$A$1:$B$45,2)),"",VLOOKUP(V18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X18" s="41"/>
+      <c r="Y18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X18,Services!$A$1:$B$45,2)),"",VLOOKUP(X18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z18" s="41"/>
+      <c r="AA18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z18,Services!$A$1:$B$45,2)),"",VLOOKUP(Z18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB18" s="41"/>
+      <c r="AC18" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB18,Services!$A$1:$B$45,2)),"",VLOOKUP(AB18,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD18" s="41"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
@@ -9023,46 +9047,46 @@
       <c r="K19" s="41"/>
       <c r="L19" s="41"/>
       <c r="M19" s="41"/>
-      <c r="N19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M19,Services!$A$1:$B$45,2)),"",VLOOKUP(M19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O19" s="41"/>
-      <c r="P19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O19,Services!$A$1:$B$45,2)),"",VLOOKUP(O19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q19" s="41"/>
-      <c r="R19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q19,Services!$A$1:$B$45,2)),"",VLOOKUP(Q19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S19" s="41"/>
-      <c r="T19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S19,Services!$A$1:$B$45,2)),"",VLOOKUP(S19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U19" s="41"/>
-      <c r="V19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U19,Services!$A$1:$B$45,2)),"",VLOOKUP(U19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W19" s="41"/>
-      <c r="X19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W19,Services!$A$1:$B$45,2)),"",VLOOKUP(W19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y19" s="41"/>
-      <c r="Z19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y19,Services!$A$1:$B$45,2)),"",VLOOKUP(Y19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA19" s="41"/>
-      <c r="AB19" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA19,Services!$A$1:$B$45,2)),"",VLOOKUP(AA19,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N19,Services!$A$1:$B$45,2)),"",VLOOKUP(N19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P19,Services!$A$1:$B$45,2)),"",VLOOKUP(P19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R19" s="41"/>
+      <c r="S19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R19,Services!$A$1:$B$45,2)),"",VLOOKUP(R19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T19" s="41"/>
+      <c r="U19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T19,Services!$A$1:$B$45,2)),"",VLOOKUP(T19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V19" s="41"/>
+      <c r="W19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V19,Services!$A$1:$B$45,2)),"",VLOOKUP(V19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X19" s="41"/>
+      <c r="Y19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X19,Services!$A$1:$B$45,2)),"",VLOOKUP(X19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z19" s="41"/>
+      <c r="AA19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z19,Services!$A$1:$B$45,2)),"",VLOOKUP(Z19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB19" s="41"/>
+      <c r="AC19" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB19,Services!$A$1:$B$45,2)),"",VLOOKUP(AB19,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD19" s="41"/>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
@@ -9088,46 +9112,46 @@
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
       <c r="M20" s="41"/>
-      <c r="N20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M20,Services!$A$1:$B$45,2)),"",VLOOKUP(M20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O20" s="41"/>
-      <c r="P20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O20,Services!$A$1:$B$45,2)),"",VLOOKUP(O20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q20" s="41"/>
-      <c r="R20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q20,Services!$A$1:$B$45,2)),"",VLOOKUP(Q20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S20" s="41"/>
-      <c r="T20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S20,Services!$A$1:$B$45,2)),"",VLOOKUP(S20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U20" s="41"/>
-      <c r="V20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U20,Services!$A$1:$B$45,2)),"",VLOOKUP(U20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W20" s="41"/>
-      <c r="X20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W20,Services!$A$1:$B$45,2)),"",VLOOKUP(W20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y20" s="41"/>
-      <c r="Z20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y20,Services!$A$1:$B$45,2)),"",VLOOKUP(Y20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA20" s="41"/>
-      <c r="AB20" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA20,Services!$A$1:$B$45,2)),"",VLOOKUP(AA20,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N20,Services!$A$1:$B$45,2)),"",VLOOKUP(N20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P20,Services!$A$1:$B$45,2)),"",VLOOKUP(P20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R20" s="41"/>
+      <c r="S20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R20,Services!$A$1:$B$45,2)),"",VLOOKUP(R20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T20" s="41"/>
+      <c r="U20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T20,Services!$A$1:$B$45,2)),"",VLOOKUP(T20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V20" s="41"/>
+      <c r="W20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V20,Services!$A$1:$B$45,2)),"",VLOOKUP(V20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X20" s="41"/>
+      <c r="Y20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X20,Services!$A$1:$B$45,2)),"",VLOOKUP(X20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z20" s="41"/>
+      <c r="AA20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z20,Services!$A$1:$B$45,2)),"",VLOOKUP(Z20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB20" s="41"/>
+      <c r="AC20" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB20,Services!$A$1:$B$45,2)),"",VLOOKUP(AB20,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD20" s="41"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
@@ -9153,46 +9177,46 @@
       <c r="K21" s="41"/>
       <c r="L21" s="41"/>
       <c r="M21" s="41"/>
-      <c r="N21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M21,Services!$A$1:$B$45,2)),"",VLOOKUP(M21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O21" s="41"/>
-      <c r="P21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O21,Services!$A$1:$B$45,2)),"",VLOOKUP(O21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q21,Services!$A$1:$B$45,2)),"",VLOOKUP(Q21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S21" s="41"/>
-      <c r="T21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S21,Services!$A$1:$B$45,2)),"",VLOOKUP(S21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U21" s="41"/>
-      <c r="V21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U21,Services!$A$1:$B$45,2)),"",VLOOKUP(U21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W21" s="41"/>
-      <c r="X21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W21,Services!$A$1:$B$45,2)),"",VLOOKUP(W21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y21" s="41"/>
-      <c r="Z21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y21,Services!$A$1:$B$45,2)),"",VLOOKUP(Y21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA21" s="41"/>
-      <c r="AB21" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA21,Services!$A$1:$B$45,2)),"",VLOOKUP(AA21,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N21,Services!$A$1:$B$45,2)),"",VLOOKUP(N21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P21,Services!$A$1:$B$45,2)),"",VLOOKUP(P21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R21" s="41"/>
+      <c r="S21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R21,Services!$A$1:$B$45,2)),"",VLOOKUP(R21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T21" s="41"/>
+      <c r="U21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T21,Services!$A$1:$B$45,2)),"",VLOOKUP(T21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V21" s="41"/>
+      <c r="W21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V21,Services!$A$1:$B$45,2)),"",VLOOKUP(V21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X21" s="41"/>
+      <c r="Y21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X21,Services!$A$1:$B$45,2)),"",VLOOKUP(X21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z21" s="41"/>
+      <c r="AA21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z21,Services!$A$1:$B$45,2)),"",VLOOKUP(Z21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB21" s="41"/>
+      <c r="AC21" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB21,Services!$A$1:$B$45,2)),"",VLOOKUP(AB21,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD21" s="41"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
@@ -9218,46 +9242,46 @@
       <c r="K22" s="41"/>
       <c r="L22" s="41"/>
       <c r="M22" s="41"/>
-      <c r="N22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M22,Services!$A$1:$B$45,2)),"",VLOOKUP(M22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O22" s="41"/>
-      <c r="P22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O22,Services!$A$1:$B$45,2)),"",VLOOKUP(O22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q22,Services!$A$1:$B$45,2)),"",VLOOKUP(Q22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S22" s="41"/>
-      <c r="T22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S22,Services!$A$1:$B$45,2)),"",VLOOKUP(S22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U22" s="41"/>
-      <c r="V22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U22,Services!$A$1:$B$45,2)),"",VLOOKUP(U22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W22" s="41"/>
-      <c r="X22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W22,Services!$A$1:$B$45,2)),"",VLOOKUP(W22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y22" s="41"/>
-      <c r="Z22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y22,Services!$A$1:$B$45,2)),"",VLOOKUP(Y22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA22" s="41"/>
-      <c r="AB22" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA22,Services!$A$1:$B$45,2)),"",VLOOKUP(AA22,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N22,Services!$A$1:$B$45,2)),"",VLOOKUP(N22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P22" s="41"/>
+      <c r="Q22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P22,Services!$A$1:$B$45,2)),"",VLOOKUP(P22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R22" s="41"/>
+      <c r="S22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R22,Services!$A$1:$B$45,2)),"",VLOOKUP(R22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T22" s="41"/>
+      <c r="U22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T22,Services!$A$1:$B$45,2)),"",VLOOKUP(T22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V22" s="41"/>
+      <c r="W22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V22,Services!$A$1:$B$45,2)),"",VLOOKUP(V22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X22" s="41"/>
+      <c r="Y22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X22,Services!$A$1:$B$45,2)),"",VLOOKUP(X22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z22" s="41"/>
+      <c r="AA22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z22,Services!$A$1:$B$45,2)),"",VLOOKUP(Z22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB22" s="41"/>
+      <c r="AC22" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB22,Services!$A$1:$B$45,2)),"",VLOOKUP(AB22,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD22" s="41"/>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
@@ -9283,46 +9307,46 @@
       <c r="K23" s="41"/>
       <c r="L23" s="41"/>
       <c r="M23" s="41"/>
-      <c r="N23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M23,Services!$A$1:$B$45,2)),"",VLOOKUP(M23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O23" s="41"/>
-      <c r="P23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O23,Services!$A$1:$B$45,2)),"",VLOOKUP(O23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q23,Services!$A$1:$B$45,2)),"",VLOOKUP(Q23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S23" s="41"/>
-      <c r="T23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S23,Services!$A$1:$B$45,2)),"",VLOOKUP(S23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U23" s="41"/>
-      <c r="V23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U23,Services!$A$1:$B$45,2)),"",VLOOKUP(U23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W23" s="41"/>
-      <c r="X23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W23,Services!$A$1:$B$45,2)),"",VLOOKUP(W23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y23" s="41"/>
-      <c r="Z23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y23,Services!$A$1:$B$45,2)),"",VLOOKUP(Y23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA23" s="41"/>
-      <c r="AB23" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA23,Services!$A$1:$B$45,2)),"",VLOOKUP(AA23,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N23,Services!$A$1:$B$45,2)),"",VLOOKUP(N23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P23,Services!$A$1:$B$45,2)),"",VLOOKUP(P23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R23" s="41"/>
+      <c r="S23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R23,Services!$A$1:$B$45,2)),"",VLOOKUP(R23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T23" s="41"/>
+      <c r="U23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T23,Services!$A$1:$B$45,2)),"",VLOOKUP(T23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V23" s="41"/>
+      <c r="W23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V23,Services!$A$1:$B$45,2)),"",VLOOKUP(V23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X23" s="41"/>
+      <c r="Y23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X23,Services!$A$1:$B$45,2)),"",VLOOKUP(X23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z23" s="41"/>
+      <c r="AA23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z23,Services!$A$1:$B$45,2)),"",VLOOKUP(Z23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB23" s="41"/>
+      <c r="AC23" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB23,Services!$A$1:$B$45,2)),"",VLOOKUP(AB23,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD23" s="41"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
@@ -9348,46 +9372,46 @@
       <c r="K24" s="41"/>
       <c r="L24" s="41"/>
       <c r="M24" s="41"/>
-      <c r="N24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M24,Services!$A$1:$B$45,2)),"",VLOOKUP(M24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O24" s="41"/>
-      <c r="P24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O24,Services!$A$1:$B$45,2)),"",VLOOKUP(O24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q24" s="41"/>
-      <c r="R24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q24,Services!$A$1:$B$45,2)),"",VLOOKUP(Q24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S24" s="41"/>
-      <c r="T24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S24,Services!$A$1:$B$45,2)),"",VLOOKUP(S24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U24" s="41"/>
-      <c r="V24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U24,Services!$A$1:$B$45,2)),"",VLOOKUP(U24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W24" s="41"/>
-      <c r="X24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W24,Services!$A$1:$B$45,2)),"",VLOOKUP(W24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y24" s="41"/>
-      <c r="Z24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y24,Services!$A$1:$B$45,2)),"",VLOOKUP(Y24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA24" s="41"/>
-      <c r="AB24" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA24,Services!$A$1:$B$45,2)),"",VLOOKUP(AA24,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N24,Services!$A$1:$B$45,2)),"",VLOOKUP(N24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P24,Services!$A$1:$B$45,2)),"",VLOOKUP(P24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R24" s="41"/>
+      <c r="S24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R24,Services!$A$1:$B$45,2)),"",VLOOKUP(R24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T24" s="41"/>
+      <c r="U24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T24,Services!$A$1:$B$45,2)),"",VLOOKUP(T24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V24" s="41"/>
+      <c r="W24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V24,Services!$A$1:$B$45,2)),"",VLOOKUP(V24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X24" s="41"/>
+      <c r="Y24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X24,Services!$A$1:$B$45,2)),"",VLOOKUP(X24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z24" s="41"/>
+      <c r="AA24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z24,Services!$A$1:$B$45,2)),"",VLOOKUP(Z24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB24" s="41"/>
+      <c r="AC24" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB24,Services!$A$1:$B$45,2)),"",VLOOKUP(AB24,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD24" s="41"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
@@ -9413,46 +9437,46 @@
       <c r="K25" s="41"/>
       <c r="L25" s="41"/>
       <c r="M25" s="41"/>
-      <c r="N25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M25,Services!$A$1:$B$45,2)),"",VLOOKUP(M25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O25" s="41"/>
-      <c r="P25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O25,Services!$A$1:$B$45,2)),"",VLOOKUP(O25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q25,Services!$A$1:$B$45,2)),"",VLOOKUP(Q25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S25" s="41"/>
-      <c r="T25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S25,Services!$A$1:$B$45,2)),"",VLOOKUP(S25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U25" s="41"/>
-      <c r="V25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U25,Services!$A$1:$B$45,2)),"",VLOOKUP(U25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W25" s="41"/>
-      <c r="X25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W25,Services!$A$1:$B$45,2)),"",VLOOKUP(W25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y25" s="41"/>
-      <c r="Z25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y25,Services!$A$1:$B$45,2)),"",VLOOKUP(Y25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA25" s="41"/>
-      <c r="AB25" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA25,Services!$A$1:$B$45,2)),"",VLOOKUP(AA25,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N25,Services!$A$1:$B$45,2)),"",VLOOKUP(N25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P25,Services!$A$1:$B$45,2)),"",VLOOKUP(P25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R25" s="41"/>
+      <c r="S25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R25,Services!$A$1:$B$45,2)),"",VLOOKUP(R25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T25" s="41"/>
+      <c r="U25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T25,Services!$A$1:$B$45,2)),"",VLOOKUP(T25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V25" s="41"/>
+      <c r="W25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V25,Services!$A$1:$B$45,2)),"",VLOOKUP(V25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X25" s="41"/>
+      <c r="Y25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X25,Services!$A$1:$B$45,2)),"",VLOOKUP(X25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z25" s="41"/>
+      <c r="AA25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z25,Services!$A$1:$B$45,2)),"",VLOOKUP(Z25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB25" s="41"/>
+      <c r="AC25" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB25,Services!$A$1:$B$45,2)),"",VLOOKUP(AB25,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD25" s="41"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
@@ -9478,46 +9502,46 @@
       <c r="K26" s="41"/>
       <c r="L26" s="41"/>
       <c r="M26" s="41"/>
-      <c r="N26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M26,Services!$A$1:$B$45,2)),"",VLOOKUP(M26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O26" s="41"/>
-      <c r="P26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O26,Services!$A$1:$B$45,2)),"",VLOOKUP(O26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q26" s="41"/>
-      <c r="R26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q26,Services!$A$1:$B$45,2)),"",VLOOKUP(Q26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S26" s="41"/>
-      <c r="T26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S26,Services!$A$1:$B$45,2)),"",VLOOKUP(S26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U26" s="41"/>
-      <c r="V26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U26,Services!$A$1:$B$45,2)),"",VLOOKUP(U26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W26" s="41"/>
-      <c r="X26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W26,Services!$A$1:$B$45,2)),"",VLOOKUP(W26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y26" s="41"/>
-      <c r="Z26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y26,Services!$A$1:$B$45,2)),"",VLOOKUP(Y26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA26" s="41"/>
-      <c r="AB26" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA26,Services!$A$1:$B$45,2)),"",VLOOKUP(AA26,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N26,Services!$A$1:$B$45,2)),"",VLOOKUP(N26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P26" s="41"/>
+      <c r="Q26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P26,Services!$A$1:$B$45,2)),"",VLOOKUP(P26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R26" s="41"/>
+      <c r="S26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R26,Services!$A$1:$B$45,2)),"",VLOOKUP(R26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T26" s="41"/>
+      <c r="U26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T26,Services!$A$1:$B$45,2)),"",VLOOKUP(T26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V26" s="41"/>
+      <c r="W26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V26,Services!$A$1:$B$45,2)),"",VLOOKUP(V26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X26" s="41"/>
+      <c r="Y26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X26,Services!$A$1:$B$45,2)),"",VLOOKUP(X26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z26" s="41"/>
+      <c r="AA26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z26,Services!$A$1:$B$45,2)),"",VLOOKUP(Z26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB26" s="41"/>
+      <c r="AC26" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB26,Services!$A$1:$B$45,2)),"",VLOOKUP(AB26,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD26" s="41"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
@@ -9543,46 +9567,46 @@
       <c r="K27" s="41"/>
       <c r="L27" s="41"/>
       <c r="M27" s="41"/>
-      <c r="N27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M27,Services!$A$1:$B$45,2)),"",VLOOKUP(M27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O27" s="41"/>
-      <c r="P27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O27,Services!$A$1:$B$45,2)),"",VLOOKUP(O27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q27" s="41"/>
-      <c r="R27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q27,Services!$A$1:$B$45,2)),"",VLOOKUP(Q27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S27" s="41"/>
-      <c r="T27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S27,Services!$A$1:$B$45,2)),"",VLOOKUP(S27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U27" s="41"/>
-      <c r="V27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U27,Services!$A$1:$B$45,2)),"",VLOOKUP(U27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W27" s="41"/>
-      <c r="X27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W27,Services!$A$1:$B$45,2)),"",VLOOKUP(W27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y27" s="41"/>
-      <c r="Z27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y27,Services!$A$1:$B$45,2)),"",VLOOKUP(Y27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA27" s="41"/>
-      <c r="AB27" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA27,Services!$A$1:$B$45,2)),"",VLOOKUP(AA27,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N27,Services!$A$1:$B$45,2)),"",VLOOKUP(N27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P27,Services!$A$1:$B$45,2)),"",VLOOKUP(P27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R27" s="41"/>
+      <c r="S27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R27,Services!$A$1:$B$45,2)),"",VLOOKUP(R27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T27" s="41"/>
+      <c r="U27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T27,Services!$A$1:$B$45,2)),"",VLOOKUP(T27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V27" s="41"/>
+      <c r="W27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V27,Services!$A$1:$B$45,2)),"",VLOOKUP(V27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X27,Services!$A$1:$B$45,2)),"",VLOOKUP(X27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z27" s="41"/>
+      <c r="AA27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z27,Services!$A$1:$B$45,2)),"",VLOOKUP(Z27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB27" s="41"/>
+      <c r="AC27" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB27,Services!$A$1:$B$45,2)),"",VLOOKUP(AB27,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD27" s="41"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
@@ -9608,46 +9632,46 @@
       <c r="K28" s="41"/>
       <c r="L28" s="41"/>
       <c r="M28" s="41"/>
-      <c r="N28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M28,Services!$A$1:$B$45,2)),"",VLOOKUP(M28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O28" s="41"/>
-      <c r="P28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O28,Services!$A$1:$B$45,2)),"",VLOOKUP(O28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q28" s="41"/>
-      <c r="R28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q28,Services!$A$1:$B$45,2)),"",VLOOKUP(Q28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S28" s="41"/>
-      <c r="T28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S28,Services!$A$1:$B$45,2)),"",VLOOKUP(S28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U28" s="41"/>
-      <c r="V28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U28,Services!$A$1:$B$45,2)),"",VLOOKUP(U28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W28" s="41"/>
-      <c r="X28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W28,Services!$A$1:$B$45,2)),"",VLOOKUP(W28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y28" s="41"/>
-      <c r="Z28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y28,Services!$A$1:$B$45,2)),"",VLOOKUP(Y28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA28" s="41"/>
-      <c r="AB28" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA28,Services!$A$1:$B$45,2)),"",VLOOKUP(AA28,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N28,Services!$A$1:$B$45,2)),"",VLOOKUP(N28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P28,Services!$A$1:$B$45,2)),"",VLOOKUP(P28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R28" s="41"/>
+      <c r="S28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R28,Services!$A$1:$B$45,2)),"",VLOOKUP(R28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T28" s="41"/>
+      <c r="U28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T28,Services!$A$1:$B$45,2)),"",VLOOKUP(T28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V28" s="41"/>
+      <c r="W28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V28,Services!$A$1:$B$45,2)),"",VLOOKUP(V28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X28" s="41"/>
+      <c r="Y28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X28,Services!$A$1:$B$45,2)),"",VLOOKUP(X28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z28" s="41"/>
+      <c r="AA28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z28,Services!$A$1:$B$45,2)),"",VLOOKUP(Z28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB28" s="41"/>
+      <c r="AC28" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB28,Services!$A$1:$B$45,2)),"",VLOOKUP(AB28,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD28" s="41"/>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
@@ -9673,46 +9697,46 @@
       <c r="K29" s="41"/>
       <c r="L29" s="41"/>
       <c r="M29" s="41"/>
-      <c r="N29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M29,Services!$A$1:$B$45,2)),"",VLOOKUP(M29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O29" s="41"/>
-      <c r="P29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O29,Services!$A$1:$B$45,2)),"",VLOOKUP(O29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q29" s="41"/>
-      <c r="R29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q29,Services!$A$1:$B$45,2)),"",VLOOKUP(Q29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S29" s="41"/>
-      <c r="T29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S29,Services!$A$1:$B$45,2)),"",VLOOKUP(S29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U29" s="41"/>
-      <c r="V29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U29,Services!$A$1:$B$45,2)),"",VLOOKUP(U29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W29" s="41"/>
-      <c r="X29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W29,Services!$A$1:$B$45,2)),"",VLOOKUP(W29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y29" s="41"/>
-      <c r="Z29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y29,Services!$A$1:$B$45,2)),"",VLOOKUP(Y29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA29" s="41"/>
-      <c r="AB29" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA29,Services!$A$1:$B$45,2)),"",VLOOKUP(AA29,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N29,Services!$A$1:$B$45,2)),"",VLOOKUP(N29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P29,Services!$A$1:$B$45,2)),"",VLOOKUP(P29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R29" s="41"/>
+      <c r="S29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R29,Services!$A$1:$B$45,2)),"",VLOOKUP(R29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T29" s="41"/>
+      <c r="U29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T29,Services!$A$1:$B$45,2)),"",VLOOKUP(T29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V29" s="41"/>
+      <c r="W29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V29,Services!$A$1:$B$45,2)),"",VLOOKUP(V29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X29" s="41"/>
+      <c r="Y29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X29,Services!$A$1:$B$45,2)),"",VLOOKUP(X29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z29" s="41"/>
+      <c r="AA29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z29,Services!$A$1:$B$45,2)),"",VLOOKUP(Z29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB29" s="41"/>
+      <c r="AC29" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB29,Services!$A$1:$B$45,2)),"",VLOOKUP(AB29,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD29" s="41"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
@@ -9738,46 +9762,46 @@
       <c r="K30" s="41"/>
       <c r="L30" s="41"/>
       <c r="M30" s="41"/>
-      <c r="N30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M30,Services!$A$1:$B$45,2)),"",VLOOKUP(M30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O30" s="41"/>
-      <c r="P30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O30,Services!$A$1:$B$45,2)),"",VLOOKUP(O30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q30" s="41"/>
-      <c r="R30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q30,Services!$A$1:$B$45,2)),"",VLOOKUP(Q30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S30" s="41"/>
-      <c r="T30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S30,Services!$A$1:$B$45,2)),"",VLOOKUP(S30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U30" s="41"/>
-      <c r="V30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U30,Services!$A$1:$B$45,2)),"",VLOOKUP(U30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W30" s="41"/>
-      <c r="X30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W30,Services!$A$1:$B$45,2)),"",VLOOKUP(W30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y30" s="41"/>
-      <c r="Z30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y30,Services!$A$1:$B$45,2)),"",VLOOKUP(Y30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA30" s="41"/>
-      <c r="AB30" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA30,Services!$A$1:$B$45,2)),"",VLOOKUP(AA30,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N30,Services!$A$1:$B$45,2)),"",VLOOKUP(N30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P30,Services!$A$1:$B$45,2)),"",VLOOKUP(P30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R30" s="41"/>
+      <c r="S30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R30,Services!$A$1:$B$45,2)),"",VLOOKUP(R30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T30" s="41"/>
+      <c r="U30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T30,Services!$A$1:$B$45,2)),"",VLOOKUP(T30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V30" s="41"/>
+      <c r="W30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V30,Services!$A$1:$B$45,2)),"",VLOOKUP(V30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X30" s="41"/>
+      <c r="Y30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X30,Services!$A$1:$B$45,2)),"",VLOOKUP(X30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z30" s="41"/>
+      <c r="AA30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z30,Services!$A$1:$B$45,2)),"",VLOOKUP(Z30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB30" s="41"/>
+      <c r="AC30" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB30,Services!$A$1:$B$45,2)),"",VLOOKUP(AB30,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD30" s="41"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
@@ -9803,46 +9827,46 @@
       <c r="K31" s="41"/>
       <c r="L31" s="41"/>
       <c r="M31" s="41"/>
-      <c r="N31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M31,Services!$A$1:$B$45,2)),"",VLOOKUP(M31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O31" s="41"/>
-      <c r="P31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O31,Services!$A$1:$B$45,2)),"",VLOOKUP(O31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q31" s="41"/>
-      <c r="R31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q31,Services!$A$1:$B$45,2)),"",VLOOKUP(Q31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S31" s="41"/>
-      <c r="T31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S31,Services!$A$1:$B$45,2)),"",VLOOKUP(S31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U31" s="41"/>
-      <c r="V31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U31,Services!$A$1:$B$45,2)),"",VLOOKUP(U31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W31" s="41"/>
-      <c r="X31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W31,Services!$A$1:$B$45,2)),"",VLOOKUP(W31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y31" s="41"/>
-      <c r="Z31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y31,Services!$A$1:$B$45,2)),"",VLOOKUP(Y31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA31" s="41"/>
-      <c r="AB31" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA31,Services!$A$1:$B$45,2)),"",VLOOKUP(AA31,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N31,Services!$A$1:$B$45,2)),"",VLOOKUP(N31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P31,Services!$A$1:$B$45,2)),"",VLOOKUP(P31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R31" s="41"/>
+      <c r="S31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R31,Services!$A$1:$B$45,2)),"",VLOOKUP(R31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T31" s="41"/>
+      <c r="U31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T31,Services!$A$1:$B$45,2)),"",VLOOKUP(T31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V31" s="41"/>
+      <c r="W31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V31,Services!$A$1:$B$45,2)),"",VLOOKUP(V31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X31" s="41"/>
+      <c r="Y31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X31,Services!$A$1:$B$45,2)),"",VLOOKUP(X31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z31" s="41"/>
+      <c r="AA31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z31,Services!$A$1:$B$45,2)),"",VLOOKUP(Z31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB31" s="41"/>
+      <c r="AC31" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB31,Services!$A$1:$B$45,2)),"",VLOOKUP(AB31,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD31" s="41"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
@@ -9868,46 +9892,46 @@
       <c r="K32" s="41"/>
       <c r="L32" s="41"/>
       <c r="M32" s="41"/>
-      <c r="N32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M32,Services!$A$1:$B$45,2)),"",VLOOKUP(M32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O32" s="41"/>
-      <c r="P32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O32,Services!$A$1:$B$45,2)),"",VLOOKUP(O32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q32" s="41"/>
-      <c r="R32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q32,Services!$A$1:$B$45,2)),"",VLOOKUP(Q32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S32" s="41"/>
-      <c r="T32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S32,Services!$A$1:$B$45,2)),"",VLOOKUP(S32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U32" s="41"/>
-      <c r="V32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U32,Services!$A$1:$B$45,2)),"",VLOOKUP(U32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W32" s="41"/>
-      <c r="X32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W32,Services!$A$1:$B$45,2)),"",VLOOKUP(W32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y32" s="41"/>
-      <c r="Z32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y32,Services!$A$1:$B$45,2)),"",VLOOKUP(Y32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA32" s="41"/>
-      <c r="AB32" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA32,Services!$A$1:$B$45,2)),"",VLOOKUP(AA32,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC32" s="41"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N32,Services!$A$1:$B$45,2)),"",VLOOKUP(N32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P32,Services!$A$1:$B$45,2)),"",VLOOKUP(P32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R32" s="41"/>
+      <c r="S32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R32,Services!$A$1:$B$45,2)),"",VLOOKUP(R32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T32" s="41"/>
+      <c r="U32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T32,Services!$A$1:$B$45,2)),"",VLOOKUP(T32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V32" s="41"/>
+      <c r="W32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V32,Services!$A$1:$B$45,2)),"",VLOOKUP(V32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X32" s="41"/>
+      <c r="Y32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X32,Services!$A$1:$B$45,2)),"",VLOOKUP(X32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z32" s="41"/>
+      <c r="AA32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z32,Services!$A$1:$B$45,2)),"",VLOOKUP(Z32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB32" s="41"/>
+      <c r="AC32" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB32,Services!$A$1:$B$45,2)),"",VLOOKUP(AB32,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD32" s="41"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
@@ -9933,46 +9957,46 @@
       <c r="K33" s="41"/>
       <c r="L33" s="41"/>
       <c r="M33" s="41"/>
-      <c r="N33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M33,Services!$A$1:$B$45,2)),"",VLOOKUP(M33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O33" s="41"/>
-      <c r="P33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O33,Services!$A$1:$B$45,2)),"",VLOOKUP(O33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q33" s="41"/>
-      <c r="R33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q33,Services!$A$1:$B$45,2)),"",VLOOKUP(Q33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S33" s="41"/>
-      <c r="T33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S33,Services!$A$1:$B$45,2)),"",VLOOKUP(S33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U33" s="41"/>
-      <c r="V33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U33,Services!$A$1:$B$45,2)),"",VLOOKUP(U33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W33" s="41"/>
-      <c r="X33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W33,Services!$A$1:$B$45,2)),"",VLOOKUP(W33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y33" s="41"/>
-      <c r="Z33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y33,Services!$A$1:$B$45,2)),"",VLOOKUP(Y33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA33" s="41"/>
-      <c r="AB33" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA33,Services!$A$1:$B$45,2)),"",VLOOKUP(AA33,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC33" s="41"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N33,Services!$A$1:$B$45,2)),"",VLOOKUP(N33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P33" s="41"/>
+      <c r="Q33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P33,Services!$A$1:$B$45,2)),"",VLOOKUP(P33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R33" s="41"/>
+      <c r="S33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R33,Services!$A$1:$B$45,2)),"",VLOOKUP(R33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T33" s="41"/>
+      <c r="U33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T33,Services!$A$1:$B$45,2)),"",VLOOKUP(T33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V33" s="41"/>
+      <c r="W33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V33,Services!$A$1:$B$45,2)),"",VLOOKUP(V33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X33" s="41"/>
+      <c r="Y33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X33,Services!$A$1:$B$45,2)),"",VLOOKUP(X33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z33" s="41"/>
+      <c r="AA33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z33,Services!$A$1:$B$45,2)),"",VLOOKUP(Z33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB33" s="41"/>
+      <c r="AC33" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB33,Services!$A$1:$B$45,2)),"",VLOOKUP(AB33,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD33" s="41"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
@@ -9998,46 +10022,46 @@
       <c r="K34" s="41"/>
       <c r="L34" s="41"/>
       <c r="M34" s="41"/>
-      <c r="N34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M34,Services!$A$1:$B$45,2)),"",VLOOKUP(M34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O34" s="41"/>
-      <c r="P34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O34,Services!$A$1:$B$45,2)),"",VLOOKUP(O34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q34" s="41"/>
-      <c r="R34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q34,Services!$A$1:$B$45,2)),"",VLOOKUP(Q34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S34" s="41"/>
-      <c r="T34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S34,Services!$A$1:$B$45,2)),"",VLOOKUP(S34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U34" s="41"/>
-      <c r="V34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U34,Services!$A$1:$B$45,2)),"",VLOOKUP(U34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W34" s="41"/>
-      <c r="X34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W34,Services!$A$1:$B$45,2)),"",VLOOKUP(W34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y34" s="41"/>
-      <c r="Z34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y34,Services!$A$1:$B$45,2)),"",VLOOKUP(Y34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA34" s="41"/>
-      <c r="AB34" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA34,Services!$A$1:$B$45,2)),"",VLOOKUP(AA34,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC34" s="41"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N34,Services!$A$1:$B$45,2)),"",VLOOKUP(N34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P34" s="41"/>
+      <c r="Q34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P34,Services!$A$1:$B$45,2)),"",VLOOKUP(P34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R34" s="41"/>
+      <c r="S34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R34,Services!$A$1:$B$45,2)),"",VLOOKUP(R34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T34" s="41"/>
+      <c r="U34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T34,Services!$A$1:$B$45,2)),"",VLOOKUP(T34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V34" s="41"/>
+      <c r="W34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V34,Services!$A$1:$B$45,2)),"",VLOOKUP(V34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X34" s="41"/>
+      <c r="Y34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X34,Services!$A$1:$B$45,2)),"",VLOOKUP(X34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z34" s="41"/>
+      <c r="AA34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z34,Services!$A$1:$B$45,2)),"",VLOOKUP(Z34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB34" s="41"/>
+      <c r="AC34" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB34,Services!$A$1:$B$45,2)),"",VLOOKUP(AB34,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD34" s="41"/>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
@@ -10063,46 +10087,46 @@
       <c r="K35" s="41"/>
       <c r="L35" s="41"/>
       <c r="M35" s="41"/>
-      <c r="N35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M35,Services!$A$1:$B$45,2)),"",VLOOKUP(M35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O35" s="41"/>
-      <c r="P35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O35,Services!$A$1:$B$45,2)),"",VLOOKUP(O35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q35" s="41"/>
-      <c r="R35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q35,Services!$A$1:$B$45,2)),"",VLOOKUP(Q35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S35" s="41"/>
-      <c r="T35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S35,Services!$A$1:$B$45,2)),"",VLOOKUP(S35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U35" s="41"/>
-      <c r="V35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U35,Services!$A$1:$B$45,2)),"",VLOOKUP(U35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W35" s="41"/>
-      <c r="X35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W35,Services!$A$1:$B$45,2)),"",VLOOKUP(W35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y35" s="41"/>
-      <c r="Z35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y35,Services!$A$1:$B$45,2)),"",VLOOKUP(Y35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA35" s="41"/>
-      <c r="AB35" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA35,Services!$A$1:$B$45,2)),"",VLOOKUP(AA35,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC35" s="41"/>
+      <c r="N35" s="41"/>
+      <c r="O35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N35,Services!$A$1:$B$45,2)),"",VLOOKUP(N35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P35" s="41"/>
+      <c r="Q35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P35,Services!$A$1:$B$45,2)),"",VLOOKUP(P35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R35" s="41"/>
+      <c r="S35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R35,Services!$A$1:$B$45,2)),"",VLOOKUP(R35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T35" s="41"/>
+      <c r="U35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T35,Services!$A$1:$B$45,2)),"",VLOOKUP(T35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V35" s="41"/>
+      <c r="W35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V35,Services!$A$1:$B$45,2)),"",VLOOKUP(V35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X35" s="41"/>
+      <c r="Y35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X35,Services!$A$1:$B$45,2)),"",VLOOKUP(X35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z35" s="41"/>
+      <c r="AA35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z35,Services!$A$1:$B$45,2)),"",VLOOKUP(Z35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB35" s="41"/>
+      <c r="AC35" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB35,Services!$A$1:$B$45,2)),"",VLOOKUP(AB35,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD35" s="41"/>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.2">
@@ -10128,46 +10152,46 @@
       <c r="K36" s="41"/>
       <c r="L36" s="41"/>
       <c r="M36" s="41"/>
-      <c r="N36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M36,Services!$A$1:$B$45,2)),"",VLOOKUP(M36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O36" s="41"/>
-      <c r="P36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O36,Services!$A$1:$B$45,2)),"",VLOOKUP(O36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q36,Services!$A$1:$B$45,2)),"",VLOOKUP(Q36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S36" s="41"/>
-      <c r="T36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S36,Services!$A$1:$B$45,2)),"",VLOOKUP(S36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U36" s="41"/>
-      <c r="V36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U36,Services!$A$1:$B$45,2)),"",VLOOKUP(U36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W36" s="41"/>
-      <c r="X36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W36,Services!$A$1:$B$45,2)),"",VLOOKUP(W36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y36" s="41"/>
-      <c r="Z36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y36,Services!$A$1:$B$45,2)),"",VLOOKUP(Y36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA36" s="41"/>
-      <c r="AB36" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA36,Services!$A$1:$B$45,2)),"",VLOOKUP(AA36,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC36" s="41"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N36,Services!$A$1:$B$45,2)),"",VLOOKUP(N36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P36" s="41"/>
+      <c r="Q36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P36,Services!$A$1:$B$45,2)),"",VLOOKUP(P36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R36" s="41"/>
+      <c r="S36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R36,Services!$A$1:$B$45,2)),"",VLOOKUP(R36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T36" s="41"/>
+      <c r="U36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T36,Services!$A$1:$B$45,2)),"",VLOOKUP(T36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V36" s="41"/>
+      <c r="W36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V36,Services!$A$1:$B$45,2)),"",VLOOKUP(V36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X36" s="41"/>
+      <c r="Y36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X36,Services!$A$1:$B$45,2)),"",VLOOKUP(X36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z36" s="41"/>
+      <c r="AA36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z36,Services!$A$1:$B$45,2)),"",VLOOKUP(Z36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB36" s="41"/>
+      <c r="AC36" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB36,Services!$A$1:$B$45,2)),"",VLOOKUP(AB36,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD36" s="41"/>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.2">
@@ -10193,46 +10217,46 @@
       <c r="K37" s="41"/>
       <c r="L37" s="41"/>
       <c r="M37" s="41"/>
-      <c r="N37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M37,Services!$A$1:$B$45,2)),"",VLOOKUP(M37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O37" s="41"/>
-      <c r="P37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O37,Services!$A$1:$B$45,2)),"",VLOOKUP(O37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q37" s="41"/>
-      <c r="R37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q37,Services!$A$1:$B$45,2)),"",VLOOKUP(Q37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S37" s="41"/>
-      <c r="T37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S37,Services!$A$1:$B$45,2)),"",VLOOKUP(S37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U37" s="41"/>
-      <c r="V37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U37,Services!$A$1:$B$45,2)),"",VLOOKUP(U37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W37" s="41"/>
-      <c r="X37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W37,Services!$A$1:$B$45,2)),"",VLOOKUP(W37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y37" s="41"/>
-      <c r="Z37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y37,Services!$A$1:$B$45,2)),"",VLOOKUP(Y37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA37" s="41"/>
-      <c r="AB37" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA37,Services!$A$1:$B$45,2)),"",VLOOKUP(AA37,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC37" s="41"/>
+      <c r="N37" s="41"/>
+      <c r="O37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N37,Services!$A$1:$B$45,2)),"",VLOOKUP(N37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P37" s="41"/>
+      <c r="Q37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P37,Services!$A$1:$B$45,2)),"",VLOOKUP(P37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R37" s="41"/>
+      <c r="S37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R37,Services!$A$1:$B$45,2)),"",VLOOKUP(R37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T37" s="41"/>
+      <c r="U37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T37,Services!$A$1:$B$45,2)),"",VLOOKUP(T37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V37" s="41"/>
+      <c r="W37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V37,Services!$A$1:$B$45,2)),"",VLOOKUP(V37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X37" s="41"/>
+      <c r="Y37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X37,Services!$A$1:$B$45,2)),"",VLOOKUP(X37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z37" s="41"/>
+      <c r="AA37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z37,Services!$A$1:$B$45,2)),"",VLOOKUP(Z37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB37" s="41"/>
+      <c r="AC37" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB37,Services!$A$1:$B$45,2)),"",VLOOKUP(AB37,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD37" s="41"/>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.2">
@@ -10258,46 +10282,46 @@
       <c r="K38" s="41"/>
       <c r="L38" s="41"/>
       <c r="M38" s="41"/>
-      <c r="N38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M38,Services!$A$1:$B$45,2)),"",VLOOKUP(M38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O38" s="41"/>
-      <c r="P38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O38,Services!$A$1:$B$45,2)),"",VLOOKUP(O38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q38,Services!$A$1:$B$45,2)),"",VLOOKUP(Q38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S38" s="41"/>
-      <c r="T38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S38,Services!$A$1:$B$45,2)),"",VLOOKUP(S38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U38" s="41"/>
-      <c r="V38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U38,Services!$A$1:$B$45,2)),"",VLOOKUP(U38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W38" s="41"/>
-      <c r="X38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W38,Services!$A$1:$B$45,2)),"",VLOOKUP(W38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y38" s="41"/>
-      <c r="Z38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y38,Services!$A$1:$B$45,2)),"",VLOOKUP(Y38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA38" s="41"/>
-      <c r="AB38" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA38,Services!$A$1:$B$45,2)),"",VLOOKUP(AA38,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC38" s="41"/>
+      <c r="N38" s="41"/>
+      <c r="O38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N38,Services!$A$1:$B$45,2)),"",VLOOKUP(N38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P38" s="41"/>
+      <c r="Q38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P38,Services!$A$1:$B$45,2)),"",VLOOKUP(P38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R38" s="41"/>
+      <c r="S38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R38,Services!$A$1:$B$45,2)),"",VLOOKUP(R38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T38" s="41"/>
+      <c r="U38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T38,Services!$A$1:$B$45,2)),"",VLOOKUP(T38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V38" s="41"/>
+      <c r="W38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V38,Services!$A$1:$B$45,2)),"",VLOOKUP(V38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X38" s="41"/>
+      <c r="Y38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X38,Services!$A$1:$B$45,2)),"",VLOOKUP(X38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z38" s="41"/>
+      <c r="AA38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z38,Services!$A$1:$B$45,2)),"",VLOOKUP(Z38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB38" s="41"/>
+      <c r="AC38" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB38,Services!$A$1:$B$45,2)),"",VLOOKUP(AB38,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD38" s="41"/>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.2">
@@ -10323,46 +10347,46 @@
       <c r="K39" s="41"/>
       <c r="L39" s="41"/>
       <c r="M39" s="41"/>
-      <c r="N39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M39,Services!$A$1:$B$45,2)),"",VLOOKUP(M39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O39" s="41"/>
-      <c r="P39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O39,Services!$A$1:$B$45,2)),"",VLOOKUP(O39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q39" s="41"/>
-      <c r="R39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q39,Services!$A$1:$B$45,2)),"",VLOOKUP(Q39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S39" s="41"/>
-      <c r="T39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S39,Services!$A$1:$B$45,2)),"",VLOOKUP(S39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U39" s="41"/>
-      <c r="V39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U39,Services!$A$1:$B$45,2)),"",VLOOKUP(U39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W39" s="41"/>
-      <c r="X39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W39,Services!$A$1:$B$45,2)),"",VLOOKUP(W39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y39" s="41"/>
-      <c r="Z39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y39,Services!$A$1:$B$45,2)),"",VLOOKUP(Y39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA39" s="41"/>
-      <c r="AB39" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA39,Services!$A$1:$B$45,2)),"",VLOOKUP(AA39,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC39" s="41"/>
+      <c r="N39" s="41"/>
+      <c r="O39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N39,Services!$A$1:$B$45,2)),"",VLOOKUP(N39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P39" s="41"/>
+      <c r="Q39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P39,Services!$A$1:$B$45,2)),"",VLOOKUP(P39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R39" s="41"/>
+      <c r="S39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R39,Services!$A$1:$B$45,2)),"",VLOOKUP(R39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T39" s="41"/>
+      <c r="U39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T39,Services!$A$1:$B$45,2)),"",VLOOKUP(T39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V39" s="41"/>
+      <c r="W39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V39,Services!$A$1:$B$45,2)),"",VLOOKUP(V39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X39" s="41"/>
+      <c r="Y39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X39,Services!$A$1:$B$45,2)),"",VLOOKUP(X39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z39" s="41"/>
+      <c r="AA39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z39,Services!$A$1:$B$45,2)),"",VLOOKUP(Z39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB39" s="41"/>
+      <c r="AC39" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB39,Services!$A$1:$B$45,2)),"",VLOOKUP(AB39,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD39" s="41"/>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.2">
@@ -10388,46 +10412,46 @@
       <c r="K40" s="41"/>
       <c r="L40" s="41"/>
       <c r="M40" s="41"/>
-      <c r="N40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M40,Services!$A$1:$B$45,2)),"",VLOOKUP(M40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O40" s="41"/>
-      <c r="P40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O40,Services!$A$1:$B$45,2)),"",VLOOKUP(O40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q40" s="41"/>
-      <c r="R40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q40,Services!$A$1:$B$45,2)),"",VLOOKUP(Q40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S40" s="41"/>
-      <c r="T40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S40,Services!$A$1:$B$45,2)),"",VLOOKUP(S40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U40" s="41"/>
-      <c r="V40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U40,Services!$A$1:$B$45,2)),"",VLOOKUP(U40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W40" s="41"/>
-      <c r="X40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W40,Services!$A$1:$B$45,2)),"",VLOOKUP(W40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y40" s="41"/>
-      <c r="Z40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y40,Services!$A$1:$B$45,2)),"",VLOOKUP(Y40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA40" s="41"/>
-      <c r="AB40" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA40,Services!$A$1:$B$45,2)),"",VLOOKUP(AA40,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC40" s="41"/>
+      <c r="N40" s="41"/>
+      <c r="O40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N40,Services!$A$1:$B$45,2)),"",VLOOKUP(N40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P40" s="41"/>
+      <c r="Q40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P40,Services!$A$1:$B$45,2)),"",VLOOKUP(P40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R40" s="41"/>
+      <c r="S40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R40,Services!$A$1:$B$45,2)),"",VLOOKUP(R40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T40" s="41"/>
+      <c r="U40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T40,Services!$A$1:$B$45,2)),"",VLOOKUP(T40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V40" s="41"/>
+      <c r="W40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V40,Services!$A$1:$B$45,2)),"",VLOOKUP(V40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X40" s="41"/>
+      <c r="Y40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X40,Services!$A$1:$B$45,2)),"",VLOOKUP(X40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z40" s="41"/>
+      <c r="AA40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z40,Services!$A$1:$B$45,2)),"",VLOOKUP(Z40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB40" s="41"/>
+      <c r="AC40" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB40,Services!$A$1:$B$45,2)),"",VLOOKUP(AB40,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD40" s="41"/>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.2">
@@ -10453,46 +10477,46 @@
       <c r="K41" s="41"/>
       <c r="L41" s="41"/>
       <c r="M41" s="41"/>
-      <c r="N41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M41,Services!$A$1:$B$45,2)),"",VLOOKUP(M41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O41" s="41"/>
-      <c r="P41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O41,Services!$A$1:$B$45,2)),"",VLOOKUP(O41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q41" s="41"/>
-      <c r="R41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q41,Services!$A$1:$B$45,2)),"",VLOOKUP(Q41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S41" s="41"/>
-      <c r="T41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S41,Services!$A$1:$B$45,2)),"",VLOOKUP(S41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U41" s="41"/>
-      <c r="V41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U41,Services!$A$1:$B$45,2)),"",VLOOKUP(U41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W41" s="41"/>
-      <c r="X41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W41,Services!$A$1:$B$45,2)),"",VLOOKUP(W41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y41" s="41"/>
-      <c r="Z41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y41,Services!$A$1:$B$45,2)),"",VLOOKUP(Y41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA41" s="41"/>
-      <c r="AB41" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA41,Services!$A$1:$B$45,2)),"",VLOOKUP(AA41,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC41" s="41"/>
+      <c r="N41" s="41"/>
+      <c r="O41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N41,Services!$A$1:$B$45,2)),"",VLOOKUP(N41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P41" s="41"/>
+      <c r="Q41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P41,Services!$A$1:$B$45,2)),"",VLOOKUP(P41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R41" s="41"/>
+      <c r="S41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R41,Services!$A$1:$B$45,2)),"",VLOOKUP(R41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T41" s="41"/>
+      <c r="U41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T41,Services!$A$1:$B$45,2)),"",VLOOKUP(T41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V41" s="41"/>
+      <c r="W41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V41,Services!$A$1:$B$45,2)),"",VLOOKUP(V41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X41" s="41"/>
+      <c r="Y41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X41,Services!$A$1:$B$45,2)),"",VLOOKUP(X41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z41" s="41"/>
+      <c r="AA41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z41,Services!$A$1:$B$45,2)),"",VLOOKUP(Z41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB41" s="41"/>
+      <c r="AC41" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB41,Services!$A$1:$B$45,2)),"",VLOOKUP(AB41,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD41" s="41"/>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
@@ -10518,46 +10542,46 @@
       <c r="K42" s="41"/>
       <c r="L42" s="41"/>
       <c r="M42" s="41"/>
-      <c r="N42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M42,Services!$A$1:$B$45,2)),"",VLOOKUP(M42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O42" s="41"/>
-      <c r="P42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O42,Services!$A$1:$B$45,2)),"",VLOOKUP(O42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q42" s="41"/>
-      <c r="R42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q42,Services!$A$1:$B$45,2)),"",VLOOKUP(Q42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S42" s="41"/>
-      <c r="T42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S42,Services!$A$1:$B$45,2)),"",VLOOKUP(S42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U42" s="41"/>
-      <c r="V42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U42,Services!$A$1:$B$45,2)),"",VLOOKUP(U42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W42" s="41"/>
-      <c r="X42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W42,Services!$A$1:$B$45,2)),"",VLOOKUP(W42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y42" s="41"/>
-      <c r="Z42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y42,Services!$A$1:$B$45,2)),"",VLOOKUP(Y42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA42" s="41"/>
-      <c r="AB42" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA42,Services!$A$1:$B$45,2)),"",VLOOKUP(AA42,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC42" s="41"/>
+      <c r="N42" s="41"/>
+      <c r="O42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N42,Services!$A$1:$B$45,2)),"",VLOOKUP(N42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P42" s="41"/>
+      <c r="Q42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P42,Services!$A$1:$B$45,2)),"",VLOOKUP(P42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R42" s="41"/>
+      <c r="S42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R42,Services!$A$1:$B$45,2)),"",VLOOKUP(R42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T42" s="41"/>
+      <c r="U42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T42,Services!$A$1:$B$45,2)),"",VLOOKUP(T42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V42" s="41"/>
+      <c r="W42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V42,Services!$A$1:$B$45,2)),"",VLOOKUP(V42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X42" s="41"/>
+      <c r="Y42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X42,Services!$A$1:$B$45,2)),"",VLOOKUP(X42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z42" s="41"/>
+      <c r="AA42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z42,Services!$A$1:$B$45,2)),"",VLOOKUP(Z42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB42" s="41"/>
+      <c r="AC42" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB42,Services!$A$1:$B$45,2)),"",VLOOKUP(AB42,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD42" s="41"/>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
@@ -10583,46 +10607,46 @@
       <c r="K43" s="41"/>
       <c r="L43" s="41"/>
       <c r="M43" s="41"/>
-      <c r="N43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M43,Services!$A$1:$B$45,2)),"",VLOOKUP(M43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O43" s="41"/>
-      <c r="P43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O43,Services!$A$1:$B$45,2)),"",VLOOKUP(O43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q43" s="41"/>
-      <c r="R43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q43,Services!$A$1:$B$45,2)),"",VLOOKUP(Q43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S43" s="41"/>
-      <c r="T43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S43,Services!$A$1:$B$45,2)),"",VLOOKUP(S43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U43" s="41"/>
-      <c r="V43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U43,Services!$A$1:$B$45,2)),"",VLOOKUP(U43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W43" s="41"/>
-      <c r="X43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W43,Services!$A$1:$B$45,2)),"",VLOOKUP(W43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y43" s="41"/>
-      <c r="Z43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y43,Services!$A$1:$B$45,2)),"",VLOOKUP(Y43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA43" s="41"/>
-      <c r="AB43" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA43,Services!$A$1:$B$45,2)),"",VLOOKUP(AA43,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC43" s="41"/>
+      <c r="N43" s="41"/>
+      <c r="O43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N43,Services!$A$1:$B$45,2)),"",VLOOKUP(N43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P43" s="41"/>
+      <c r="Q43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P43,Services!$A$1:$B$45,2)),"",VLOOKUP(P43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R43" s="41"/>
+      <c r="S43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R43,Services!$A$1:$B$45,2)),"",VLOOKUP(R43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T43" s="41"/>
+      <c r="U43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T43,Services!$A$1:$B$45,2)),"",VLOOKUP(T43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V43" s="41"/>
+      <c r="W43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V43,Services!$A$1:$B$45,2)),"",VLOOKUP(V43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X43" s="41"/>
+      <c r="Y43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X43,Services!$A$1:$B$45,2)),"",VLOOKUP(X43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z43" s="41"/>
+      <c r="AA43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z43,Services!$A$1:$B$45,2)),"",VLOOKUP(Z43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB43" s="41"/>
+      <c r="AC43" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB43,Services!$A$1:$B$45,2)),"",VLOOKUP(AB43,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD43" s="41"/>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.2">
@@ -10648,46 +10672,46 @@
       <c r="K44" s="41"/>
       <c r="L44" s="41"/>
       <c r="M44" s="41"/>
-      <c r="N44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M44,Services!$A$1:$B$45,2)),"",VLOOKUP(M44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O44" s="41"/>
-      <c r="P44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O44,Services!$A$1:$B$45,2)),"",VLOOKUP(O44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q44" s="41"/>
-      <c r="R44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q44,Services!$A$1:$B$45,2)),"",VLOOKUP(Q44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S44" s="41"/>
-      <c r="T44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S44,Services!$A$1:$B$45,2)),"",VLOOKUP(S44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U44" s="41"/>
-      <c r="V44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U44,Services!$A$1:$B$45,2)),"",VLOOKUP(U44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W44" s="41"/>
-      <c r="X44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W44,Services!$A$1:$B$45,2)),"",VLOOKUP(W44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y44" s="41"/>
-      <c r="Z44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y44,Services!$A$1:$B$45,2)),"",VLOOKUP(Y44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA44" s="41"/>
-      <c r="AB44" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA44,Services!$A$1:$B$45,2)),"",VLOOKUP(AA44,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC44" s="41"/>
+      <c r="N44" s="41"/>
+      <c r="O44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N44,Services!$A$1:$B$45,2)),"",VLOOKUP(N44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P44" s="41"/>
+      <c r="Q44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P44,Services!$A$1:$B$45,2)),"",VLOOKUP(P44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R44" s="41"/>
+      <c r="S44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R44,Services!$A$1:$B$45,2)),"",VLOOKUP(R44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T44" s="41"/>
+      <c r="U44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T44,Services!$A$1:$B$45,2)),"",VLOOKUP(T44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V44" s="41"/>
+      <c r="W44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V44,Services!$A$1:$B$45,2)),"",VLOOKUP(V44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X44" s="41"/>
+      <c r="Y44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X44,Services!$A$1:$B$45,2)),"",VLOOKUP(X44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z44" s="41"/>
+      <c r="AA44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z44,Services!$A$1:$B$45,2)),"",VLOOKUP(Z44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB44" s="41"/>
+      <c r="AC44" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB44,Services!$A$1:$B$45,2)),"",VLOOKUP(AB44,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD44" s="41"/>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.2">
@@ -10713,46 +10737,46 @@
       <c r="K45" s="41"/>
       <c r="L45" s="41"/>
       <c r="M45" s="41"/>
-      <c r="N45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M45,Services!$A$1:$B$45,2)),"",VLOOKUP(M45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O45" s="41"/>
-      <c r="P45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O45,Services!$A$1:$B$45,2)),"",VLOOKUP(O45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q45" s="41"/>
-      <c r="R45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q45,Services!$A$1:$B$45,2)),"",VLOOKUP(Q45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S45" s="41"/>
-      <c r="T45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S45,Services!$A$1:$B$45,2)),"",VLOOKUP(S45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U45" s="41"/>
-      <c r="V45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U45,Services!$A$1:$B$45,2)),"",VLOOKUP(U45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W45" s="41"/>
-      <c r="X45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W45,Services!$A$1:$B$45,2)),"",VLOOKUP(W45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y45" s="41"/>
-      <c r="Z45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y45,Services!$A$1:$B$45,2)),"",VLOOKUP(Y45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA45" s="41"/>
-      <c r="AB45" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA45,Services!$A$1:$B$45,2)),"",VLOOKUP(AA45,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC45" s="41"/>
+      <c r="N45" s="41"/>
+      <c r="O45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N45,Services!$A$1:$B$45,2)),"",VLOOKUP(N45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P45" s="41"/>
+      <c r="Q45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P45,Services!$A$1:$B$45,2)),"",VLOOKUP(P45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R45" s="41"/>
+      <c r="S45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R45,Services!$A$1:$B$45,2)),"",VLOOKUP(R45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T45" s="41"/>
+      <c r="U45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T45,Services!$A$1:$B$45,2)),"",VLOOKUP(T45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V45" s="41"/>
+      <c r="W45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V45,Services!$A$1:$B$45,2)),"",VLOOKUP(V45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X45" s="41"/>
+      <c r="Y45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X45,Services!$A$1:$B$45,2)),"",VLOOKUP(X45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z45" s="41"/>
+      <c r="AA45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z45,Services!$A$1:$B$45,2)),"",VLOOKUP(Z45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB45" s="41"/>
+      <c r="AC45" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB45,Services!$A$1:$B$45,2)),"",VLOOKUP(AB45,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD45" s="41"/>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.2">
@@ -10778,46 +10802,46 @@
       <c r="K46" s="41"/>
       <c r="L46" s="41"/>
       <c r="M46" s="41"/>
-      <c r="N46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M46,Services!$A$1:$B$45,2)),"",VLOOKUP(M46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O46" s="41"/>
-      <c r="P46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O46,Services!$A$1:$B$45,2)),"",VLOOKUP(O46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q46" s="41"/>
-      <c r="R46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q46,Services!$A$1:$B$45,2)),"",VLOOKUP(Q46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S46" s="41"/>
-      <c r="T46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S46,Services!$A$1:$B$45,2)),"",VLOOKUP(S46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U46" s="41"/>
-      <c r="V46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U46,Services!$A$1:$B$45,2)),"",VLOOKUP(U46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W46" s="41"/>
-      <c r="X46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W46,Services!$A$1:$B$45,2)),"",VLOOKUP(W46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y46" s="41"/>
-      <c r="Z46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y46,Services!$A$1:$B$45,2)),"",VLOOKUP(Y46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA46" s="41"/>
-      <c r="AB46" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA46,Services!$A$1:$B$45,2)),"",VLOOKUP(AA46,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC46" s="41"/>
+      <c r="N46" s="41"/>
+      <c r="O46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N46,Services!$A$1:$B$45,2)),"",VLOOKUP(N46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P46" s="41"/>
+      <c r="Q46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P46,Services!$A$1:$B$45,2)),"",VLOOKUP(P46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R46" s="41"/>
+      <c r="S46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R46,Services!$A$1:$B$45,2)),"",VLOOKUP(R46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T46" s="41"/>
+      <c r="U46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T46,Services!$A$1:$B$45,2)),"",VLOOKUP(T46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V46" s="41"/>
+      <c r="W46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V46,Services!$A$1:$B$45,2)),"",VLOOKUP(V46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X46" s="41"/>
+      <c r="Y46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X46,Services!$A$1:$B$45,2)),"",VLOOKUP(X46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z46" s="41"/>
+      <c r="AA46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z46,Services!$A$1:$B$45,2)),"",VLOOKUP(Z46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB46" s="41"/>
+      <c r="AC46" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB46,Services!$A$1:$B$45,2)),"",VLOOKUP(AB46,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD46" s="41"/>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.2">
@@ -10843,46 +10867,46 @@
       <c r="K47" s="41"/>
       <c r="L47" s="41"/>
       <c r="M47" s="41"/>
-      <c r="N47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M47,Services!$A$1:$B$45,2)),"",VLOOKUP(M47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O47" s="41"/>
-      <c r="P47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O47,Services!$A$1:$B$45,2)),"",VLOOKUP(O47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q47" s="41"/>
-      <c r="R47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q47,Services!$A$1:$B$45,2)),"",VLOOKUP(Q47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S47" s="41"/>
-      <c r="T47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S47,Services!$A$1:$B$45,2)),"",VLOOKUP(S47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U47" s="41"/>
-      <c r="V47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U47,Services!$A$1:$B$45,2)),"",VLOOKUP(U47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W47" s="41"/>
-      <c r="X47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W47,Services!$A$1:$B$45,2)),"",VLOOKUP(W47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y47" s="41"/>
-      <c r="Z47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y47,Services!$A$1:$B$45,2)),"",VLOOKUP(Y47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA47" s="41"/>
-      <c r="AB47" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA47,Services!$A$1:$B$45,2)),"",VLOOKUP(AA47,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC47" s="41"/>
+      <c r="N47" s="41"/>
+      <c r="O47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N47,Services!$A$1:$B$45,2)),"",VLOOKUP(N47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P47" s="41"/>
+      <c r="Q47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P47,Services!$A$1:$B$45,2)),"",VLOOKUP(P47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R47" s="41"/>
+      <c r="S47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R47,Services!$A$1:$B$45,2)),"",VLOOKUP(R47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T47" s="41"/>
+      <c r="U47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T47,Services!$A$1:$B$45,2)),"",VLOOKUP(T47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V47" s="41"/>
+      <c r="W47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V47,Services!$A$1:$B$45,2)),"",VLOOKUP(V47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X47" s="41"/>
+      <c r="Y47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X47,Services!$A$1:$B$45,2)),"",VLOOKUP(X47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z47" s="41"/>
+      <c r="AA47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z47,Services!$A$1:$B$45,2)),"",VLOOKUP(Z47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB47" s="41"/>
+      <c r="AC47" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB47,Services!$A$1:$B$45,2)),"",VLOOKUP(AB47,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD47" s="41"/>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
@@ -10908,46 +10932,46 @@
       <c r="K48" s="41"/>
       <c r="L48" s="41"/>
       <c r="M48" s="41"/>
-      <c r="N48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M48,Services!$A$1:$B$45,2)),"",VLOOKUP(M48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O48" s="41"/>
-      <c r="P48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O48,Services!$A$1:$B$45,2)),"",VLOOKUP(O48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q48" s="41"/>
-      <c r="R48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q48,Services!$A$1:$B$45,2)),"",VLOOKUP(Q48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S48" s="41"/>
-      <c r="T48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S48,Services!$A$1:$B$45,2)),"",VLOOKUP(S48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U48" s="41"/>
-      <c r="V48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U48,Services!$A$1:$B$45,2)),"",VLOOKUP(U48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W48" s="41"/>
-      <c r="X48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W48,Services!$A$1:$B$45,2)),"",VLOOKUP(W48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y48" s="41"/>
-      <c r="Z48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y48,Services!$A$1:$B$45,2)),"",VLOOKUP(Y48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA48" s="41"/>
-      <c r="AB48" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA48,Services!$A$1:$B$45,2)),"",VLOOKUP(AA48,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC48" s="41"/>
+      <c r="N48" s="41"/>
+      <c r="O48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N48,Services!$A$1:$B$45,2)),"",VLOOKUP(N48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P48" s="41"/>
+      <c r="Q48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P48,Services!$A$1:$B$45,2)),"",VLOOKUP(P48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R48" s="41"/>
+      <c r="S48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R48,Services!$A$1:$B$45,2)),"",VLOOKUP(R48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T48" s="41"/>
+      <c r="U48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T48,Services!$A$1:$B$45,2)),"",VLOOKUP(T48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V48" s="41"/>
+      <c r="W48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V48,Services!$A$1:$B$45,2)),"",VLOOKUP(V48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X48" s="41"/>
+      <c r="Y48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X48,Services!$A$1:$B$45,2)),"",VLOOKUP(X48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z48" s="41"/>
+      <c r="AA48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z48,Services!$A$1:$B$45,2)),"",VLOOKUP(Z48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB48" s="41"/>
+      <c r="AC48" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB48,Services!$A$1:$B$45,2)),"",VLOOKUP(AB48,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD48" s="41"/>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.2">
@@ -10973,46 +10997,46 @@
       <c r="K49" s="41"/>
       <c r="L49" s="41"/>
       <c r="M49" s="41"/>
-      <c r="N49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M49,Services!$A$1:$B$45,2)),"",VLOOKUP(M49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O49" s="41"/>
-      <c r="P49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O49,Services!$A$1:$B$45,2)),"",VLOOKUP(O49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q49" s="41"/>
-      <c r="R49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q49,Services!$A$1:$B$45,2)),"",VLOOKUP(Q49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S49" s="41"/>
-      <c r="T49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S49,Services!$A$1:$B$45,2)),"",VLOOKUP(S49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U49" s="41"/>
-      <c r="V49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U49,Services!$A$1:$B$45,2)),"",VLOOKUP(U49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W49" s="41"/>
-      <c r="X49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W49,Services!$A$1:$B$45,2)),"",VLOOKUP(W49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y49" s="41"/>
-      <c r="Z49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y49,Services!$A$1:$B$45,2)),"",VLOOKUP(Y49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA49" s="41"/>
-      <c r="AB49" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA49,Services!$A$1:$B$45,2)),"",VLOOKUP(AA49,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC49" s="41"/>
+      <c r="N49" s="41"/>
+      <c r="O49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N49,Services!$A$1:$B$45,2)),"",VLOOKUP(N49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P49" s="41"/>
+      <c r="Q49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P49,Services!$A$1:$B$45,2)),"",VLOOKUP(P49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R49" s="41"/>
+      <c r="S49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R49,Services!$A$1:$B$45,2)),"",VLOOKUP(R49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T49" s="41"/>
+      <c r="U49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T49,Services!$A$1:$B$45,2)),"",VLOOKUP(T49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V49" s="41"/>
+      <c r="W49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V49,Services!$A$1:$B$45,2)),"",VLOOKUP(V49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X49" s="41"/>
+      <c r="Y49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X49,Services!$A$1:$B$45,2)),"",VLOOKUP(X49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z49" s="41"/>
+      <c r="AA49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z49,Services!$A$1:$B$45,2)),"",VLOOKUP(Z49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB49" s="41"/>
+      <c r="AC49" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB49,Services!$A$1:$B$45,2)),"",VLOOKUP(AB49,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD49" s="41"/>
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.2">
@@ -11038,46 +11062,46 @@
       <c r="K50" s="41"/>
       <c r="L50" s="41"/>
       <c r="M50" s="41"/>
-      <c r="N50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(M50,Services!$A$1:$B$45,2)),"",VLOOKUP(M50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O50" s="41"/>
-      <c r="P50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(O50,Services!$A$1:$B$45,2)),"",VLOOKUP(O50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Q50" s="41"/>
-      <c r="R50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Q50,Services!$A$1:$B$45,2)),"",VLOOKUP(Q50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="S50" s="41"/>
-      <c r="T50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(S50,Services!$A$1:$B$45,2)),"",VLOOKUP(S50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="U50" s="41"/>
-      <c r="V50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(U50,Services!$A$1:$B$45,2)),"",VLOOKUP(U50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="W50" s="41"/>
-      <c r="X50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(W50,Services!$A$1:$B$45,2)),"",VLOOKUP(W50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="Y50" s="41"/>
-      <c r="Z50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(Y50,Services!$A$1:$B$45,2)),"",VLOOKUP(Y50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AA50" s="41"/>
-      <c r="AB50" s="1" t="str">
-        <f>IF(ISNA(VLOOKUP(AA50,Services!$A$1:$B$45,2)),"",VLOOKUP(AA50,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="AC50" s="41"/>
+      <c r="N50" s="41"/>
+      <c r="O50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(N50,Services!$A$1:$B$45,2)),"",VLOOKUP(N50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="P50" s="41"/>
+      <c r="Q50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(P50,Services!$A$1:$B$45,2)),"",VLOOKUP(P50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="R50" s="41"/>
+      <c r="S50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(R50,Services!$A$1:$B$45,2)),"",VLOOKUP(R50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="T50" s="41"/>
+      <c r="U50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(T50,Services!$A$1:$B$45,2)),"",VLOOKUP(T50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="V50" s="41"/>
+      <c r="W50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(V50,Services!$A$1:$B$45,2)),"",VLOOKUP(V50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="X50" s="41"/>
+      <c r="Y50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(X50,Services!$A$1:$B$45,2)),"",VLOOKUP(X50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="Z50" s="41"/>
+      <c r="AA50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(Z50,Services!$A$1:$B$45,2)),"",VLOOKUP(Z50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
+      <c r="AB50" s="41"/>
+      <c r="AC50" s="1" t="str">
+        <f>IF(ISNA(VLOOKUP(AB50,Services!$A$1:$B$45,2)),"",VLOOKUP(AB50,Services!$A$1:$B$45,2))</f>
+        <v/>
+      </c>
       <c r="AD50" s="41"/>
     </row>
   </sheetData>
@@ -11097,7 +11121,7 @@
           <x14:formula1>
             <xm:f>Services!$A$1:$A$43</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q50 S2:S50 U2:U50 W2:W50 Y2:Y50 AA2:AA50 M2:M50 O2:O50</xm:sqref>
+          <xm:sqref>R2:R50 T2:T50 V2:V50 X2:X50 Z2:Z50 AB2:AB50 N2:N50 P2:P50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{69AD3E96-9986-4437-A6D2-54EE41465A4B}">
           <x14:formula1>
@@ -11115,13 +11139,13 @@
           <x14:formula1>
             <xm:f>Roles!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:L50</xm:sqref>
+          <xm:sqref>K2:M50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0B1666EF-45EA-466E-BF9B-CD6C235D8633}">
           <x14:formula1>
             <xm:f>Validations!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>AD2:AD50</xm:sqref>
+          <xm:sqref>M2:M50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11170,7 +11194,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="IrVQ7Ukz2v/R7gQxangUL5wAqS1715tiGhzT8zLeCz8UJwUIBrCLI/UycSYlC8mt/P4bgWL9vpSls59MeyEaVg==" saltValue="9syDTPxVg8TLEzOvGTicbQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11552,7 +11575,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="aMZLA0VNhh5Onc5JvFgRcO+m2AuGfgKZ7BoJklGYjHaipO31AQ3xGW7Ut3i3WYaf9wFLoxFNYPTBp+0/KJwncA==" saltValue="2GsNMsCJLWlXXOIX1gAyDg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18784,7 +18806,6 @@
     <row r="741" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="742" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="m8UckgdD1dcYD9lqf4mZ6sweQUAjls9wUBQbAbH6Fx4sDdSYOTY5ss+Y9DW0iJlEs+St9Rf87Aa3SmKNJ6YBnQ==" saltValue="jfT1mkCRVBT5GRvlbF+nFg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <hyperlinks>
     <hyperlink ref="A287" r:id="rId1" display="https://courttribunalfinder.service.gov.uk/courts/sunderland-county-family-magistrates-and-tribunal-hearings" xr:uid="{E75D3469-3062-4D00-9760-56E3C0055DF4}"/>
   </hyperlinks>
@@ -18878,7 +18899,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9Dzbl1Vp2as7XYFJXUh3e5BVC8sA06Mwnij3IjqsMXS9OIFgu8FBluC3Lbx7+HH6n1k9gv2FDDtFo6g8N0a+SA==" saltValue="2ONKPZCzYuddgylpf3RncA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -18888,10 +18908,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18916,8 +18936,71 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="K9Ci/eHmkmskFS0u1ZcnQkRZSqVBH/Kvod5Cg143QmMMqKBzxu71t7mKY0rKC7jAIRToE1wAYtCUnAacyc3hTg==" saltValue="vAGcL88qkz3LKuOeKothwQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -18943,7 +19026,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="D22dSHc3htXuo0x/4I3E9zXiFJcvy3Um+2pZMVdKjhStG73OU02OP04I/9LO7uth2Ls3E1T7wBkvo4tC4iIMtQ==" saltValue="zUVhzd2HkNeGZm+LUf4U+A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: RDCC-5181 Fixed the failing test by modifying the test data to include the correct work area whose corresponding role has been configured in idam
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/new/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D4A799-FD82-5946-A013-6C9848557538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F21AF26-914D-D54C-8EF9-7DAE8FB7D767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -31,7 +31,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="1223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="1223">
   <si>
     <t>Region</t>
   </si>
@@ -7710,8 +7714,8 @@
   </sheetPr>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7843,15 +7847,15 @@
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="str">
         <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Nsvg</v>
+        <v>Tmek</v>
       </c>
       <c r="B2" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Uxsv</v>
+        <v>Aylc</v>
       </c>
       <c r="C2" s="41" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-7379430719@justice.gov.uk</v>
+        <v>CWR-func-test-user-1873865442@justice.gov.uk</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>5</v>
@@ -7933,15 +7937,15 @@
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rvsv</v>
+        <v>Gmgz</v>
       </c>
       <c r="B3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Cirx</v>
+        <v>Hjev</v>
       </c>
       <c r="C3" s="41" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-4727387448@justice.gov.uk</v>
+        <v>CWR-func-test-user-9616547353@justice.gov.uk</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>6</v>
@@ -8019,15 +8023,15 @@
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Wjca</v>
+        <v>Taom</v>
       </c>
       <c r="B4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rfpz</v>
+        <v>Mdot</v>
       </c>
       <c r="C4" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-876759313@justice.gov.uk</v>
+        <v>CWR-func-test-user-4875266102@justice.gov.uk</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>9</v>
@@ -8113,7 +8117,7 @@
       </c>
       <c r="C5" s="41" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-5566951720@justice.gov.uk</v>
+        <v>CWR-func-test-user-988485094@justice.gov.uk</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>4</v>
@@ -8160,10 +8164,12 @@
         <f>IF(ISNA(VLOOKUP(P5,Services!$A$1:$B$45,2)),"",VLOOKUP(P5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
-      <c r="R5" s="40"/>
+      <c r="R5" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="S5" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(R5,Services!$A$1:$B$45,2)),"",VLOOKUP(R5,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BAA4</v>
       </c>
       <c r="T5" s="40"/>
       <c r="U5" s="1" t="str">

</xml_diff>

<commit_message>
fix: RDCC-5181 Fixed the failing test by modifying the test data to include the correct work area whose corresponding role has been configured in idam(#530)
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/new/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D4A799-FD82-5946-A013-6C9848557538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F21AF26-914D-D54C-8EF9-7DAE8FB7D767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -31,7 +31,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="1223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="1223">
   <si>
     <t>Region</t>
   </si>
@@ -7710,8 +7714,8 @@
   </sheetPr>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7843,15 +7847,15 @@
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="str">
         <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Nsvg</v>
+        <v>Tmek</v>
       </c>
       <c r="B2" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Uxsv</v>
+        <v>Aylc</v>
       </c>
       <c r="C2" s="41" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-7379430719@justice.gov.uk</v>
+        <v>CWR-func-test-user-1873865442@justice.gov.uk</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>5</v>
@@ -7933,15 +7937,15 @@
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rvsv</v>
+        <v>Gmgz</v>
       </c>
       <c r="B3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Cirx</v>
+        <v>Hjev</v>
       </c>
       <c r="C3" s="41" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-4727387448@justice.gov.uk</v>
+        <v>CWR-func-test-user-9616547353@justice.gov.uk</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>6</v>
@@ -8019,15 +8023,15 @@
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Wjca</v>
+        <v>Taom</v>
       </c>
       <c r="B4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Rfpz</v>
+        <v>Mdot</v>
       </c>
       <c r="C4" s="41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-876759313@justice.gov.uk</v>
+        <v>CWR-func-test-user-4875266102@justice.gov.uk</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>9</v>
@@ -8113,7 +8117,7 @@
       </c>
       <c r="C5" s="41" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-5566951720@justice.gov.uk</v>
+        <v>CWR-func-test-user-988485094@justice.gov.uk</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>4</v>
@@ -8160,10 +8164,12 @@
         <f>IF(ISNA(VLOOKUP(P5,Services!$A$1:$B$45,2)),"",VLOOKUP(P5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
-      <c r="R5" s="40"/>
+      <c r="R5" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="S5" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(R5,Services!$A$1:$B$45,2)),"",VLOOKUP(R5,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BAA4</v>
       </c>
       <c r="T5" s="40"/>
       <c r="U5" s="1" t="str">

</xml_diff>

<commit_message>
RDCC-5489 - Staff : configure domain as list - functional test
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/new/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_659064/HMCTS/rd-caseworker-ref-api-Email-domainchanges/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F21AF26-914D-D54C-8EF9-7DAE8FB7D767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BB4141-889C-B548-8344-346016068247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="11" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="1223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="1223">
   <si>
     <t>Region</t>
   </si>
@@ -3957,7 +3957,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -4026,7 +4026,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4049,7 +4049,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -4065,9 +4065,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -7714,8 +7711,8 @@
   </sheetPr>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7725,18 +7722,18 @@
     <col min="3" max="3" width="30.1640625" style="39" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" style="39" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="62.5" style="39" customWidth="1"/>
-    <col min="7" max="7" width="33.83203125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="49.83203125" style="39" customWidth="1"/>
-    <col min="9" max="9" width="32.1640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="43.83203125" style="39" customWidth="1"/>
+    <col min="7" max="7" width="33.83203125" customWidth="1"/>
+    <col min="8" max="8" width="36.83203125" style="39" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5" style="39" customWidth="1"/>
     <col min="11" max="11" width="25.5" style="39" customWidth="1"/>
     <col min="12" max="12" width="19.5" style="39" customWidth="1"/>
     <col min="13" max="13" width="8.83203125" style="39"/>
     <col min="14" max="14" width="24" style="39" customWidth="1"/>
-    <col min="15" max="15" width="24" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21.33203125" style="39" customWidth="1"/>
-    <col min="17" max="17" width="21.33203125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.1640625" style="39" customWidth="1"/>
     <col min="19" max="19" width="19.1640625" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="19.1640625" style="39" customWidth="1"/>
@@ -7789,7 +7786,7 @@
       <c r="L1" s="36" t="s">
         <v>409</v>
       </c>
-      <c r="M1" s="42" t="s">
+      <c r="M1" s="41" t="s">
         <v>1110</v>
       </c>
       <c r="N1" s="37" t="s">
@@ -7847,15 +7844,15 @@
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="str">
         <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Tmek</v>
+        <v>Vcjh</v>
       </c>
       <c r="B2" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Aylc</v>
-      </c>
-      <c r="C2" s="41" t="str">
+        <v>Vsuj</v>
+      </c>
+      <c r="C2" s="40" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-1873865442@justice.gov.uk</v>
+        <v>CWR-func-test-user-6746470943@justice.gov.uk</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>5</v>
@@ -7937,15 +7934,15 @@
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gmgz</v>
+        <v>Hvgt</v>
       </c>
       <c r="B3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Hjev</v>
-      </c>
-      <c r="C3" s="41" t="str">
+        <v>Lcti</v>
+      </c>
+      <c r="C3" s="40" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-9616547353@justice.gov.uk</v>
+        <v>CWR-func-test-user-5409784713@justice.gov.uk</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>6</v>
@@ -8023,15 +8020,15 @@
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Taom</v>
+        <v>Sgla</v>
       </c>
       <c r="B4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Mdot</v>
-      </c>
-      <c r="C4" s="41" t="str">
+        <v>Qvqy</v>
+      </c>
+      <c r="C4" s="40" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-4875266102@justice.gov.uk</v>
+        <v>CWR-func-test-user-6781109191@justice.gov.uk</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>9</v>
@@ -8115,9 +8112,9 @@
       <c r="B5" s="40" t="s">
         <v>1190</v>
       </c>
-      <c r="C5" s="41" t="str">
+      <c r="C5" s="40" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-988485094@justice.gov.uk</v>
+        <v>CWR-func-test-user-6650638345@justice.gov.uk</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>4</v>
@@ -8201,37 +8198,62 @@
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="1" t="str">
+      <c r="A6" s="40" t="str">
+        <f ca="1">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
+        <v>Dcdk</v>
+      </c>
+      <c r="B6" s="40" t="str">
+        <f ca="1">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
+        <v>Sked</v>
+      </c>
+      <c r="C6" s="40" t="str">
+        <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","DWP.GOV.UK")</f>
+        <v>CWR-func-test-user-7251165068@DWP.GOV.UK</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
         <f>IF(ISNA(VLOOKUP(D6,Region!$A$2:$B$11,2)),"",VLOOKUP(D6,Region!$A$2:$B$11,2))</f>
-        <v/>
-      </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="1" t="str">
+        <v>2</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="1">
         <f>IF(ISNA(VLOOKUP(F6,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F6,'Base Locations'!$A$1:$F$341,2))</f>
-        <v/>
-      </c>
-      <c r="H6" s="40"/>
-      <c r="I6" s="1" t="str">
+        <v>219164</v>
+      </c>
+      <c r="H6" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="1">
         <f>IF(ISNA(VLOOKUP(H6,'Base Locations'!A5:F345,2)),"",VLOOKUP(H6,'Base Locations'!A5:F345,2))</f>
-        <v/>
-      </c>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
+        <v>271588</v>
+      </c>
+      <c r="J6" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="40" t="s">
+        <v>1221</v>
+      </c>
+      <c r="L6" s="40" t="s">
+        <v>1222</v>
+      </c>
       <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
+      <c r="N6" s="40" t="s">
+        <v>12</v>
+      </c>
       <c r="O6" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(N6,Services!$A$1:$B$45,2)),"",VLOOKUP(N6,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="P6" s="40"/>
+        <v>BAA2</v>
+      </c>
+      <c r="P6" s="40" t="s">
+        <v>1160</v>
+      </c>
       <c r="Q6" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P6,Services!$A$1:$B$45,2)),"",VLOOKUP(P6,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BHA3</v>
       </c>
       <c r="R6" s="40"/>
       <c r="S6" s="1" t="str">
@@ -8266,37 +8288,62 @@
       <c r="AD6" s="40"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="1" t="str">
+      <c r="A7" s="40" t="str">
+        <f ca="1">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
+        <v>Alwn</v>
+      </c>
+      <c r="B7" s="40" t="str">
+        <f ca="1">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
+        <v>Nosu</v>
+      </c>
+      <c r="C7" s="40" t="str">
+        <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","hmrc.gov.uk")</f>
+        <v>CWR-func-test-user-8638237900@hmrc.gov.uk</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1">
         <f>IF(ISNA(VLOOKUP(D7,Region!$A$2:$B$11,2)),"",VLOOKUP(D7,Region!$A$2:$B$11,2))</f>
-        <v/>
-      </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="1" t="str">
+        <v>2</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="1">
         <f>IF(ISNA(VLOOKUP(F7,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F7,'Base Locations'!$A$1:$F$341,2))</f>
-        <v/>
-      </c>
-      <c r="H7" s="40"/>
-      <c r="I7" s="1" t="str">
+        <v>827534</v>
+      </c>
+      <c r="H7" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="1">
         <f>IF(ISNA(VLOOKUP(H7,'Base Locations'!A6:F346,2)),"",VLOOKUP(H7,'Base Locations'!A6:F346,2))</f>
-        <v/>
-      </c>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
+        <v>817181</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="40" t="s">
+        <v>1222</v>
+      </c>
+      <c r="L7" s="40" t="s">
+        <v>1221</v>
+      </c>
       <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
+      <c r="N7" s="40" t="s">
+        <v>13</v>
+      </c>
       <c r="O7" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(N7,Services!$A$1:$B$45,2)),"",VLOOKUP(N7,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="P7" s="40"/>
+        <v>BAB1</v>
+      </c>
+      <c r="P7" s="40" t="s">
+        <v>1157</v>
+      </c>
       <c r="Q7" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(P7,Services!$A$1:$B$45,2)),"",VLOOKUP(P7,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BAB2</v>
       </c>
       <c r="R7" s="40"/>
       <c r="S7" s="1" t="str">
@@ -8333,7 +8380,7 @@
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="40"/>
       <c r="B8" s="40"/>
-      <c r="C8" s="41"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="40"/>
       <c r="E8" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D8,Region!$A$2:$B$11,2)),"",VLOOKUP(D8,Region!$A$2:$B$11,2))</f>
@@ -8398,7 +8445,7 @@
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="40"/>
       <c r="B9" s="40"/>
-      <c r="C9" s="41"/>
+      <c r="C9" s="40"/>
       <c r="D9" s="40"/>
       <c r="E9" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D9,Region!$A$2:$B$11,2)),"",VLOOKUP(D9,Region!$A$2:$B$11,2))</f>
@@ -8463,7 +8510,7 @@
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="40"/>
       <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
+      <c r="C10" s="40"/>
       <c r="D10" s="40"/>
       <c r="E10" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D10,Region!$A$2:$B$11,2)),"",VLOOKUP(D10,Region!$A$2:$B$11,2))</f>
@@ -8528,7 +8575,7 @@
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="40"/>
       <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="40"/>
       <c r="E11" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D11,Region!$A$2:$B$11,2)),"",VLOOKUP(D11,Region!$A$2:$B$11,2))</f>
@@ -8593,7 +8640,7 @@
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="40"/>
       <c r="B12" s="40"/>
-      <c r="C12" s="41"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="40"/>
       <c r="E12" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D12,Region!$A$2:$B$11,2)),"",VLOOKUP(D12,Region!$A$2:$B$11,2))</f>
@@ -8658,7 +8705,7 @@
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="40"/>
       <c r="B13" s="40"/>
-      <c r="C13" s="41"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="40"/>
       <c r="E13" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D13,Region!$A$2:$B$11,2)),"",VLOOKUP(D13,Region!$A$2:$B$11,2))</f>
@@ -8723,7 +8770,7 @@
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="40"/>
       <c r="B14" s="40"/>
-      <c r="C14" s="41"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="40"/>
       <c r="E14" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D14,Region!$A$2:$B$11,2)),"",VLOOKUP(D14,Region!$A$2:$B$11,2))</f>
@@ -8788,7 +8835,7 @@
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="40"/>
       <c r="B15" s="40"/>
-      <c r="C15" s="41"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D15,Region!$A$2:$B$11,2)),"",VLOOKUP(D15,Region!$A$2:$B$11,2))</f>
@@ -8853,7 +8900,7 @@
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="40"/>
       <c r="B16" s="40"/>
-      <c r="C16" s="41"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D16,Region!$A$2:$B$11,2)),"",VLOOKUP(D16,Region!$A$2:$B$11,2))</f>
@@ -8918,7 +8965,7 @@
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="40"/>
       <c r="B17" s="40"/>
-      <c r="C17" s="41"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="40"/>
       <c r="E17" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D17,Region!$A$2:$B$11,2)),"",VLOOKUP(D17,Region!$A$2:$B$11,2))</f>
@@ -8983,7 +9030,7 @@
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="40"/>
       <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="40"/>
       <c r="E18" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D18,Region!$A$2:$B$11,2)),"",VLOOKUP(D18,Region!$A$2:$B$11,2))</f>
@@ -9048,7 +9095,7 @@
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="40"/>
       <c r="B19" s="40"/>
-      <c r="C19" s="41"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="40"/>
       <c r="E19" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D19,Region!$A$2:$B$11,2)),"",VLOOKUP(D19,Region!$A$2:$B$11,2))</f>
@@ -9113,7 +9160,7 @@
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="40"/>
       <c r="B20" s="40"/>
-      <c r="C20" s="41"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="40"/>
       <c r="E20" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D20,Region!$A$2:$B$11,2)),"",VLOOKUP(D20,Region!$A$2:$B$11,2))</f>
@@ -9178,7 +9225,7 @@
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="40"/>
       <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="40"/>
       <c r="E21" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D21,Region!$A$2:$B$11,2)),"",VLOOKUP(D21,Region!$A$2:$B$11,2))</f>
@@ -9243,7 +9290,7 @@
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="40"/>
       <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="40"/>
       <c r="E22" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D22,Region!$A$2:$B$11,2)),"",VLOOKUP(D22,Region!$A$2:$B$11,2))</f>
@@ -9308,7 +9355,7 @@
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="40"/>
       <c r="B23" s="40"/>
-      <c r="C23" s="41"/>
+      <c r="C23" s="40"/>
       <c r="D23" s="40"/>
       <c r="E23" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D23,Region!$A$2:$B$11,2)),"",VLOOKUP(D23,Region!$A$2:$B$11,2))</f>
@@ -9373,7 +9420,7 @@
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="40"/>
       <c r="B24" s="40"/>
-      <c r="C24" s="41"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="40"/>
       <c r="E24" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D24,Region!$A$2:$B$11,2)),"",VLOOKUP(D24,Region!$A$2:$B$11,2))</f>
@@ -9438,7 +9485,7 @@
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="40"/>
       <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
+      <c r="C25" s="40"/>
       <c r="D25" s="40"/>
       <c r="E25" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D25,Region!$A$2:$B$11,2)),"",VLOOKUP(D25,Region!$A$2:$B$11,2))</f>
@@ -9503,7 +9550,7 @@
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="40"/>
       <c r="B26" s="40"/>
-      <c r="C26" s="41"/>
+      <c r="C26" s="40"/>
       <c r="D26" s="40"/>
       <c r="E26" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D26,Region!$A$2:$B$11,2)),"",VLOOKUP(D26,Region!$A$2:$B$11,2))</f>
@@ -9568,7 +9615,7 @@
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="40"/>
       <c r="B27" s="40"/>
-      <c r="C27" s="41"/>
+      <c r="C27" s="40"/>
       <c r="D27" s="40"/>
       <c r="E27" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D27,Region!$A$2:$B$11,2)),"",VLOOKUP(D27,Region!$A$2:$B$11,2))</f>
@@ -9633,7 +9680,7 @@
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="40"/>
       <c r="B28" s="40"/>
-      <c r="C28" s="41"/>
+      <c r="C28" s="40"/>
       <c r="D28" s="40"/>
       <c r="E28" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D28,Region!$A$2:$B$11,2)),"",VLOOKUP(D28,Region!$A$2:$B$11,2))</f>
@@ -9698,7 +9745,7 @@
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="40"/>
       <c r="B29" s="40"/>
-      <c r="C29" s="41"/>
+      <c r="C29" s="40"/>
       <c r="D29" s="40"/>
       <c r="E29" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D29,Region!$A$2:$B$11,2)),"",VLOOKUP(D29,Region!$A$2:$B$11,2))</f>
@@ -9763,7 +9810,7 @@
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="40"/>
       <c r="B30" s="40"/>
-      <c r="C30" s="41"/>
+      <c r="C30" s="40"/>
       <c r="D30" s="40"/>
       <c r="E30" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D30,Region!$A$2:$B$11,2)),"",VLOOKUP(D30,Region!$A$2:$B$11,2))</f>
@@ -9828,7 +9875,7 @@
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="40"/>
       <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
+      <c r="C31" s="40"/>
       <c r="D31" s="40"/>
       <c r="E31" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D31,Region!$A$2:$B$11,2)),"",VLOOKUP(D31,Region!$A$2:$B$11,2))</f>
@@ -9893,7 +9940,7 @@
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="40"/>
       <c r="B32" s="40"/>
-      <c r="C32" s="41"/>
+      <c r="C32" s="40"/>
       <c r="D32" s="40"/>
       <c r="E32" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D32,Region!$A$2:$B$11,2)),"",VLOOKUP(D32,Region!$A$2:$B$11,2))</f>
@@ -9958,7 +10005,7 @@
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="40"/>
       <c r="B33" s="40"/>
-      <c r="C33" s="41"/>
+      <c r="C33" s="40"/>
       <c r="D33" s="40"/>
       <c r="E33" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D33,Region!$A$2:$B$11,2)),"",VLOOKUP(D33,Region!$A$2:$B$11,2))</f>
@@ -10023,7 +10070,7 @@
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="40"/>
       <c r="B34" s="40"/>
-      <c r="C34" s="41"/>
+      <c r="C34" s="40"/>
       <c r="D34" s="40"/>
       <c r="E34" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D34,Region!$A$2:$B$11,2)),"",VLOOKUP(D34,Region!$A$2:$B$11,2))</f>
@@ -10088,7 +10135,7 @@
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="40"/>
       <c r="B35" s="40"/>
-      <c r="C35" s="41"/>
+      <c r="C35" s="40"/>
       <c r="D35" s="40"/>
       <c r="E35" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D35,Region!$A$2:$B$11,2)),"",VLOOKUP(D35,Region!$A$2:$B$11,2))</f>
@@ -10153,7 +10200,7 @@
     <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" s="40"/>
       <c r="B36" s="40"/>
-      <c r="C36" s="41"/>
+      <c r="C36" s="40"/>
       <c r="D36" s="40"/>
       <c r="E36" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D36,Region!$A$2:$B$11,2)),"",VLOOKUP(D36,Region!$A$2:$B$11,2))</f>
@@ -10218,7 +10265,7 @@
     <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="40"/>
       <c r="B37" s="40"/>
-      <c r="C37" s="41"/>
+      <c r="C37" s="40"/>
       <c r="D37" s="40"/>
       <c r="E37" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D37,Region!$A$2:$B$11,2)),"",VLOOKUP(D37,Region!$A$2:$B$11,2))</f>
@@ -10283,7 +10330,7 @@
     <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" s="40"/>
       <c r="B38" s="40"/>
-      <c r="C38" s="41"/>
+      <c r="C38" s="40"/>
       <c r="D38" s="40"/>
       <c r="E38" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D38,Region!$A$2:$B$11,2)),"",VLOOKUP(D38,Region!$A$2:$B$11,2))</f>
@@ -10348,7 +10395,7 @@
     <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" s="40"/>
       <c r="B39" s="40"/>
-      <c r="C39" s="41"/>
+      <c r="C39" s="40"/>
       <c r="D39" s="40"/>
       <c r="E39" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D39,Region!$A$2:$B$11,2)),"",VLOOKUP(D39,Region!$A$2:$B$11,2))</f>
@@ -10413,7 +10460,7 @@
     <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="40"/>
       <c r="B40" s="40"/>
-      <c r="C40" s="41"/>
+      <c r="C40" s="40"/>
       <c r="D40" s="40"/>
       <c r="E40" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D40,Region!$A$2:$B$11,2)),"",VLOOKUP(D40,Region!$A$2:$B$11,2))</f>
@@ -10478,7 +10525,7 @@
     <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="40"/>
       <c r="B41" s="40"/>
-      <c r="C41" s="41"/>
+      <c r="C41" s="40"/>
       <c r="D41" s="40"/>
       <c r="E41" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D41,Region!$A$2:$B$11,2)),"",VLOOKUP(D41,Region!$A$2:$B$11,2))</f>
@@ -10543,7 +10590,7 @@
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="40"/>
       <c r="B42" s="40"/>
-      <c r="C42" s="41"/>
+      <c r="C42" s="40"/>
       <c r="D42" s="40"/>
       <c r="E42" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D42,Region!$A$2:$B$11,2)),"",VLOOKUP(D42,Region!$A$2:$B$11,2))</f>
@@ -10608,7 +10655,7 @@
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="40"/>
       <c r="B43" s="40"/>
-      <c r="C43" s="41"/>
+      <c r="C43" s="40"/>
       <c r="D43" s="40"/>
       <c r="E43" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D43,Region!$A$2:$B$11,2)),"",VLOOKUP(D43,Region!$A$2:$B$11,2))</f>
@@ -10673,7 +10720,7 @@
     <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="40"/>
       <c r="B44" s="40"/>
-      <c r="C44" s="41"/>
+      <c r="C44" s="40"/>
       <c r="D44" s="40"/>
       <c r="E44" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D44,Region!$A$2:$B$11,2)),"",VLOOKUP(D44,Region!$A$2:$B$11,2))</f>
@@ -10738,7 +10785,7 @@
     <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="40"/>
       <c r="B45" s="40"/>
-      <c r="C45" s="41"/>
+      <c r="C45" s="40"/>
       <c r="D45" s="40"/>
       <c r="E45" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D45,Region!$A$2:$B$11,2)),"",VLOOKUP(D45,Region!$A$2:$B$11,2))</f>
@@ -10803,7 +10850,7 @@
     <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" s="40"/>
       <c r="B46" s="40"/>
-      <c r="C46" s="41"/>
+      <c r="C46" s="40"/>
       <c r="D46" s="40"/>
       <c r="E46" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D46,Region!$A$2:$B$11,2)),"",VLOOKUP(D46,Region!$A$2:$B$11,2))</f>
@@ -10868,7 +10915,7 @@
     <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="40"/>
       <c r="B47" s="40"/>
-      <c r="C47" s="41"/>
+      <c r="C47" s="40"/>
       <c r="D47" s="40"/>
       <c r="E47" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D47,Region!$A$2:$B$11,2)),"",VLOOKUP(D47,Region!$A$2:$B$11,2))</f>
@@ -10933,7 +10980,7 @@
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="40"/>
       <c r="B48" s="40"/>
-      <c r="C48" s="41"/>
+      <c r="C48" s="40"/>
       <c r="D48" s="40"/>
       <c r="E48" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D48,Region!$A$2:$B$11,2)),"",VLOOKUP(D48,Region!$A$2:$B$11,2))</f>
@@ -10998,7 +11045,7 @@
     <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49" s="40"/>
       <c r="B49" s="40"/>
-      <c r="C49" s="41"/>
+      <c r="C49" s="40"/>
       <c r="D49" s="40"/>
       <c r="E49" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D49,Region!$A$2:$B$11,2)),"",VLOOKUP(D49,Region!$A$2:$B$11,2))</f>
@@ -11063,7 +11110,7 @@
     <row r="50" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A50" s="40"/>
       <c r="B50" s="40"/>
-      <c r="C50" s="41"/>
+      <c r="C50" s="40"/>
       <c r="D50" s="40"/>
       <c r="E50" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D50,Region!$A$2:$B$11,2)),"",VLOOKUP(D50,Region!$A$2:$B$11,2))</f>
@@ -18942,122 +18989,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>1221</v>
       </c>
-      <c r="B1" s="44">
+      <c r="B1" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="44" t="s">
         <v>1222</v>
       </c>
-      <c r="B2" s="44">
+      <c r="B2" s="43">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>1211</v>
       </c>
-      <c r="B3" s="44">
+      <c r="B3" s="43">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>1208</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="43">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>1209</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="43">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>1212</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="43">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>1213</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="43">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>1214</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="43">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>1215</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="43">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>1216</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="43">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>1210</v>
       </c>
-      <c r="B11" s="44">
+      <c r="B11" s="43">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="44" t="s">
         <v>1217</v>
       </c>
-      <c r="B12" s="44">
+      <c r="B12" s="43">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>1218</v>
       </c>
-      <c r="B13" s="44">
+      <c r="B13" s="43">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="44" t="s">
         <v>1219</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="43">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="44" t="s">
         <v>1220</v>
       </c>
-      <c r="B15" s="44">
+      <c r="B15" s="43">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first Name Change in the XL sheet
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/Staff Data Upload.xlsx
+++ b/src/functionalTest/resources/Staff Data Upload.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vasthava/IdeaProjects/nayeem/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcts/IdeaProjects/rd-caseworker/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB58EA4-C603-6744-98B4-D4F97C1CE93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5244F6B-3AD4-C54D-9E10-C16392C1B6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -3717,7 +3717,7 @@
     <t>Legal Caseworker</t>
   </si>
   <si>
-    <t>cwr-func-test-user</t>
+    <t>cwr-rd-func-test-user-only</t>
   </si>
 </sst>
 </file>
@@ -7715,7 +7715,7 @@
   <dimension ref="A1:AD50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7849,12 +7849,12 @@
         <v>1223</v>
       </c>
       <c r="B2" s="40" t="str">
-        <f t="shared" ref="A2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Kizt</v>
+        <f t="shared" ref="B2:B4" ca="1" si="0">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
+        <v>Hwiq</v>
       </c>
       <c r="C2" s="40" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-91058765@justice.gov.uk</v>
+        <v>CWR-func-test-user-300742146@justice.gov.uk</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>5</v>
@@ -7939,11 +7939,11 @@
       </c>
       <c r="B3" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gpcq</v>
+        <v>Cibx</v>
       </c>
       <c r="C3" s="40" t="str">
         <f t="shared" ref="C3:C4" ca="1" si="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-478990703@justice.gov.uk</v>
+        <v>CWR-func-test-user-769148935@justice.gov.uk</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>6</v>
@@ -8024,11 +8024,11 @@
       </c>
       <c r="B4" s="40" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Icuv</v>
+        <v>Avix</v>
       </c>
       <c r="C4" s="40" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CWR-func-test-user-6001834887@justice.gov.uk</v>
+        <v>CWR-func-test-user-2188841207@justice.gov.uk</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>9</v>
@@ -8114,7 +8114,7 @@
       </c>
       <c r="C5" s="40" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","justice.gov.uk")</f>
-        <v>CWR-func-test-user-287428807@justice.gov.uk</v>
+        <v>CWR-func-test-user-9496093467@justice.gov.uk</v>
       </c>
       <c r="D5" s="40" t="s">
         <v>4</v>
@@ -8203,11 +8203,11 @@
       </c>
       <c r="B6" s="40" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Laem</v>
+        <v>Vhhv</v>
       </c>
       <c r="C6" s="40" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","DWP.GOV.UK")</f>
-        <v>CWR-func-test-user-7535073122@DWP.GOV.UK</v>
+        <v>CWR-func-test-user-4200481668@DWP.GOV.UK</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>4</v>
@@ -8292,11 +8292,11 @@
       </c>
       <c r="B7" s="40" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122)) &amp; CHAR(RANDBETWEEN(97,122))</f>
-        <v>Hsik</v>
+        <v>Auak</v>
       </c>
       <c r="C7" s="40" t="str">
         <f ca="1">CONCATENATE("CWR-func-test-user-",RANDBETWEEN(1,9999999999),"@","hmrc.gov.uk")</f>
-        <v>CWR-func-test-user-2564127652@hmrc.gov.uk</v>
+        <v>CWR-func-test-user-8797199326@hmrc.gov.uk</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>4</v>

</xml_diff>